<commit_message>
Added flags for chaos level
</commit_message>
<xml_diff>
--- a/FakeRoyaltyData.xlsx
+++ b/FakeRoyaltyData.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L51"/>
+  <dimension ref="A1:M51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -460,40 +460,45 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
+          <t>Months Since Release</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
           <t>Platform</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Book Price</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Narrator Split</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Monthly Units</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Production Cost</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Royalty Rate</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Monthly Earnings</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>Months to Break Even</t>
         </is>
@@ -502,2201 +507,2351 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Mary Guerra</t>
+          <t>Phillip Sloan</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Pull paper.</t>
+          <t>Today season their oil true.</t>
         </is>
       </c>
       <c r="C2" s="2" t="n">
-        <v>45541</v>
+        <v>45584</v>
       </c>
       <c r="D2" t="b">
         <v>0</v>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Spotify</t>
-        </is>
-      </c>
-      <c r="F2" t="n">
-        <v>12.22</v>
-      </c>
-      <c r="G2" t="b">
-        <v>1</v>
-      </c>
-      <c r="H2" t="n">
-        <v>275</v>
+      <c r="E2" t="n">
+        <v>9</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>ACX Exclusive</t>
+        </is>
+      </c>
+      <c r="G2" t="n">
+        <v>16.87</v>
+      </c>
+      <c r="H2" t="b">
+        <v>1</v>
       </c>
       <c r="I2" t="n">
-        <v>5137</v>
+        <v>859</v>
       </c>
       <c r="J2" t="n">
-        <v>0.25</v>
+        <v>4795</v>
       </c>
       <c r="K2" t="n">
-        <v>840.12</v>
+        <v>0.2</v>
       </c>
       <c r="L2" t="n">
-        <v>6.1</v>
+        <v>2898.27</v>
+      </c>
+      <c r="M2" t="n">
+        <v>1.7</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Mr. Jared Obrien MD</t>
+          <t>Andrea Bell</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Successful reflect few policy final.</t>
+          <t>Send TV she.</t>
         </is>
       </c>
       <c r="C3" s="2" t="n">
-        <v>45604</v>
+        <v>45401</v>
       </c>
       <c r="D3" t="b">
         <v>0</v>
       </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>ACX Exclusive</t>
-        </is>
-      </c>
-      <c r="F3" t="n">
-        <v>15.77</v>
-      </c>
-      <c r="G3" t="b">
-        <v>1</v>
-      </c>
-      <c r="H3" t="n">
-        <v>455</v>
+      <c r="E3" t="n">
+        <v>15</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>BookFunnel</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>18.29</v>
+      </c>
+      <c r="H3" t="b">
+        <v>1</v>
       </c>
       <c r="I3" t="n">
-        <v>2919</v>
+        <v>853</v>
       </c>
       <c r="J3" t="n">
-        <v>0.2</v>
+        <v>2246</v>
       </c>
       <c r="K3" t="n">
-        <v>1435.07</v>
+        <v>0.5</v>
       </c>
       <c r="L3" t="n">
-        <v>2</v>
+        <v>7800.68</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0.3</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Lindsay Tran</t>
+          <t>Seth Brown</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Out response hot.</t>
+          <t>Good health cultural control determine.</t>
         </is>
       </c>
       <c r="C4" s="2" t="n">
-        <v>45630</v>
+        <v>45152</v>
       </c>
       <c r="D4" t="b">
         <v>0</v>
       </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>ACX Royalty Share</t>
-        </is>
-      </c>
-      <c r="F4" t="n">
-        <v>8.98</v>
-      </c>
-      <c r="G4" t="b">
-        <v>1</v>
-      </c>
-      <c r="H4" t="n">
-        <v>718</v>
+      <c r="E4" t="n">
+        <v>23</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>ACX Exclusive</t>
+        </is>
+      </c>
+      <c r="G4" t="n">
+        <v>14.03</v>
+      </c>
+      <c r="H4" t="b">
+        <v>1</v>
       </c>
       <c r="I4" t="n">
-        <v>5729</v>
+        <v>785</v>
       </c>
       <c r="J4" t="n">
-        <v>0.1</v>
+        <v>5345</v>
       </c>
       <c r="K4" t="n">
-        <v>644.76</v>
+        <v>0.2</v>
       </c>
       <c r="L4" t="n">
-        <v>8.9</v>
+        <v>2202.71</v>
+      </c>
+      <c r="M4" t="n">
+        <v>2.4</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Paul Robertson</t>
+          <t>Judy Ramirez</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Woman specific analysis eye.</t>
+          <t>Movement man our.</t>
         </is>
       </c>
       <c r="C5" s="2" t="n">
-        <v>45423</v>
+        <v>45261</v>
       </c>
       <c r="D5" t="b">
         <v>0</v>
       </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>BookFunnel</t>
-        </is>
-      </c>
-      <c r="F5" t="n">
-        <v>8.220000000000001</v>
-      </c>
-      <c r="G5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H5" t="n">
-        <v>319</v>
+      <c r="E5" t="n">
+        <v>20</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>ACX Royalty Share</t>
+        </is>
+      </c>
+      <c r="G5" t="n">
+        <v>13.68</v>
+      </c>
+      <c r="H5" t="b">
+        <v>0</v>
       </c>
       <c r="I5" t="n">
-        <v>5831</v>
+        <v>950</v>
       </c>
       <c r="J5" t="n">
-        <v>1</v>
+        <v>3207</v>
       </c>
       <c r="K5" t="n">
-        <v>2622.18</v>
+        <v>0.4</v>
       </c>
       <c r="L5" t="n">
-        <v>2.2</v>
+        <v>5198.4</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0.6</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Laura Roberts</t>
+          <t>Jennifer Powell</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Appear official.</t>
+          <t>Reflect must trade happen.</t>
         </is>
       </c>
       <c r="C6" s="2" t="n">
-        <v>45765</v>
+        <v>45557</v>
       </c>
       <c r="D6" t="b">
         <v>0</v>
       </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Findaway</t>
-        </is>
-      </c>
-      <c r="F6" t="n">
-        <v>8.300000000000001</v>
-      </c>
-      <c r="G6" t="b">
-        <v>0</v>
-      </c>
-      <c r="H6" t="n">
-        <v>219</v>
+      <c r="E6" t="n">
+        <v>10</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>BookFunnel</t>
+        </is>
+      </c>
+      <c r="G6" t="n">
+        <v>19.73</v>
+      </c>
+      <c r="H6" t="b">
+        <v>1</v>
       </c>
       <c r="I6" t="n">
-        <v>3963</v>
+        <v>342</v>
       </c>
       <c r="J6" t="n">
-        <v>0.45</v>
+        <v>2994</v>
       </c>
       <c r="K6" t="n">
-        <v>817.97</v>
+        <v>0.5</v>
       </c>
       <c r="L6" t="n">
-        <v>4.8</v>
+        <v>3373.83</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0.9</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Stacey Clark</t>
+          <t>Willie Medina</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Oil thought this student.</t>
+          <t>Similar available own.</t>
         </is>
       </c>
       <c r="C7" s="2" t="n">
-        <v>45396</v>
+        <v>45341</v>
       </c>
       <c r="D7" t="b">
         <v>0</v>
       </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>ACX Exclusive</t>
-        </is>
-      </c>
-      <c r="F7" t="n">
-        <v>9.640000000000001</v>
-      </c>
-      <c r="G7" t="b">
-        <v>1</v>
-      </c>
-      <c r="H7" t="n">
-        <v>602</v>
+      <c r="E7" t="n">
+        <v>17</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>ACX Royalty Share</t>
+        </is>
+      </c>
+      <c r="G7" t="n">
+        <v>11.87</v>
+      </c>
+      <c r="H7" t="b">
+        <v>1</v>
       </c>
       <c r="I7" t="n">
-        <v>3642</v>
+        <v>306</v>
       </c>
       <c r="J7" t="n">
-        <v>0.2</v>
+        <v>5887</v>
       </c>
       <c r="K7" t="n">
-        <v>1160.66</v>
+        <v>0.1</v>
       </c>
       <c r="L7" t="n">
-        <v>3.1</v>
+        <v>363.22</v>
+      </c>
+      <c r="M7" t="n">
+        <v>16.2</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Mason Stephenson</t>
+          <t>Jesse Arroyo</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Care they himself or book.</t>
+          <t>Chair suffer year time probably.</t>
         </is>
       </c>
       <c r="C8" s="2" t="n">
-        <v>45544</v>
+        <v>45745</v>
       </c>
       <c r="D8" t="b">
         <v>0</v>
       </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>Findaway</t>
-        </is>
-      </c>
-      <c r="F8" t="n">
-        <v>14.61</v>
-      </c>
-      <c r="G8" t="b">
-        <v>0</v>
-      </c>
-      <c r="H8" t="n">
-        <v>283</v>
+      <c r="E8" t="n">
+        <v>4</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>BookFunnel</t>
+        </is>
+      </c>
+      <c r="G8" t="n">
+        <v>12.15</v>
+      </c>
+      <c r="H8" t="b">
+        <v>1</v>
       </c>
       <c r="I8" t="n">
-        <v>5515</v>
+        <v>597</v>
       </c>
       <c r="J8" t="n">
-        <v>0.45</v>
+        <v>2070</v>
       </c>
       <c r="K8" t="n">
-        <v>1860.58</v>
+        <v>0.5</v>
       </c>
       <c r="L8" t="n">
-        <v>3</v>
+        <v>3626.78</v>
+      </c>
+      <c r="M8" t="n">
+        <v>0.6</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Nicholas Green</t>
+          <t>Vanessa Cantrell</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Participant southern someone.</t>
+          <t>Machine offer become within.</t>
         </is>
       </c>
       <c r="C9" s="2" t="n">
-        <v>45626</v>
+        <v>45441</v>
       </c>
       <c r="D9" t="b">
         <v>0</v>
       </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>BookFunnel</t>
-        </is>
-      </c>
-      <c r="F9" t="n">
-        <v>8.470000000000001</v>
-      </c>
-      <c r="G9" t="b">
-        <v>1</v>
-      </c>
-      <c r="H9" t="n">
-        <v>438</v>
+      <c r="E9" t="n">
+        <v>14</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Findaway</t>
+        </is>
+      </c>
+      <c r="G9" t="n">
+        <v>19.76</v>
+      </c>
+      <c r="H9" t="b">
+        <v>1</v>
       </c>
       <c r="I9" t="n">
-        <v>2251</v>
+        <v>813</v>
       </c>
       <c r="J9" t="n">
-        <v>0.5</v>
+        <v>3503</v>
       </c>
       <c r="K9" t="n">
-        <v>1854.93</v>
+        <v>0.225</v>
       </c>
       <c r="L9" t="n">
-        <v>1.2</v>
+        <v>3614.6</v>
+      </c>
+      <c r="M9" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Abigail Thomas</t>
+          <t>Debra Kelly</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Big force.</t>
+          <t>Physical only four person campaign.</t>
         </is>
       </c>
       <c r="C10" s="2" t="n">
-        <v>45526</v>
+        <v>45649</v>
       </c>
       <c r="D10" t="b">
         <v>0</v>
       </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>ACX Exclusive</t>
-        </is>
-      </c>
-      <c r="F10" t="n">
-        <v>17.52</v>
-      </c>
-      <c r="G10" t="b">
-        <v>1</v>
-      </c>
-      <c r="H10" t="n">
-        <v>895</v>
+      <c r="E10" t="n">
+        <v>7</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Findaway</t>
+        </is>
+      </c>
+      <c r="G10" t="n">
+        <v>17.83</v>
+      </c>
+      <c r="H10" t="b">
+        <v>0</v>
       </c>
       <c r="I10" t="n">
-        <v>2013</v>
+        <v>292</v>
       </c>
       <c r="J10" t="n">
-        <v>0.2</v>
+        <v>2288</v>
       </c>
       <c r="K10" t="n">
-        <v>3136.08</v>
+        <v>0.45</v>
       </c>
       <c r="L10" t="n">
-        <v>0.6</v>
+        <v>2342.86</v>
+      </c>
+      <c r="M10" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Jeffrey Butler</t>
+          <t>Lauren Franco</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Economy short all around.</t>
+          <t>Deep seem do serious.</t>
         </is>
       </c>
       <c r="C11" s="2" t="n">
-        <v>45356</v>
+        <v>45486</v>
       </c>
       <c r="D11" t="b">
         <v>0</v>
       </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>BookFunnel</t>
-        </is>
-      </c>
-      <c r="F11" t="n">
-        <v>18.33</v>
-      </c>
-      <c r="G11" t="b">
-        <v>0</v>
-      </c>
-      <c r="H11" t="n">
-        <v>897</v>
+      <c r="E11" t="n">
+        <v>12</v>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Findaway</t>
+        </is>
+      </c>
+      <c r="G11" t="n">
+        <v>13.57</v>
+      </c>
+      <c r="H11" t="b">
+        <v>0</v>
       </c>
       <c r="I11" t="n">
-        <v>3091</v>
+        <v>729</v>
       </c>
       <c r="J11" t="n">
-        <v>1</v>
+        <v>2137</v>
       </c>
       <c r="K11" t="n">
-        <v>16442.01</v>
+        <v>0.45</v>
       </c>
       <c r="L11" t="n">
-        <v>0.2</v>
+        <v>4451.64</v>
+      </c>
+      <c r="M11" t="n">
+        <v>0.5</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Karen Peck</t>
+          <t>Colton Lopez</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Model take then.</t>
+          <t>Level respond general.</t>
         </is>
       </c>
       <c r="C12" s="2" t="n">
-        <v>45184</v>
+        <v>45236</v>
       </c>
       <c r="D12" t="b">
         <v>0</v>
       </c>
-      <c r="E12" t="inlineStr">
+      <c r="E12" t="n">
+        <v>21</v>
+      </c>
+      <c r="F12" t="inlineStr">
         <is>
           <t>Findaway</t>
         </is>
       </c>
-      <c r="F12" t="n">
-        <v>8.76</v>
-      </c>
-      <c r="G12" t="b">
-        <v>0</v>
-      </c>
-      <c r="H12" t="n">
-        <v>353</v>
+      <c r="G12" t="n">
+        <v>13.32</v>
+      </c>
+      <c r="H12" t="b">
+        <v>0</v>
       </c>
       <c r="I12" t="n">
-        <v>2242</v>
+        <v>598</v>
       </c>
       <c r="J12" t="n">
+        <v>4038</v>
+      </c>
+      <c r="K12" t="n">
         <v>0.45</v>
       </c>
-      <c r="K12" t="n">
-        <v>1391.53</v>
-      </c>
       <c r="L12" t="n">
-        <v>1.6</v>
+        <v>3584.41</v>
+      </c>
+      <c r="M12" t="n">
+        <v>1.1</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Cassie Montes</t>
+          <t>Anthony Anderson</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Summer soon.</t>
+          <t>Investment agent front song certain.</t>
         </is>
       </c>
       <c r="C13" s="2" t="n">
-        <v>45557</v>
+        <v>45508</v>
       </c>
       <c r="D13" t="b">
         <v>0</v>
       </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>ACX Royalty Share</t>
-        </is>
-      </c>
-      <c r="F13" t="n">
-        <v>15.24</v>
-      </c>
-      <c r="G13" t="b">
-        <v>1</v>
-      </c>
-      <c r="H13" t="n">
-        <v>416</v>
+      <c r="E13" t="n">
+        <v>12</v>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Findaway</t>
+        </is>
+      </c>
+      <c r="G13" t="n">
+        <v>15.19</v>
+      </c>
+      <c r="H13" t="b">
+        <v>0</v>
       </c>
       <c r="I13" t="n">
-        <v>4419</v>
+        <v>208</v>
       </c>
       <c r="J13" t="n">
-        <v>0.1</v>
+        <v>4160</v>
       </c>
       <c r="K13" t="n">
-        <v>633.98</v>
+        <v>0.45</v>
       </c>
       <c r="L13" t="n">
-        <v>7</v>
+        <v>1421.78</v>
+      </c>
+      <c r="M13" t="n">
+        <v>2.9</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Erin Chase</t>
+          <t>Maria Dean</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Cut three hear.</t>
+          <t>Blood investment wind.</t>
         </is>
       </c>
       <c r="C14" s="2" t="n">
-        <v>45783</v>
+        <v>45586</v>
       </c>
       <c r="D14" t="b">
         <v>0</v>
       </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>BookFunnel</t>
-        </is>
-      </c>
-      <c r="F14" t="n">
-        <v>8.949999999999999</v>
-      </c>
-      <c r="G14" t="b">
-        <v>1</v>
-      </c>
-      <c r="H14" t="n">
-        <v>416</v>
+      <c r="E14" t="n">
+        <v>9</v>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>ACX Royalty Share</t>
+        </is>
+      </c>
+      <c r="G14" t="n">
+        <v>10.8</v>
+      </c>
+      <c r="H14" t="b">
+        <v>0</v>
       </c>
       <c r="I14" t="n">
-        <v>1693</v>
+        <v>454</v>
       </c>
       <c r="J14" t="n">
-        <v>0.5</v>
+        <v>2514</v>
       </c>
       <c r="K14" t="n">
-        <v>1861.6</v>
+        <v>0.4</v>
       </c>
       <c r="L14" t="n">
-        <v>0.9</v>
+        <v>1961.28</v>
+      </c>
+      <c r="M14" t="n">
+        <v>1.3</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Amber Love DDS</t>
+          <t>Tracey Rodriguez</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Need entire.</t>
+          <t>Employee no.</t>
         </is>
       </c>
       <c r="C15" s="2" t="n">
-        <v>45621</v>
+        <v>45316</v>
       </c>
       <c r="D15" t="b">
         <v>0</v>
       </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>Spotify</t>
-        </is>
-      </c>
-      <c r="F15" t="n">
-        <v>11.99</v>
-      </c>
-      <c r="G15" t="b">
-        <v>1</v>
-      </c>
-      <c r="H15" t="n">
-        <v>223</v>
+      <c r="E15" t="n">
+        <v>18</v>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Findaway</t>
+        </is>
+      </c>
+      <c r="G15" t="n">
+        <v>14.75</v>
+      </c>
+      <c r="H15" t="b">
+        <v>1</v>
       </c>
       <c r="I15" t="n">
-        <v>4932</v>
+        <v>263</v>
       </c>
       <c r="J15" t="n">
-        <v>0.25</v>
+        <v>3515</v>
       </c>
       <c r="K15" t="n">
-        <v>668.4400000000001</v>
+        <v>0.225</v>
       </c>
       <c r="L15" t="n">
-        <v>7.4</v>
+        <v>872.83</v>
+      </c>
+      <c r="M15" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Daniel Martinez</t>
+          <t>Brandon Frey</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Large each find economy.</t>
+          <t>Soldier money worry staff.</t>
         </is>
       </c>
       <c r="C16" s="2" t="n">
-        <v>45469</v>
+        <v>45406</v>
       </c>
       <c r="D16" t="b">
         <v>0</v>
       </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>Findaway</t>
-        </is>
-      </c>
-      <c r="F16" t="n">
-        <v>15.12</v>
-      </c>
-      <c r="G16" t="b">
-        <v>1</v>
-      </c>
-      <c r="H16" t="n">
-        <v>914</v>
+      <c r="E16" t="n">
+        <v>15</v>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>ACX Exclusive</t>
+        </is>
+      </c>
+      <c r="G16" t="n">
+        <v>10.9</v>
+      </c>
+      <c r="H16" t="b">
+        <v>1</v>
       </c>
       <c r="I16" t="n">
-        <v>2805</v>
+        <v>413</v>
       </c>
       <c r="J16" t="n">
-        <v>0.225</v>
+        <v>2114</v>
       </c>
       <c r="K16" t="n">
-        <v>3109.43</v>
+        <v>0.2</v>
       </c>
       <c r="L16" t="n">
-        <v>0.9</v>
+        <v>900.34</v>
+      </c>
+      <c r="M16" t="n">
+        <v>2.3</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Stephen Norris</t>
+          <t>Jeffery Pham</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Financial form social training.</t>
+          <t>Some site wait those.</t>
         </is>
       </c>
       <c r="C17" s="2" t="n">
-        <v>45612</v>
+        <v>45320</v>
       </c>
       <c r="D17" t="b">
         <v>0</v>
       </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>ACX Exclusive</t>
-        </is>
-      </c>
-      <c r="F17" t="n">
-        <v>10.22</v>
-      </c>
-      <c r="G17" t="b">
-        <v>0</v>
-      </c>
-      <c r="H17" t="n">
-        <v>848</v>
+      <c r="E17" t="n">
+        <v>18</v>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>BookFunnel</t>
+        </is>
+      </c>
+      <c r="G17" t="n">
+        <v>15.74</v>
+      </c>
+      <c r="H17" t="b">
+        <v>1</v>
       </c>
       <c r="I17" t="n">
-        <v>4077</v>
+        <v>293</v>
       </c>
       <c r="J17" t="n">
-        <v>0.4</v>
+        <v>4564</v>
       </c>
       <c r="K17" t="n">
-        <v>3466.62</v>
+        <v>0.5</v>
       </c>
       <c r="L17" t="n">
-        <v>1.2</v>
+        <v>2305.91</v>
+      </c>
+      <c r="M17" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Ronald Peterson DVM</t>
+          <t>Dennis Davis</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>They right near.</t>
+          <t>Realize real control.</t>
         </is>
       </c>
       <c r="C18" s="2" t="n">
-        <v>45717</v>
+        <v>45555</v>
       </c>
       <c r="D18" t="b">
         <v>0</v>
       </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>ACX Exclusive</t>
-        </is>
-      </c>
-      <c r="F18" t="n">
-        <v>18.34</v>
-      </c>
-      <c r="G18" t="b">
-        <v>0</v>
-      </c>
-      <c r="H18" t="n">
-        <v>664</v>
+      <c r="E18" t="n">
+        <v>10</v>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>BookFunnel</t>
+        </is>
+      </c>
+      <c r="G18" t="n">
+        <v>9.6</v>
+      </c>
+      <c r="H18" t="b">
+        <v>1</v>
       </c>
       <c r="I18" t="n">
-        <v>3252</v>
+        <v>608</v>
       </c>
       <c r="J18" t="n">
-        <v>0.4</v>
+        <v>1676</v>
       </c>
       <c r="K18" t="n">
-        <v>4871.1</v>
+        <v>0.5</v>
       </c>
       <c r="L18" t="n">
-        <v>0.7</v>
+        <v>2918.4</v>
+      </c>
+      <c r="M18" t="n">
+        <v>0.6</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Richard Hanson DDS</t>
+          <t>Anthony Cunningham</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Least music.</t>
+          <t>Arm full since democratic.</t>
         </is>
       </c>
       <c r="C19" s="2" t="n">
-        <v>45769</v>
+        <v>45372</v>
       </c>
       <c r="D19" t="b">
         <v>0</v>
       </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>ACX Exclusive</t>
-        </is>
-      </c>
-      <c r="F19" t="n">
-        <v>13.88</v>
-      </c>
-      <c r="G19" t="b">
-        <v>1</v>
-      </c>
-      <c r="H19" t="n">
-        <v>539</v>
+      <c r="E19" t="n">
+        <v>16</v>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Findaway</t>
+        </is>
+      </c>
+      <c r="G19" t="n">
+        <v>8.82</v>
+      </c>
+      <c r="H19" t="b">
+        <v>0</v>
       </c>
       <c r="I19" t="n">
-        <v>2856</v>
+        <v>246</v>
       </c>
       <c r="J19" t="n">
-        <v>0.2</v>
+        <v>4420</v>
       </c>
       <c r="K19" t="n">
-        <v>1496.26</v>
+        <v>0.45</v>
       </c>
       <c r="L19" t="n">
-        <v>1.9</v>
+        <v>976.37</v>
+      </c>
+      <c r="M19" t="n">
+        <v>4.5</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Kenneth Wolfe</t>
+          <t>Monique Colon</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Leader professor kid beyond especially.</t>
+          <t>Officer race suddenly rule ten.</t>
         </is>
       </c>
       <c r="C20" s="2" t="n">
-        <v>45254</v>
+        <v>45438</v>
       </c>
       <c r="D20" t="b">
         <v>0</v>
       </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>Findaway</t>
-        </is>
-      </c>
-      <c r="F20" t="n">
-        <v>12.42</v>
-      </c>
-      <c r="G20" t="b">
-        <v>0</v>
-      </c>
-      <c r="H20" t="n">
-        <v>356</v>
+      <c r="E20" t="n">
+        <v>14</v>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>BookFunnel</t>
+        </is>
+      </c>
+      <c r="G20" t="n">
+        <v>11.13</v>
+      </c>
+      <c r="H20" t="b">
+        <v>1</v>
       </c>
       <c r="I20" t="n">
-        <v>4979</v>
+        <v>444</v>
       </c>
       <c r="J20" t="n">
-        <v>0.45</v>
+        <v>4621</v>
       </c>
       <c r="K20" t="n">
-        <v>1989.68</v>
+        <v>0.5</v>
       </c>
       <c r="L20" t="n">
-        <v>2.5</v>
+        <v>2470.86</v>
+      </c>
+      <c r="M20" t="n">
+        <v>1.9</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Kim Davis</t>
+          <t>Kayla Black</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Today compare institution enough.</t>
+          <t>Us network business white thing.</t>
         </is>
       </c>
       <c r="C21" s="2" t="n">
-        <v>45196</v>
+        <v>45647</v>
       </c>
       <c r="D21" t="b">
         <v>0</v>
       </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>BookFunnel</t>
-        </is>
-      </c>
-      <c r="F21" t="n">
-        <v>11.24</v>
-      </c>
-      <c r="G21" t="b">
-        <v>0</v>
-      </c>
-      <c r="H21" t="n">
-        <v>780</v>
+      <c r="E21" t="n">
+        <v>7</v>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Spotify</t>
+        </is>
+      </c>
+      <c r="G21" t="n">
+        <v>15.14</v>
+      </c>
+      <c r="H21" t="b">
+        <v>1</v>
       </c>
       <c r="I21" t="n">
-        <v>2996</v>
+        <v>515</v>
       </c>
       <c r="J21" t="n">
-        <v>1</v>
+        <v>1791</v>
       </c>
       <c r="K21" t="n">
-        <v>8767.200000000001</v>
+        <v>0.25</v>
       </c>
       <c r="L21" t="n">
-        <v>0.3</v>
+        <v>1949.28</v>
+      </c>
+      <c r="M21" t="n">
+        <v>0.9</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Steve Ferguson</t>
+          <t>Kenneth Graham</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Action hair environment off.</t>
+          <t>Pressure wind second value.</t>
         </is>
       </c>
       <c r="C22" s="2" t="n">
-        <v>45637</v>
+        <v>45289</v>
       </c>
       <c r="D22" t="b">
         <v>0</v>
       </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>Spotify</t>
-        </is>
-      </c>
-      <c r="F22" t="n">
-        <v>9.32</v>
-      </c>
-      <c r="G22" t="b">
-        <v>0</v>
-      </c>
-      <c r="H22" t="n">
-        <v>501</v>
+      <c r="E22" t="n">
+        <v>19</v>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>ACX Exclusive</t>
+        </is>
+      </c>
+      <c r="G22" t="n">
+        <v>12.39</v>
+      </c>
+      <c r="H22" t="b">
+        <v>1</v>
       </c>
       <c r="I22" t="n">
-        <v>5214</v>
+        <v>820</v>
       </c>
       <c r="J22" t="n">
-        <v>0.5</v>
+        <v>5992</v>
       </c>
       <c r="K22" t="n">
-        <v>2334.66</v>
+        <v>0.2</v>
       </c>
       <c r="L22" t="n">
-        <v>2.2</v>
+        <v>2031.96</v>
+      </c>
+      <c r="M22" t="n">
+        <v>2.9</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Joseph Gonzalez</t>
+          <t>Brian Hart</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Share child take.</t>
+          <t>New situation.</t>
         </is>
       </c>
       <c r="C23" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="D23" t="b">
         <v>0</v>
       </c>
-      <c r="E23" t="inlineStr">
+      <c r="E23" t="n">
+        <v>2</v>
+      </c>
+      <c r="F23" t="inlineStr">
         <is>
           <t>Spotify</t>
         </is>
       </c>
-      <c r="F23" t="n">
-        <v>11.2</v>
-      </c>
-      <c r="G23" t="b">
-        <v>0</v>
-      </c>
-      <c r="H23" t="n">
-        <v>632</v>
+      <c r="G23" t="n">
+        <v>12.17</v>
+      </c>
+      <c r="H23" t="b">
+        <v>1</v>
       </c>
       <c r="I23" t="n">
-        <v>5402</v>
+        <v>421</v>
       </c>
       <c r="J23" t="n">
-        <v>0.5</v>
+        <v>4668</v>
       </c>
       <c r="K23" t="n">
-        <v>3539.2</v>
+        <v>0.25</v>
       </c>
       <c r="L23" t="n">
-        <v>1.5</v>
+        <v>1280.89</v>
+      </c>
+      <c r="M23" t="n">
+        <v>3.6</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Gene Miller</t>
+          <t>David Mendoza</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Parent to stuff wonder.</t>
+          <t>Just world dream.</t>
         </is>
       </c>
       <c r="C24" s="2" t="n">
-        <v>45714</v>
+        <v>45775</v>
       </c>
       <c r="D24" t="b">
         <v>0</v>
       </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>ACX Exclusive</t>
-        </is>
-      </c>
-      <c r="F24" t="n">
-        <v>9.75</v>
-      </c>
-      <c r="G24" t="b">
-        <v>1</v>
-      </c>
-      <c r="H24" t="n">
-        <v>296</v>
+      <c r="E24" t="n">
+        <v>3</v>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>BookFunnel</t>
+        </is>
+      </c>
+      <c r="G24" t="n">
+        <v>13.64</v>
+      </c>
+      <c r="H24" t="b">
+        <v>0</v>
       </c>
       <c r="I24" t="n">
-        <v>1842</v>
+        <v>681</v>
       </c>
       <c r="J24" t="n">
-        <v>0.2</v>
+        <v>4827</v>
       </c>
       <c r="K24" t="n">
-        <v>577.2</v>
+        <v>1</v>
       </c>
       <c r="L24" t="n">
-        <v>3.2</v>
+        <v>9288.84</v>
+      </c>
+      <c r="M24" t="n">
+        <v>0.5</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Joy Andrade</t>
+          <t>Cathy Smith</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Child other each.</t>
+          <t>Front woman son.</t>
         </is>
       </c>
       <c r="C25" s="2" t="n">
-        <v>45498</v>
+        <v>45542</v>
       </c>
       <c r="D25" t="b">
         <v>0</v>
       </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>ACX Exclusive</t>
-        </is>
-      </c>
-      <c r="F25" t="n">
-        <v>9.67</v>
-      </c>
-      <c r="G25" t="b">
-        <v>0</v>
-      </c>
-      <c r="H25" t="n">
-        <v>840</v>
+      <c r="E25" t="n">
+        <v>10</v>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>Spotify</t>
+        </is>
+      </c>
+      <c r="G25" t="n">
+        <v>11.5</v>
+      </c>
+      <c r="H25" t="b">
+        <v>0</v>
       </c>
       <c r="I25" t="n">
-        <v>4471</v>
+        <v>401</v>
       </c>
       <c r="J25" t="n">
-        <v>0.4</v>
+        <v>3952</v>
       </c>
       <c r="K25" t="n">
-        <v>3249.12</v>
+        <v>0.5</v>
       </c>
       <c r="L25" t="n">
-        <v>1.4</v>
+        <v>2305.75</v>
+      </c>
+      <c r="M25" t="n">
+        <v>1.7</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Brooke Garza</t>
+          <t>Phillip Vance</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Computer play wide bring.</t>
+          <t>Edge treat.</t>
         </is>
       </c>
       <c r="C26" s="2" t="n">
-        <v>45529</v>
+        <v>45628</v>
       </c>
       <c r="D26" t="b">
         <v>0</v>
       </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>Findaway</t>
-        </is>
-      </c>
-      <c r="F26" t="n">
-        <v>16.94</v>
-      </c>
-      <c r="G26" t="b">
-        <v>1</v>
-      </c>
-      <c r="H26" t="n">
-        <v>751</v>
+      <c r="E26" t="n">
+        <v>8</v>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>ACX Exclusive</t>
+        </is>
+      </c>
+      <c r="G26" t="n">
+        <v>14.32</v>
+      </c>
+      <c r="H26" t="b">
+        <v>0</v>
       </c>
       <c r="I26" t="n">
-        <v>2818</v>
+        <v>509</v>
       </c>
       <c r="J26" t="n">
-        <v>0.225</v>
+        <v>5988</v>
       </c>
       <c r="K26" t="n">
-        <v>2862.44</v>
+        <v>0.4</v>
       </c>
       <c r="L26" t="n">
-        <v>1</v>
+        <v>2915.55</v>
+      </c>
+      <c r="M26" t="n">
+        <v>2.1</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Samantha Davis</t>
+          <t>Daniel Clark</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>With would professional.</t>
+          <t>Scene picture.</t>
         </is>
       </c>
       <c r="C27" s="2" t="n">
-        <v>45447</v>
+        <v>45399</v>
       </c>
       <c r="D27" t="b">
         <v>0</v>
       </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>Spotify</t>
-        </is>
-      </c>
-      <c r="F27" t="n">
-        <v>12.91</v>
-      </c>
-      <c r="G27" t="b">
-        <v>0</v>
-      </c>
-      <c r="H27" t="n">
-        <v>436</v>
+      <c r="E27" t="n">
+        <v>15</v>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>BookFunnel</t>
+        </is>
+      </c>
+      <c r="G27" t="n">
+        <v>19.04</v>
+      </c>
+      <c r="H27" t="b">
+        <v>0</v>
       </c>
       <c r="I27" t="n">
-        <v>3801</v>
+        <v>672</v>
       </c>
       <c r="J27" t="n">
-        <v>0.5</v>
+        <v>4089</v>
       </c>
       <c r="K27" t="n">
-        <v>2814.38</v>
+        <v>1</v>
       </c>
       <c r="L27" t="n">
-        <v>1.4</v>
+        <v>12794.88</v>
+      </c>
+      <c r="M27" t="n">
+        <v>0.3</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Christopher Monroe</t>
+          <t>Megan Williams</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Perhaps already sound sport ok.</t>
+          <t>Since themselves player another now.</t>
         </is>
       </c>
       <c r="C28" s="2" t="n">
-        <v>45499</v>
+        <v>45680</v>
       </c>
       <c r="D28" t="b">
         <v>0</v>
       </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>BookFunnel</t>
-        </is>
-      </c>
-      <c r="F28" t="n">
-        <v>19.48</v>
-      </c>
-      <c r="G28" t="b">
-        <v>0</v>
-      </c>
-      <c r="H28" t="n">
-        <v>666</v>
+      <c r="E28" t="n">
+        <v>6</v>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>Findaway</t>
+        </is>
+      </c>
+      <c r="G28" t="n">
+        <v>12.24</v>
+      </c>
+      <c r="H28" t="b">
+        <v>0</v>
       </c>
       <c r="I28" t="n">
-        <v>3010</v>
+        <v>911</v>
       </c>
       <c r="J28" t="n">
-        <v>1</v>
+        <v>5174</v>
       </c>
       <c r="K28" t="n">
-        <v>12973.68</v>
+        <v>0.45</v>
       </c>
       <c r="L28" t="n">
-        <v>0.2</v>
+        <v>5017.79</v>
+      </c>
+      <c r="M28" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Jackie Gill</t>
+          <t>Heather Jones</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Democrat rich best.</t>
+          <t>Item fear card matter TV.</t>
         </is>
       </c>
       <c r="C29" s="2" t="n">
-        <v>45750</v>
+        <v>45195</v>
       </c>
       <c r="D29" t="b">
         <v>0</v>
       </c>
-      <c r="E29" t="inlineStr">
+      <c r="E29" t="n">
+        <v>22</v>
+      </c>
+      <c r="F29" t="inlineStr">
         <is>
           <t>BookFunnel</t>
         </is>
       </c>
-      <c r="F29" t="n">
-        <v>13.2</v>
-      </c>
-      <c r="G29" t="b">
-        <v>1</v>
-      </c>
-      <c r="H29" t="n">
-        <v>424</v>
+      <c r="G29" t="n">
+        <v>16.61</v>
+      </c>
+      <c r="H29" t="b">
+        <v>1</v>
       </c>
       <c r="I29" t="n">
-        <v>3819</v>
+        <v>395</v>
       </c>
       <c r="J29" t="n">
+        <v>5770</v>
+      </c>
+      <c r="K29" t="n">
         <v>0.5</v>
       </c>
-      <c r="K29" t="n">
-        <v>2798.4</v>
-      </c>
       <c r="L29" t="n">
-        <v>1.4</v>
+        <v>3280.47</v>
+      </c>
+      <c r="M29" t="n">
+        <v>1.8</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Brian Bowen</t>
+          <t>Michael Gray</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Certainly yes.</t>
+          <t>Act half.</t>
         </is>
       </c>
       <c r="C30" s="2" t="n">
-        <v>45826</v>
+        <v>45139</v>
       </c>
       <c r="D30" t="b">
         <v>0</v>
       </c>
-      <c r="E30" t="inlineStr">
+      <c r="E30" t="n">
+        <v>24</v>
+      </c>
+      <c r="F30" t="inlineStr">
         <is>
           <t>Findaway</t>
         </is>
       </c>
-      <c r="F30" t="n">
-        <v>17.62</v>
-      </c>
-      <c r="G30" t="b">
-        <v>0</v>
-      </c>
-      <c r="H30" t="n">
-        <v>499</v>
+      <c r="G30" t="n">
+        <v>14.44</v>
+      </c>
+      <c r="H30" t="b">
+        <v>0</v>
       </c>
       <c r="I30" t="n">
-        <v>5108</v>
+        <v>723</v>
       </c>
       <c r="J30" t="n">
+        <v>5257</v>
+      </c>
+      <c r="K30" t="n">
         <v>0.45</v>
       </c>
-      <c r="K30" t="n">
-        <v>3956.57</v>
-      </c>
       <c r="L30" t="n">
-        <v>1.3</v>
+        <v>4698.05</v>
+      </c>
+      <c r="M30" t="n">
+        <v>1.1</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Melvin Garcia</t>
+          <t>Jennifer Williamson</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>American practice later.</t>
+          <t>Husband our business.</t>
         </is>
       </c>
       <c r="C31" s="2" t="n">
-        <v>45522</v>
+        <v>45848</v>
       </c>
       <c r="D31" t="b">
-        <v>0</v>
-      </c>
-      <c r="E31" t="inlineStr">
+        <v>1</v>
+      </c>
+      <c r="E31" t="n">
+        <v>0</v>
+      </c>
+      <c r="F31" t="inlineStr">
         <is>
           <t>Spotify</t>
         </is>
       </c>
-      <c r="F31" t="n">
-        <v>17.47</v>
-      </c>
-      <c r="G31" t="b">
-        <v>1</v>
-      </c>
-      <c r="H31" t="n">
-        <v>796</v>
+      <c r="G31" t="n">
+        <v>14.26</v>
+      </c>
+      <c r="H31" t="b">
+        <v>1</v>
       </c>
       <c r="I31" t="n">
-        <v>2813</v>
+        <v>63</v>
       </c>
       <c r="J31" t="n">
+        <v>2323</v>
+      </c>
+      <c r="K31" t="n">
         <v>0.25</v>
       </c>
-      <c r="K31" t="n">
-        <v>3476.53</v>
-      </c>
       <c r="L31" t="n">
-        <v>0.8</v>
+        <v>224.59</v>
+      </c>
+      <c r="M31" t="n">
+        <v>10.3</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Rodney Wallace</t>
+          <t>Michael Cisneros</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Alone that join sister.</t>
+          <t>Join big clear true.</t>
         </is>
       </c>
       <c r="C32" s="2" t="n">
-        <v>45667</v>
+        <v>45487</v>
       </c>
       <c r="D32" t="b">
         <v>0</v>
       </c>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t>ACX Royalty Share</t>
-        </is>
-      </c>
-      <c r="F32" t="n">
-        <v>13.47</v>
-      </c>
-      <c r="G32" t="b">
-        <v>0</v>
-      </c>
-      <c r="H32" t="n">
-        <v>608</v>
+      <c r="E32" t="n">
+        <v>12</v>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>ACX Exclusive</t>
+        </is>
+      </c>
+      <c r="G32" t="n">
+        <v>12.51</v>
+      </c>
+      <c r="H32" t="b">
+        <v>1</v>
       </c>
       <c r="I32" t="n">
-        <v>1622</v>
+        <v>733</v>
       </c>
       <c r="J32" t="n">
-        <v>0.4</v>
+        <v>1732</v>
       </c>
       <c r="K32" t="n">
-        <v>3275.9</v>
+        <v>0.2</v>
       </c>
       <c r="L32" t="n">
-        <v>0.5</v>
+        <v>1833.97</v>
+      </c>
+      <c r="M32" t="n">
+        <v>0.9</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Heather Frye</t>
+          <t>Laura Wilson</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Hear model institution mission.</t>
+          <t>Cost budget relationship administration collection.</t>
         </is>
       </c>
       <c r="C33" s="2" t="n">
-        <v>45590</v>
+        <v>45390</v>
       </c>
       <c r="D33" t="b">
         <v>0</v>
       </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>BookFunnel</t>
-        </is>
-      </c>
-      <c r="F33" t="n">
-        <v>11.48</v>
-      </c>
-      <c r="G33" t="b">
-        <v>0</v>
-      </c>
-      <c r="H33" t="n">
-        <v>853</v>
+      <c r="E33" t="n">
+        <v>15</v>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>ACX Exclusive</t>
+        </is>
+      </c>
+      <c r="G33" t="n">
+        <v>16.43</v>
+      </c>
+      <c r="H33" t="b">
+        <v>0</v>
       </c>
       <c r="I33" t="n">
-        <v>3966</v>
+        <v>864</v>
       </c>
       <c r="J33" t="n">
-        <v>1</v>
+        <v>2431</v>
       </c>
       <c r="K33" t="n">
-        <v>9792.440000000001</v>
+        <v>0.4</v>
       </c>
       <c r="L33" t="n">
+        <v>5678.21</v>
+      </c>
+      <c r="M33" t="n">
         <v>0.4</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Rachel Blair</t>
+          <t>Emily Davis</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Experience picture physical.</t>
+          <t>Father network because.</t>
         </is>
       </c>
       <c r="C34" s="2" t="n">
-        <v>45489</v>
+        <v>45721</v>
       </c>
       <c r="D34" t="b">
         <v>0</v>
       </c>
-      <c r="E34" t="inlineStr">
-        <is>
-          <t>ACX Royalty Share</t>
-        </is>
-      </c>
-      <c r="F34" t="n">
-        <v>11.12</v>
-      </c>
-      <c r="G34" t="b">
-        <v>1</v>
-      </c>
-      <c r="H34" t="n">
-        <v>304</v>
+      <c r="E34" t="n">
+        <v>4</v>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>Findaway</t>
+        </is>
+      </c>
+      <c r="G34" t="n">
+        <v>8.9</v>
+      </c>
+      <c r="H34" t="b">
+        <v>0</v>
       </c>
       <c r="I34" t="n">
-        <v>3847</v>
+        <v>413</v>
       </c>
       <c r="J34" t="n">
-        <v>0.1</v>
+        <v>2429</v>
       </c>
       <c r="K34" t="n">
-        <v>338.05</v>
+        <v>0.45</v>
       </c>
       <c r="L34" t="n">
-        <v>11.4</v>
+        <v>1654.07</v>
+      </c>
+      <c r="M34" t="n">
+        <v>1.5</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Zachary Burnett</t>
+          <t>Scott Ramsey</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Simple stock develop no.</t>
+          <t>Because young already follow than.</t>
         </is>
       </c>
       <c r="C35" s="2" t="n">
-        <v>45549</v>
+        <v>45298</v>
       </c>
       <c r="D35" t="b">
         <v>0</v>
       </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>ACX Royalty Share</t>
-        </is>
-      </c>
-      <c r="F35" t="n">
-        <v>12.53</v>
-      </c>
-      <c r="G35" t="b">
-        <v>1</v>
-      </c>
-      <c r="H35" t="n">
-        <v>734</v>
+      <c r="E35" t="n">
+        <v>19</v>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>BookFunnel</t>
+        </is>
+      </c>
+      <c r="G35" t="n">
+        <v>14.42</v>
+      </c>
+      <c r="H35" t="b">
+        <v>0</v>
       </c>
       <c r="I35" t="n">
-        <v>3635</v>
+        <v>666</v>
       </c>
       <c r="J35" t="n">
-        <v>0.1</v>
+        <v>4815</v>
       </c>
       <c r="K35" t="n">
-        <v>919.7</v>
+        <v>1</v>
       </c>
       <c r="L35" t="n">
-        <v>4</v>
+        <v>9603.719999999999</v>
+      </c>
+      <c r="M35" t="n">
+        <v>0.5</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>John Strickland</t>
+          <t>Victor Clements</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Water ability wonder wear.</t>
+          <t>Tough process American fine.</t>
         </is>
       </c>
       <c r="C36" s="2" t="n">
-        <v>45845</v>
+        <v>45671</v>
       </c>
       <c r="D36" t="b">
         <v>0</v>
       </c>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>ACX Royalty Share</t>
-        </is>
-      </c>
-      <c r="F36" t="n">
-        <v>19.38</v>
-      </c>
-      <c r="G36" t="b">
-        <v>0</v>
-      </c>
-      <c r="H36" t="n">
-        <v>36</v>
+      <c r="E36" t="n">
+        <v>6</v>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>BookFunnel</t>
+        </is>
+      </c>
+      <c r="G36" t="n">
+        <v>16.39</v>
+      </c>
+      <c r="H36" t="b">
+        <v>0</v>
       </c>
       <c r="I36" t="n">
-        <v>3790</v>
+        <v>638</v>
       </c>
       <c r="J36" t="n">
-        <v>0.4</v>
+        <v>5314</v>
       </c>
       <c r="K36" t="n">
-        <v>279.07</v>
+        <v>1</v>
       </c>
       <c r="L36" t="n">
-        <v>13.6</v>
+        <v>10456.82</v>
+      </c>
+      <c r="M36" t="n">
+        <v>0.5</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Kathryn Curry</t>
+          <t>Lauren Howell</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Accept result fall government.</t>
+          <t>Soldier white seem rich PM.</t>
         </is>
       </c>
       <c r="C37" s="2" t="n">
-        <v>45146</v>
+        <v>45731</v>
       </c>
       <c r="D37" t="b">
         <v>0</v>
       </c>
-      <c r="E37" t="inlineStr">
-        <is>
-          <t>ACX Exclusive</t>
-        </is>
-      </c>
-      <c r="F37" t="n">
-        <v>12.03</v>
-      </c>
-      <c r="G37" t="b">
-        <v>0</v>
-      </c>
-      <c r="H37" t="n">
-        <v>526</v>
+      <c r="E37" t="n">
+        <v>4</v>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>BookFunnel</t>
+        </is>
+      </c>
+      <c r="G37" t="n">
+        <v>8.94</v>
+      </c>
+      <c r="H37" t="b">
+        <v>1</v>
       </c>
       <c r="I37" t="n">
-        <v>5299</v>
+        <v>322</v>
       </c>
       <c r="J37" t="n">
-        <v>0.4</v>
+        <v>3225</v>
       </c>
       <c r="K37" t="n">
-        <v>2531.11</v>
+        <v>0.5</v>
       </c>
       <c r="L37" t="n">
-        <v>2.1</v>
+        <v>1439.34</v>
+      </c>
+      <c r="M37" t="n">
+        <v>2.2</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Laurie Bolton</t>
+          <t>Maria Lester</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Reveal on.</t>
+          <t>Act evening.</t>
         </is>
       </c>
       <c r="C38" s="2" t="n">
-        <v>45241</v>
+        <v>45216</v>
       </c>
       <c r="D38" t="b">
         <v>0</v>
       </c>
-      <c r="E38" t="inlineStr">
-        <is>
-          <t>ACX Exclusive</t>
-        </is>
-      </c>
-      <c r="F38" t="n">
-        <v>9.029999999999999</v>
-      </c>
-      <c r="G38" t="b">
-        <v>1</v>
-      </c>
-      <c r="H38" t="n">
-        <v>685</v>
+      <c r="E38" t="n">
+        <v>21</v>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>Findaway</t>
+        </is>
+      </c>
+      <c r="G38" t="n">
+        <v>11.18</v>
+      </c>
+      <c r="H38" t="b">
+        <v>0</v>
       </c>
       <c r="I38" t="n">
-        <v>2710</v>
+        <v>798</v>
       </c>
       <c r="J38" t="n">
-        <v>0.2</v>
+        <v>2038</v>
       </c>
       <c r="K38" t="n">
-        <v>1237.11</v>
+        <v>0.45</v>
       </c>
       <c r="L38" t="n">
-        <v>2.2</v>
+        <v>4014.74</v>
+      </c>
+      <c r="M38" t="n">
+        <v>0.5</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Douglas Thompson</t>
+          <t>Nicholas Brown</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Exactly dream form.</t>
+          <t>Style president option.</t>
         </is>
       </c>
       <c r="C39" s="2" t="n">
-        <v>45535</v>
+        <v>45463</v>
       </c>
       <c r="D39" t="b">
         <v>0</v>
       </c>
-      <c r="E39" t="inlineStr">
-        <is>
-          <t>ACX Exclusive</t>
-        </is>
-      </c>
-      <c r="F39" t="n">
-        <v>11.31</v>
-      </c>
-      <c r="G39" t="b">
-        <v>0</v>
-      </c>
-      <c r="H39" t="n">
-        <v>916</v>
+      <c r="E39" t="n">
+        <v>13</v>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>BookFunnel</t>
+        </is>
+      </c>
+      <c r="G39" t="n">
+        <v>18.81</v>
+      </c>
+      <c r="H39" t="b">
+        <v>1</v>
       </c>
       <c r="I39" t="n">
-        <v>5106</v>
+        <v>774</v>
       </c>
       <c r="J39" t="n">
-        <v>0.4</v>
+        <v>4953</v>
       </c>
       <c r="K39" t="n">
-        <v>4143.98</v>
+        <v>0.5</v>
       </c>
       <c r="L39" t="n">
-        <v>1.2</v>
+        <v>7279.47</v>
+      </c>
+      <c r="M39" t="n">
+        <v>0.7</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Patricia Ramirez</t>
+          <t>Abigail Cameron</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Magazine provide or.</t>
+          <t>Court drive everything late.</t>
         </is>
       </c>
       <c r="C40" s="2" t="n">
-        <v>45702</v>
+        <v>45517</v>
       </c>
       <c r="D40" t="b">
         <v>0</v>
       </c>
-      <c r="E40" t="inlineStr">
-        <is>
-          <t>Spotify</t>
-        </is>
-      </c>
-      <c r="F40" t="n">
-        <v>18.54</v>
-      </c>
-      <c r="G40" t="b">
-        <v>1</v>
-      </c>
-      <c r="H40" t="n">
-        <v>538</v>
+      <c r="E40" t="n">
+        <v>11</v>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>BookFunnel</t>
+        </is>
+      </c>
+      <c r="G40" t="n">
+        <v>10.45</v>
+      </c>
+      <c r="H40" t="b">
+        <v>1</v>
       </c>
       <c r="I40" t="n">
-        <v>2928</v>
+        <v>290</v>
       </c>
       <c r="J40" t="n">
-        <v>0.25</v>
+        <v>5860</v>
       </c>
       <c r="K40" t="n">
-        <v>2493.63</v>
+        <v>0.5</v>
       </c>
       <c r="L40" t="n">
-        <v>1.2</v>
+        <v>1515.25</v>
+      </c>
+      <c r="M40" t="n">
+        <v>3.9</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Emily Fernandez</t>
+          <t>Sean Kidd</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Situation step.</t>
+          <t>Morning guess remain third.</t>
         </is>
       </c>
       <c r="C41" s="2" t="n">
-        <v>45199</v>
+        <v>45868</v>
       </c>
       <c r="D41" t="b">
-        <v>0</v>
-      </c>
-      <c r="E41" t="inlineStr">
-        <is>
-          <t>ACX Exclusive</t>
-        </is>
-      </c>
-      <c r="F41" t="n">
-        <v>11.6</v>
-      </c>
-      <c r="G41" t="b">
-        <v>1</v>
-      </c>
-      <c r="H41" t="n">
-        <v>737</v>
+        <v>1</v>
+      </c>
+      <c r="E41" t="n">
+        <v>0</v>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>Spotify</t>
+        </is>
+      </c>
+      <c r="G41" t="n">
+        <v>8.85</v>
+      </c>
+      <c r="H41" t="b">
+        <v>0</v>
       </c>
       <c r="I41" t="n">
-        <v>1606</v>
+        <v>289</v>
       </c>
       <c r="J41" t="n">
-        <v>0.2</v>
+        <v>5263</v>
       </c>
       <c r="K41" t="n">
-        <v>1709.84</v>
+        <v>0.5</v>
       </c>
       <c r="L41" t="n">
-        <v>0.9</v>
+        <v>1278.83</v>
+      </c>
+      <c r="M41" t="n">
+        <v>4.1</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Brenda Buchanan</t>
+          <t>Gregory Miller</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>View box fast answer door.</t>
+          <t>East environmental.</t>
         </is>
       </c>
       <c r="C42" s="2" t="n">
-        <v>45463</v>
+        <v>45650</v>
       </c>
       <c r="D42" t="b">
         <v>0</v>
       </c>
-      <c r="E42" t="inlineStr">
-        <is>
-          <t>Findaway</t>
-        </is>
-      </c>
-      <c r="F42" t="n">
-        <v>11.44</v>
-      </c>
-      <c r="G42" t="b">
-        <v>1</v>
-      </c>
-      <c r="H42" t="n">
-        <v>979</v>
+      <c r="E42" t="n">
+        <v>7</v>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>ACX Exclusive</t>
+        </is>
+      </c>
+      <c r="G42" t="n">
+        <v>11.33</v>
+      </c>
+      <c r="H42" t="b">
+        <v>0</v>
       </c>
       <c r="I42" t="n">
-        <v>1946</v>
+        <v>377</v>
       </c>
       <c r="J42" t="n">
-        <v>0.225</v>
+        <v>4569</v>
       </c>
       <c r="K42" t="n">
-        <v>2519.95</v>
+        <v>0.4</v>
       </c>
       <c r="L42" t="n">
-        <v>0.8</v>
+        <v>1708.56</v>
+      </c>
+      <c r="M42" t="n">
+        <v>2.7</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Gary Cooper</t>
+          <t>Juan Payne</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Her vote east summer.</t>
+          <t>Design dinner upon he.</t>
         </is>
       </c>
       <c r="C43" s="2" t="n">
-        <v>45349</v>
+        <v>45548</v>
       </c>
       <c r="D43" t="b">
         <v>0</v>
       </c>
-      <c r="E43" t="inlineStr">
-        <is>
-          <t>ACX Royalty Share</t>
-        </is>
-      </c>
-      <c r="F43" t="n">
-        <v>11.87</v>
-      </c>
-      <c r="G43" t="b">
-        <v>0</v>
-      </c>
-      <c r="H43" t="n">
-        <v>581</v>
+      <c r="E43" t="n">
+        <v>10</v>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>Findaway</t>
+        </is>
+      </c>
+      <c r="G43" t="n">
+        <v>15.17</v>
+      </c>
+      <c r="H43" t="b">
+        <v>0</v>
       </c>
       <c r="I43" t="n">
-        <v>1612</v>
+        <v>317</v>
       </c>
       <c r="J43" t="n">
-        <v>0.4</v>
+        <v>4597</v>
       </c>
       <c r="K43" t="n">
-        <v>2758.59</v>
+        <v>0.45</v>
       </c>
       <c r="L43" t="n">
-        <v>0.6</v>
+        <v>2164</v>
+      </c>
+      <c r="M43" t="n">
+        <v>2.1</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Stephen Thompson</t>
+          <t>Janet Flores</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Republican whom Republican report stage.</t>
+          <t>Analysis degree machine husband.</t>
         </is>
       </c>
       <c r="C44" s="2" t="n">
-        <v>45626</v>
+        <v>45580</v>
       </c>
       <c r="D44" t="b">
         <v>0</v>
       </c>
-      <c r="E44" t="inlineStr">
+      <c r="E44" t="n">
+        <v>9</v>
+      </c>
+      <c r="F44" t="inlineStr">
         <is>
           <t>ACX Royalty Share</t>
         </is>
       </c>
-      <c r="F44" t="n">
-        <v>16.29</v>
-      </c>
-      <c r="G44" t="b">
-        <v>1</v>
-      </c>
-      <c r="H44" t="n">
-        <v>945</v>
+      <c r="G44" t="n">
+        <v>15.55</v>
+      </c>
+      <c r="H44" t="b">
+        <v>0</v>
       </c>
       <c r="I44" t="n">
-        <v>5329</v>
+        <v>922</v>
       </c>
       <c r="J44" t="n">
-        <v>0.1</v>
+        <v>2031</v>
       </c>
       <c r="K44" t="n">
-        <v>1539.4</v>
+        <v>0.4</v>
       </c>
       <c r="L44" t="n">
-        <v>3.5</v>
+        <v>5734.84</v>
+      </c>
+      <c r="M44" t="n">
+        <v>0.4</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Jeffrey Owens</t>
+          <t>Susan Shelton</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Wonder response if.</t>
+          <t>Hard public.</t>
         </is>
       </c>
       <c r="C45" s="2" t="n">
-        <v>45478</v>
+        <v>45307</v>
       </c>
       <c r="D45" t="b">
         <v>0</v>
       </c>
-      <c r="E45" t="inlineStr">
-        <is>
-          <t>ACX Royalty Share</t>
-        </is>
-      </c>
-      <c r="F45" t="n">
-        <v>15.98</v>
-      </c>
-      <c r="G45" t="b">
-        <v>1</v>
-      </c>
-      <c r="H45" t="n">
-        <v>389</v>
+      <c r="E45" t="n">
+        <v>18</v>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>ACX Exclusive</t>
+        </is>
+      </c>
+      <c r="G45" t="n">
+        <v>16.89</v>
+      </c>
+      <c r="H45" t="b">
+        <v>0</v>
       </c>
       <c r="I45" t="n">
-        <v>3369</v>
+        <v>930</v>
       </c>
       <c r="J45" t="n">
-        <v>0.1</v>
+        <v>4111</v>
       </c>
       <c r="K45" t="n">
-        <v>621.62</v>
+        <v>0.4</v>
       </c>
       <c r="L45" t="n">
-        <v>5.4</v>
+        <v>6283.08</v>
+      </c>
+      <c r="M45" t="n">
+        <v>0.7</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Carol Griffith</t>
+          <t>Margaret Lucas</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Subject nature down least open.</t>
+          <t>Character voice book keep.</t>
         </is>
       </c>
       <c r="C46" s="2" t="n">
-        <v>45403</v>
+        <v>45708</v>
       </c>
       <c r="D46" t="b">
         <v>0</v>
       </c>
-      <c r="E46" t="inlineStr">
+      <c r="E46" t="n">
+        <v>5</v>
+      </c>
+      <c r="F46" t="inlineStr">
         <is>
           <t>Spotify</t>
         </is>
       </c>
-      <c r="F46" t="n">
-        <v>8.42</v>
-      </c>
-      <c r="G46" t="b">
-        <v>1</v>
-      </c>
-      <c r="H46" t="n">
-        <v>321</v>
+      <c r="G46" t="n">
+        <v>10.44</v>
+      </c>
+      <c r="H46" t="b">
+        <v>0</v>
       </c>
       <c r="I46" t="n">
-        <v>4935</v>
+        <v>654</v>
       </c>
       <c r="J46" t="n">
-        <v>0.25</v>
+        <v>2300</v>
       </c>
       <c r="K46" t="n">
-        <v>675.71</v>
+        <v>0.5</v>
       </c>
       <c r="L46" t="n">
-        <v>7.3</v>
+        <v>3413.88</v>
+      </c>
+      <c r="M46" t="n">
+        <v>0.7</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Sara Howell</t>
+          <t>John Dickerson</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Son attention building out model.</t>
+          <t>Media go wide themselves.</t>
         </is>
       </c>
       <c r="C47" s="2" t="n">
-        <v>45194</v>
+        <v>45710</v>
       </c>
       <c r="D47" t="b">
         <v>0</v>
       </c>
-      <c r="E47" t="inlineStr">
-        <is>
-          <t>BookFunnel</t>
-        </is>
-      </c>
-      <c r="F47" t="n">
-        <v>13.64</v>
-      </c>
-      <c r="G47" t="b">
-        <v>1</v>
-      </c>
-      <c r="H47" t="n">
-        <v>623</v>
+      <c r="E47" t="n">
+        <v>5</v>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>Spotify</t>
+        </is>
+      </c>
+      <c r="G47" t="n">
+        <v>19.73</v>
+      </c>
+      <c r="H47" t="b">
+        <v>0</v>
       </c>
       <c r="I47" t="n">
-        <v>4932</v>
+        <v>332</v>
       </c>
       <c r="J47" t="n">
+        <v>1547</v>
+      </c>
+      <c r="K47" t="n">
         <v>0.5</v>
       </c>
-      <c r="K47" t="n">
-        <v>4248.86</v>
-      </c>
       <c r="L47" t="n">
-        <v>1.2</v>
+        <v>3275.18</v>
+      </c>
+      <c r="M47" t="n">
+        <v>0.5</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Sarah Blackwell</t>
+          <t>Rita Jenkins</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Protect stage.</t>
+          <t>Hospital down speech see level.</t>
         </is>
       </c>
       <c r="C48" s="2" t="n">
-        <v>45286</v>
+        <v>45598</v>
       </c>
       <c r="D48" t="b">
         <v>0</v>
       </c>
-      <c r="E48" t="inlineStr">
-        <is>
-          <t>Spotify</t>
-        </is>
-      </c>
-      <c r="F48" t="n">
-        <v>12.65</v>
-      </c>
-      <c r="G48" t="b">
-        <v>0</v>
-      </c>
-      <c r="H48" t="n">
-        <v>663</v>
+      <c r="E48" t="n">
+        <v>9</v>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>ACX Royalty Share</t>
+        </is>
+      </c>
+      <c r="G48" t="n">
+        <v>13.16</v>
+      </c>
+      <c r="H48" t="b">
+        <v>0</v>
       </c>
       <c r="I48" t="n">
-        <v>2158</v>
+        <v>243</v>
       </c>
       <c r="J48" t="n">
-        <v>0.5</v>
+        <v>5400</v>
       </c>
       <c r="K48" t="n">
-        <v>4193.48</v>
+        <v>0.4</v>
       </c>
       <c r="L48" t="n">
-        <v>0.5</v>
+        <v>1279.15</v>
+      </c>
+      <c r="M48" t="n">
+        <v>4.2</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Mr. Jared Diaz</t>
+          <t>Kristopher Holden</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Father family capital especially.</t>
+          <t>Seem thing six race.</t>
         </is>
       </c>
       <c r="C49" s="2" t="n">
-        <v>45722</v>
+        <v>45654</v>
       </c>
       <c r="D49" t="b">
         <v>0</v>
       </c>
-      <c r="E49" t="inlineStr">
-        <is>
-          <t>ACX Royalty Share</t>
-        </is>
-      </c>
-      <c r="F49" t="n">
-        <v>17.8</v>
-      </c>
-      <c r="G49" t="b">
-        <v>1</v>
-      </c>
-      <c r="H49" t="n">
-        <v>605</v>
+      <c r="E49" t="n">
+        <v>7</v>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>Findaway</t>
+        </is>
+      </c>
+      <c r="G49" t="n">
+        <v>14.48</v>
+      </c>
+      <c r="H49" t="b">
+        <v>1</v>
       </c>
       <c r="I49" t="n">
-        <v>3527</v>
+        <v>900</v>
       </c>
       <c r="J49" t="n">
-        <v>0.1</v>
+        <v>4943</v>
       </c>
       <c r="K49" t="n">
-        <v>1076.9</v>
+        <v>0.225</v>
       </c>
       <c r="L49" t="n">
-        <v>3.3</v>
+        <v>2932.2</v>
+      </c>
+      <c r="M49" t="n">
+        <v>1.7</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Briana Nunez</t>
+          <t>Edward Frazier</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Movement else guess meet.</t>
+          <t>Option seem official.</t>
         </is>
       </c>
       <c r="C50" s="2" t="n">
-        <v>45341</v>
+        <v>45699</v>
       </c>
       <c r="D50" t="b">
         <v>0</v>
       </c>
-      <c r="E50" t="inlineStr">
-        <is>
-          <t>ACX Exclusive</t>
-        </is>
-      </c>
-      <c r="F50" t="n">
-        <v>12.89</v>
-      </c>
-      <c r="G50" t="b">
-        <v>0</v>
-      </c>
-      <c r="H50" t="n">
-        <v>247</v>
+      <c r="E50" t="n">
+        <v>5</v>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>Spotify</t>
+        </is>
+      </c>
+      <c r="G50" t="n">
+        <v>12.45</v>
+      </c>
+      <c r="H50" t="b">
+        <v>0</v>
       </c>
       <c r="I50" t="n">
-        <v>4917</v>
+        <v>542</v>
       </c>
       <c r="J50" t="n">
-        <v>0.4</v>
+        <v>5935</v>
       </c>
       <c r="K50" t="n">
-        <v>1273.53</v>
+        <v>0.5</v>
       </c>
       <c r="L50" t="n">
-        <v>3.9</v>
+        <v>3373.95</v>
+      </c>
+      <c r="M50" t="n">
+        <v>1.8</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Sydney Thomas</t>
+          <t>Zachary Jones</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Marriage tell.</t>
+          <t>Top though cut capital.</t>
         </is>
       </c>
       <c r="C51" s="2" t="n">
-        <v>45374</v>
+        <v>45777</v>
       </c>
       <c r="D51" t="b">
         <v>0</v>
       </c>
-      <c r="E51" t="inlineStr">
-        <is>
-          <t>Findaway</t>
-        </is>
-      </c>
-      <c r="F51" t="n">
-        <v>16.36</v>
-      </c>
-      <c r="G51" t="b">
-        <v>1</v>
-      </c>
-      <c r="H51" t="n">
-        <v>915</v>
+      <c r="E51" t="n">
+        <v>3</v>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>Spotify</t>
+        </is>
+      </c>
+      <c r="G51" t="n">
+        <v>16.02</v>
+      </c>
+      <c r="H51" t="b">
+        <v>0</v>
       </c>
       <c r="I51" t="n">
-        <v>2260</v>
+        <v>214</v>
       </c>
       <c r="J51" t="n">
-        <v>0.225</v>
+        <v>5780</v>
       </c>
       <c r="K51" t="n">
-        <v>3368.12</v>
+        <v>0.5</v>
       </c>
       <c r="L51" t="n">
-        <v>0.7</v>
+        <v>1714.14</v>
+      </c>
+      <c r="M51" t="n">
+        <v>3.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added parameters around narrators and royalty rate to get a more realistic outlook into what an audiobook costs
</commit_message>
<xml_diff>
--- a/FakeRoyaltyData.xlsx
+++ b/FakeRoyaltyData.xlsx
@@ -527,48 +527,48 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Sylvia Richardson</t>
+          <t>Christina Burns</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Nothing pretty section.</t>
+          <t>Also check.</t>
         </is>
       </c>
       <c r="C2" s="2" t="n">
-        <v>45594</v>
+        <v>45371</v>
       </c>
       <c r="D2" t="b">
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Findaway</t>
+          <t>BookFunnel</t>
         </is>
       </c>
       <c r="G2" t="n">
-        <v>15.38</v>
+        <v>18.08</v>
       </c>
       <c r="H2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I2" t="n">
-        <v>717</v>
+        <v>358</v>
       </c>
       <c r="J2" t="n">
-        <v>2421</v>
+        <v>1751</v>
       </c>
       <c r="K2" t="n">
-        <v>0.225</v>
+        <v>1</v>
       </c>
       <c r="L2" t="n">
-        <v>2481.18</v>
+        <v>6472.64</v>
       </c>
       <c r="M2" t="n">
-        <v>1</v>
+        <v>0.3</v>
       </c>
       <c r="N2" t="b">
         <v>1</v>
@@ -586,51 +586,51 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Jennifer Howard</t>
+          <t>Kelly Mills</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Employee everything must lot history.</t>
+          <t>Most character enter choose.</t>
         </is>
       </c>
       <c r="C3" s="2" t="n">
-        <v>45808</v>
+        <v>45814</v>
       </c>
       <c r="D3" t="b">
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>BookFunnel</t>
+          <t>Findaway</t>
         </is>
       </c>
       <c r="G3" t="n">
-        <v>19.51</v>
+        <v>10.34</v>
       </c>
       <c r="H3" t="b">
         <v>1</v>
       </c>
       <c r="I3" t="n">
-        <v>290</v>
+        <v>153</v>
       </c>
       <c r="J3" t="n">
-        <v>4120</v>
+        <v>3256</v>
       </c>
       <c r="K3" t="n">
-        <v>0.5</v>
+        <v>0.225</v>
       </c>
       <c r="L3" t="n">
-        <v>2828.95</v>
+        <v>355.95</v>
       </c>
       <c r="M3" t="n">
-        <v>1.5</v>
+        <v>9.1</v>
       </c>
       <c r="N3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O3" t="b">
         <v>0</v>
@@ -645,48 +645,48 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Eugene Clark</t>
+          <t>Margaret Miller</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Might often country fly use.</t>
+          <t>Article others perform mission relationship.</t>
         </is>
       </c>
       <c r="C4" s="2" t="n">
-        <v>45357</v>
+        <v>45712</v>
       </c>
       <c r="D4" t="b">
         <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>ACX Royalty Share</t>
+          <t>ACX Exclusive</t>
         </is>
       </c>
       <c r="G4" t="n">
-        <v>8.94</v>
+        <v>14.57</v>
       </c>
       <c r="H4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I4" t="n">
-        <v>310</v>
+        <v>518</v>
       </c>
       <c r="J4" t="n">
-        <v>5935</v>
+        <v>4203</v>
       </c>
       <c r="K4" t="n">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="L4" t="n">
-        <v>1108.56</v>
+        <v>1509.45</v>
       </c>
       <c r="M4" t="n">
-        <v>5.4</v>
+        <v>2.8</v>
       </c>
       <c r="N4" t="b">
         <v>1</v>
@@ -704,22 +704,22 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Jimmy Robbins</t>
+          <t>Barbara Williams</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Argue after message.</t>
+          <t>Bar lose sort.</t>
         </is>
       </c>
       <c r="C5" s="2" t="n">
-        <v>45674</v>
+        <v>45548</v>
       </c>
       <c r="D5" t="b">
         <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
@@ -727,25 +727,25 @@
         </is>
       </c>
       <c r="G5" t="n">
-        <v>19.93</v>
+        <v>9.720000000000001</v>
       </c>
       <c r="H5" t="b">
         <v>1</v>
       </c>
       <c r="I5" t="n">
-        <v>651</v>
+        <v>694</v>
       </c>
       <c r="J5" t="n">
-        <v>2060</v>
+        <v>3120</v>
       </c>
       <c r="K5" t="n">
         <v>0.2</v>
       </c>
       <c r="L5" t="n">
-        <v>2594.89</v>
+        <v>1349.14</v>
       </c>
       <c r="M5" t="n">
-        <v>0.8</v>
+        <v>2.3</v>
       </c>
       <c r="N5" t="b">
         <v>1</v>
@@ -763,48 +763,48 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Stephen Barton DDS</t>
+          <t>Shawn Kelley</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Board tonight generation level bag.</t>
+          <t>Clearly well.</t>
         </is>
       </c>
       <c r="C6" s="2" t="n">
-        <v>45829</v>
+        <v>45507</v>
       </c>
       <c r="D6" t="b">
         <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>BookFunnel</t>
+          <t>Findaway</t>
         </is>
       </c>
       <c r="G6" t="n">
-        <v>14.35</v>
+        <v>15.6</v>
       </c>
       <c r="H6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I6" t="n">
-        <v>170</v>
+        <v>375</v>
       </c>
       <c r="J6" t="n">
-        <v>2348</v>
+        <v>2524</v>
       </c>
       <c r="K6" t="n">
-        <v>1</v>
+        <v>0.225</v>
       </c>
       <c r="L6" t="n">
-        <v>2439.5</v>
+        <v>1316.25</v>
       </c>
       <c r="M6" t="n">
-        <v>1</v>
+        <v>1.9</v>
       </c>
       <c r="N6" t="b">
         <v>1</v>
@@ -822,22 +822,22 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Sergio Griffin</t>
+          <t>Joshua Murphy</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Involve girl large.</t>
+          <t>Entire information subject actually.</t>
         </is>
       </c>
       <c r="C7" s="2" t="n">
-        <v>45343</v>
+        <v>45596</v>
       </c>
       <c r="D7" t="b">
         <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
@@ -845,25 +845,25 @@
         </is>
       </c>
       <c r="G7" t="n">
-        <v>19.9</v>
+        <v>18.36</v>
       </c>
       <c r="H7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I7" t="n">
-        <v>345</v>
+        <v>889</v>
       </c>
       <c r="J7" t="n">
-        <v>3569</v>
+        <v>2805</v>
       </c>
       <c r="K7" t="n">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="L7" t="n">
-        <v>3432.75</v>
+        <v>4080.51</v>
       </c>
       <c r="M7" t="n">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="N7" t="b">
         <v>1</v>
@@ -881,22 +881,22 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Sharon Golden</t>
+          <t>Jeffrey Howard</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Report remain stand.</t>
+          <t>Inside modern bit knowledge out.</t>
         </is>
       </c>
       <c r="C8" s="2" t="n">
-        <v>45555</v>
+        <v>45807</v>
       </c>
       <c r="D8" t="b">
         <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
@@ -904,28 +904,28 @@
         </is>
       </c>
       <c r="G8" t="n">
-        <v>8.859999999999999</v>
+        <v>10.72</v>
       </c>
       <c r="H8" t="b">
         <v>0</v>
       </c>
       <c r="I8" t="n">
-        <v>957</v>
+        <v>333</v>
       </c>
       <c r="J8" t="n">
-        <v>3085</v>
+        <v>5495</v>
       </c>
       <c r="K8" t="n">
         <v>0.4</v>
       </c>
       <c r="L8" t="n">
-        <v>3391.61</v>
+        <v>1427.9</v>
       </c>
       <c r="M8" t="n">
-        <v>0.9</v>
+        <v>3.8</v>
       </c>
       <c r="N8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O8" t="b">
         <v>0</v>
@@ -940,22 +940,22 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Casey Martinez</t>
+          <t>Donna Brown</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Call whom ahead.</t>
+          <t>Still certainly democratic.</t>
         </is>
       </c>
       <c r="C9" s="2" t="n">
-        <v>45190</v>
+        <v>45553</v>
       </c>
       <c r="D9" t="b">
         <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
@@ -963,25 +963,25 @@
         </is>
       </c>
       <c r="G9" t="n">
-        <v>19.02</v>
+        <v>13.17</v>
       </c>
       <c r="H9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I9" t="n">
-        <v>343</v>
+        <v>578</v>
       </c>
       <c r="J9" t="n">
-        <v>5266</v>
+        <v>4416</v>
       </c>
       <c r="K9" t="n">
-        <v>0.4</v>
+        <v>0.1</v>
       </c>
       <c r="L9" t="n">
-        <v>2609.54</v>
+        <v>761.23</v>
       </c>
       <c r="M9" t="n">
-        <v>2</v>
+        <v>5.8</v>
       </c>
       <c r="N9" t="b">
         <v>1</v>
@@ -999,48 +999,48 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Benjamin Robinson</t>
+          <t>Christopher Davenport</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Issue meeting beautiful join medical.</t>
+          <t>Green face everyone pattern.</t>
         </is>
       </c>
       <c r="C10" s="2" t="n">
-        <v>45356</v>
+        <v>45221</v>
       </c>
       <c r="D10" t="b">
         <v>0</v>
       </c>
       <c r="E10" t="n">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>ACX Exclusive</t>
+          <t>ACX Royalty Share</t>
         </is>
       </c>
       <c r="G10" t="n">
-        <v>12.97</v>
+        <v>18.31</v>
       </c>
       <c r="H10" t="b">
         <v>1</v>
       </c>
       <c r="I10" t="n">
-        <v>376</v>
+        <v>780</v>
       </c>
       <c r="J10" t="n">
-        <v>3537</v>
+        <v>4253</v>
       </c>
       <c r="K10" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="L10" t="n">
-        <v>975.34</v>
+        <v>1428.18</v>
       </c>
       <c r="M10" t="n">
-        <v>3.6</v>
+        <v>3</v>
       </c>
       <c r="N10" t="b">
         <v>1</v>
@@ -1058,48 +1058,48 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Alex Brown</t>
+          <t>Kelly Thomas</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Fund past.</t>
+          <t>Too address find.</t>
         </is>
       </c>
       <c r="C11" s="2" t="n">
-        <v>45641</v>
+        <v>45700</v>
       </c>
       <c r="D11" t="b">
         <v>0</v>
       </c>
       <c r="E11" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Findaway</t>
+          <t>BookFunnel</t>
         </is>
       </c>
       <c r="G11" t="n">
-        <v>14.23</v>
+        <v>11.37</v>
       </c>
       <c r="H11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I11" t="n">
-        <v>896</v>
+        <v>700</v>
       </c>
       <c r="J11" t="n">
-        <v>1683</v>
+        <v>3561</v>
       </c>
       <c r="K11" t="n">
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="L11" t="n">
-        <v>5737.54</v>
+        <v>3979.5</v>
       </c>
       <c r="M11" t="n">
-        <v>0.3</v>
+        <v>0.9</v>
       </c>
       <c r="N11" t="b">
         <v>1</v>
@@ -1117,48 +1117,48 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Tammie Roberts</t>
+          <t>Jessica Collins</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>About once by test.</t>
+          <t>Show participant follow story.</t>
         </is>
       </c>
       <c r="C12" s="2" t="n">
-        <v>45328</v>
+        <v>45474</v>
       </c>
       <c r="D12" t="b">
         <v>0</v>
       </c>
       <c r="E12" t="n">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>BookFunnel</t>
+          <t>Spotify</t>
         </is>
       </c>
       <c r="G12" t="n">
-        <v>13.14</v>
+        <v>11.88</v>
       </c>
       <c r="H12" t="b">
         <v>0</v>
       </c>
       <c r="I12" t="n">
-        <v>435</v>
+        <v>472</v>
       </c>
       <c r="J12" t="n">
-        <v>3127</v>
+        <v>2294</v>
       </c>
       <c r="K12" t="n">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="L12" t="n">
-        <v>5715.9</v>
+        <v>2803.68</v>
       </c>
       <c r="M12" t="n">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="N12" t="b">
         <v>1</v>
@@ -1176,48 +1176,48 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Jill Martinez</t>
+          <t>John Lopez</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Certainly set live guy sign.</t>
+          <t>Raise thank could.</t>
         </is>
       </c>
       <c r="C13" s="2" t="n">
-        <v>45162</v>
+        <v>45601</v>
       </c>
       <c r="D13" t="b">
         <v>0</v>
       </c>
       <c r="E13" t="n">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Spotify</t>
+          <t>ACX Exclusive</t>
         </is>
       </c>
       <c r="G13" t="n">
-        <v>12.94</v>
+        <v>14.65</v>
       </c>
       <c r="H13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I13" t="n">
-        <v>354</v>
+        <v>216</v>
       </c>
       <c r="J13" t="n">
-        <v>4432</v>
+        <v>1861</v>
       </c>
       <c r="K13" t="n">
-        <v>0.25</v>
+        <v>0.4</v>
       </c>
       <c r="L13" t="n">
-        <v>1145.19</v>
+        <v>1265.76</v>
       </c>
       <c r="M13" t="n">
-        <v>3.9</v>
+        <v>1.5</v>
       </c>
       <c r="N13" t="b">
         <v>1</v>
@@ -1235,48 +1235,48 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Pamela Douglas</t>
+          <t>Lee Graham</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Respond respond teach.</t>
+          <t>Section trade.</t>
         </is>
       </c>
       <c r="C14" s="2" t="n">
-        <v>45336</v>
+        <v>45553</v>
       </c>
       <c r="D14" t="b">
         <v>0</v>
       </c>
       <c r="E14" t="n">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Findaway</t>
+          <t>BookFunnel</t>
         </is>
       </c>
       <c r="G14" t="n">
-        <v>18.92</v>
+        <v>11.62</v>
       </c>
       <c r="H14" t="b">
         <v>1</v>
       </c>
       <c r="I14" t="n">
-        <v>465</v>
+        <v>351</v>
       </c>
       <c r="J14" t="n">
-        <v>4850</v>
+        <v>3289</v>
       </c>
       <c r="K14" t="n">
-        <v>0.225</v>
+        <v>0.5</v>
       </c>
       <c r="L14" t="n">
-        <v>1979.51</v>
+        <v>2039.31</v>
       </c>
       <c r="M14" t="n">
-        <v>2.5</v>
+        <v>1.6</v>
       </c>
       <c r="N14" t="b">
         <v>1</v>
@@ -1294,16 +1294,16 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Melissa Sanders</t>
+          <t>Vicki Ruiz</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Television partner.</t>
+          <t>Unit rate traditional.</t>
         </is>
       </c>
       <c r="C15" s="2" t="n">
-        <v>45287</v>
+        <v>45288</v>
       </c>
       <c r="D15" t="b">
         <v>0</v>
@@ -1313,29 +1313,29 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Spotify</t>
+          <t>ACX Royalty Share</t>
         </is>
       </c>
       <c r="G15" t="n">
-        <v>14.97</v>
+        <v>9.720000000000001</v>
       </c>
       <c r="H15" t="b">
         <v>1</v>
       </c>
       <c r="I15" t="n">
-        <v>557</v>
+        <v>654</v>
       </c>
       <c r="J15" t="n">
-        <v>4365</v>
+        <v>2938</v>
       </c>
       <c r="K15" t="n">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
       <c r="L15" t="n">
-        <v>2084.57</v>
+        <v>635.6900000000001</v>
       </c>
       <c r="M15" t="n">
-        <v>2.1</v>
+        <v>4.6</v>
       </c>
       <c r="N15" t="b">
         <v>1</v>
@@ -1353,22 +1353,22 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Kelly Potter</t>
+          <t>Daniel Castaneda</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Cover institution then car others.</t>
+          <t>Suddenly rise south positive.</t>
         </is>
       </c>
       <c r="C16" s="2" t="n">
-        <v>45491</v>
+        <v>45411</v>
       </c>
       <c r="D16" t="b">
         <v>0</v>
       </c>
       <c r="E16" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
@@ -1376,25 +1376,25 @@
         </is>
       </c>
       <c r="G16" t="n">
-        <v>16.02</v>
+        <v>17.93</v>
       </c>
       <c r="H16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I16" t="n">
-        <v>643</v>
+        <v>647</v>
       </c>
       <c r="J16" t="n">
-        <v>4885</v>
+        <v>5861</v>
       </c>
       <c r="K16" t="n">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="L16" t="n">
-        <v>2060.17</v>
+        <v>4640.28</v>
       </c>
       <c r="M16" t="n">
-        <v>2.4</v>
+        <v>1.3</v>
       </c>
       <c r="N16" t="b">
         <v>1</v>
@@ -1412,22 +1412,22 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Steven Smith</t>
+          <t>Brent Lopez</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>None figure sit because.</t>
+          <t>Mention someone.</t>
         </is>
       </c>
       <c r="C17" s="2" t="n">
-        <v>45753</v>
+        <v>45670</v>
       </c>
       <c r="D17" t="b">
         <v>0</v>
       </c>
       <c r="E17" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
@@ -1435,25 +1435,25 @@
         </is>
       </c>
       <c r="G17" t="n">
-        <v>14.48</v>
+        <v>15.48</v>
       </c>
       <c r="H17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I17" t="n">
-        <v>746</v>
+        <v>622</v>
       </c>
       <c r="J17" t="n">
-        <v>2396</v>
+        <v>3297</v>
       </c>
       <c r="K17" t="n">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="L17" t="n">
-        <v>4320.83</v>
+        <v>1925.71</v>
       </c>
       <c r="M17" t="n">
-        <v>0.6</v>
+        <v>1.7</v>
       </c>
       <c r="N17" t="b">
         <v>1</v>
@@ -1471,16 +1471,16 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Lisa Davis</t>
+          <t>Sarah Rice</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Clearly example report.</t>
+          <t>Like director activity close.</t>
         </is>
       </c>
       <c r="C18" s="2" t="n">
-        <v>45643</v>
+        <v>45648</v>
       </c>
       <c r="D18" t="b">
         <v>0</v>
@@ -1494,25 +1494,25 @@
         </is>
       </c>
       <c r="G18" t="n">
-        <v>16.38</v>
+        <v>12.93</v>
       </c>
       <c r="H18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I18" t="n">
-        <v>892</v>
+        <v>544</v>
       </c>
       <c r="J18" t="n">
-        <v>5240</v>
+        <v>3073</v>
       </c>
       <c r="K18" t="n">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="L18" t="n">
-        <v>5844.38</v>
+        <v>1406.78</v>
       </c>
       <c r="M18" t="n">
-        <v>0.9</v>
+        <v>2.2</v>
       </c>
       <c r="N18" t="b">
         <v>1</v>
@@ -1530,48 +1530,48 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Michael Boyle</t>
+          <t>Debra Jackson</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Clear bad.</t>
+          <t>Town everything town.</t>
         </is>
       </c>
       <c r="C19" s="2" t="n">
-        <v>45532</v>
+        <v>45411</v>
       </c>
       <c r="D19" t="b">
         <v>0</v>
       </c>
       <c r="E19" t="n">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Spotify</t>
+          <t>ACX Royalty Share</t>
         </is>
       </c>
       <c r="G19" t="n">
-        <v>16.58</v>
+        <v>9.43</v>
       </c>
       <c r="H19" t="b">
         <v>0</v>
       </c>
       <c r="I19" t="n">
-        <v>587</v>
+        <v>532</v>
       </c>
       <c r="J19" t="n">
-        <v>2275</v>
+        <v>2576</v>
       </c>
       <c r="K19" t="n">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="L19" t="n">
-        <v>4866.23</v>
+        <v>2006.7</v>
       </c>
       <c r="M19" t="n">
-        <v>0.5</v>
+        <v>1.3</v>
       </c>
       <c r="N19" t="b">
         <v>1</v>
@@ -1589,48 +1589,48 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Dana Jones</t>
+          <t>Bryan Cherry</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Crime suffer claim investment.</t>
+          <t>Speak however bit boy west.</t>
         </is>
       </c>
       <c r="C20" s="2" t="n">
-        <v>45728</v>
+        <v>45141</v>
       </c>
       <c r="D20" t="b">
         <v>0</v>
       </c>
       <c r="E20" t="n">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>ACX Exclusive</t>
+          <t>BookFunnel</t>
         </is>
       </c>
       <c r="G20" t="n">
-        <v>12.7</v>
+        <v>16.22</v>
       </c>
       <c r="H20" t="b">
         <v>0</v>
       </c>
       <c r="I20" t="n">
-        <v>513</v>
+        <v>882</v>
       </c>
       <c r="J20" t="n">
-        <v>2637</v>
+        <v>4185</v>
       </c>
       <c r="K20" t="n">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="L20" t="n">
-        <v>2606.04</v>
+        <v>14306.04</v>
       </c>
       <c r="M20" t="n">
-        <v>1</v>
+        <v>0.3</v>
       </c>
       <c r="N20" t="b">
         <v>1</v>
@@ -1642,54 +1642,54 @@
         <v>0</v>
       </c>
       <c r="Q20" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Molly Lewis</t>
+          <t>Dr. Margaret Salinas</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Radio word others difficult everybody.</t>
+          <t>Pay popular challenge.</t>
         </is>
       </c>
       <c r="C21" s="2" t="n">
-        <v>45307</v>
+        <v>45480</v>
       </c>
       <c r="D21" t="b">
         <v>0</v>
       </c>
       <c r="E21" t="n">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>ACX Exclusive</t>
+          <t>BookFunnel</t>
         </is>
       </c>
       <c r="G21" t="n">
-        <v>9.140000000000001</v>
+        <v>19.59</v>
       </c>
       <c r="H21" t="b">
         <v>0</v>
       </c>
       <c r="I21" t="n">
-        <v>955</v>
+        <v>980</v>
       </c>
       <c r="J21" t="n">
-        <v>2677</v>
+        <v>3080</v>
       </c>
       <c r="K21" t="n">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="L21" t="n">
-        <v>3491.48</v>
+        <v>19198.2</v>
       </c>
       <c r="M21" t="n">
-        <v>0.8</v>
+        <v>0.2</v>
       </c>
       <c r="N21" t="b">
         <v>1</v>
@@ -1701,54 +1701,54 @@
         <v>0</v>
       </c>
       <c r="Q21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Mr. David Dorsey</t>
+          <t>Ashley Torres</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Pm themselves stop.</t>
+          <t>Item economy.</t>
         </is>
       </c>
       <c r="C22" s="2" t="n">
-        <v>45633</v>
+        <v>45560</v>
       </c>
       <c r="D22" t="b">
         <v>0</v>
       </c>
       <c r="E22" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>ACX Royalty Share</t>
+          <t>Spotify</t>
         </is>
       </c>
       <c r="G22" t="n">
-        <v>14.06</v>
+        <v>13.98</v>
       </c>
       <c r="H22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I22" t="n">
-        <v>690</v>
+        <v>526</v>
       </c>
       <c r="J22" t="n">
-        <v>2662</v>
+        <v>5619</v>
       </c>
       <c r="K22" t="n">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="L22" t="n">
-        <v>970.14</v>
+        <v>3676.74</v>
       </c>
       <c r="M22" t="n">
-        <v>2.7</v>
+        <v>1.5</v>
       </c>
       <c r="N22" t="b">
         <v>1</v>
@@ -1766,48 +1766,48 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Amanda Henry</t>
+          <t>Tiffany Scott</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Bank fill similar.</t>
+          <t>Investment police television million keep.</t>
         </is>
       </c>
       <c r="C23" s="2" t="n">
-        <v>45444</v>
+        <v>45245</v>
       </c>
       <c r="D23" t="b">
         <v>0</v>
       </c>
       <c r="E23" t="n">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>ACX Royalty Share</t>
+          <t>Spotify</t>
         </is>
       </c>
       <c r="G23" t="n">
-        <v>15.24</v>
+        <v>8.27</v>
       </c>
       <c r="H23" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I23" t="n">
-        <v>478</v>
+        <v>427</v>
       </c>
       <c r="J23" t="n">
-        <v>5810</v>
+        <v>5589</v>
       </c>
       <c r="K23" t="n">
-        <v>0.4</v>
+        <v>0.25</v>
       </c>
       <c r="L23" t="n">
-        <v>2913.89</v>
+        <v>882.8200000000001</v>
       </c>
       <c r="M23" t="n">
-        <v>2</v>
+        <v>6.3</v>
       </c>
       <c r="N23" t="b">
         <v>1</v>
@@ -1816,7 +1816,7 @@
         <v>0</v>
       </c>
       <c r="P23" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q23" t="b">
         <v>0</v>
@@ -1825,48 +1825,48 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Benjamin Lara</t>
+          <t>Daniel Smith</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Computer heavy audience soldier charge.</t>
+          <t>Exactly up.</t>
         </is>
       </c>
       <c r="C24" s="2" t="n">
-        <v>45322</v>
+        <v>45516</v>
       </c>
       <c r="D24" t="b">
         <v>0</v>
       </c>
       <c r="E24" t="n">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Findaway</t>
+          <t>ACX Exclusive</t>
         </is>
       </c>
       <c r="G24" t="n">
-        <v>12.56</v>
+        <v>16.91</v>
       </c>
       <c r="H24" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I24" t="n">
-        <v>501</v>
+        <v>801</v>
       </c>
       <c r="J24" t="n">
-        <v>2768</v>
+        <v>4534</v>
       </c>
       <c r="K24" t="n">
-        <v>0.45</v>
+        <v>0.2</v>
       </c>
       <c r="L24" t="n">
-        <v>2831.65</v>
+        <v>2708.98</v>
       </c>
       <c r="M24" t="n">
-        <v>1</v>
+        <v>1.7</v>
       </c>
       <c r="N24" t="b">
         <v>1</v>
@@ -1884,48 +1884,48 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Maria Lewis</t>
+          <t>Erica Fleming</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Nature TV.</t>
+          <t>Action book bring play.</t>
         </is>
       </c>
       <c r="C25" s="2" t="n">
-        <v>45633</v>
+        <v>45192</v>
       </c>
       <c r="D25" t="b">
         <v>0</v>
       </c>
       <c r="E25" t="n">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Findaway</t>
+          <t>ACX Exclusive</t>
         </is>
       </c>
       <c r="G25" t="n">
-        <v>9.83</v>
+        <v>18.77</v>
       </c>
       <c r="H25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I25" t="n">
-        <v>234</v>
+        <v>255</v>
       </c>
       <c r="J25" t="n">
-        <v>1871</v>
+        <v>5032</v>
       </c>
       <c r="K25" t="n">
-        <v>0.45</v>
+        <v>0.2</v>
       </c>
       <c r="L25" t="n">
-        <v>1035.1</v>
+        <v>957.27</v>
       </c>
       <c r="M25" t="n">
-        <v>1.8</v>
+        <v>5.3</v>
       </c>
       <c r="N25" t="b">
         <v>1</v>
@@ -1934,7 +1934,7 @@
         <v>0</v>
       </c>
       <c r="P25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q25" t="b">
         <v>0</v>
@@ -1943,49 +1943,49 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Alan Graves</t>
+          <t>John Fisher</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Public skin position.</t>
+          <t>Between morning church.</t>
         </is>
       </c>
       <c r="C26" s="2" t="n">
-        <v>45165</v>
+        <v>45494</v>
       </c>
       <c r="D26" t="b">
         <v>0</v>
       </c>
       <c r="E26" t="n">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>ACX Royalty Share</t>
+          <t>BookFunnel</t>
         </is>
       </c>
       <c r="G26" t="n">
-        <v>12.79</v>
+        <v>15.37</v>
       </c>
       <c r="H26" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I26" t="n">
-        <v>586</v>
+        <v>928</v>
       </c>
       <c r="J26" t="n">
-        <v>4453</v>
+        <v>1551</v>
       </c>
       <c r="K26" t="n">
+        <v>1</v>
+      </c>
+      <c r="L26" t="n">
+        <v>14263.36</v>
+      </c>
+      <c r="M26" t="n">
         <v>0.1</v>
       </c>
-      <c r="L26" t="n">
-        <v>749.49</v>
-      </c>
-      <c r="M26" t="n">
-        <v>5.9</v>
-      </c>
       <c r="N26" t="b">
         <v>1</v>
       </c>
@@ -1996,57 +1996,57 @@
         <v>0</v>
       </c>
       <c r="Q26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Edward Williams</t>
+          <t>Valerie Reyes</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Large color this.</t>
+          <t>Local tough special idea positive.</t>
         </is>
       </c>
       <c r="C27" s="2" t="n">
-        <v>45844</v>
+        <v>45803</v>
       </c>
       <c r="D27" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E27" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>Spotify</t>
+          <t>BookFunnel</t>
         </is>
       </c>
       <c r="G27" t="n">
-        <v>15.22</v>
+        <v>13.46</v>
       </c>
       <c r="H27" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I27" t="n">
-        <v>154</v>
+        <v>400</v>
       </c>
       <c r="J27" t="n">
-        <v>4953</v>
+        <v>3942</v>
       </c>
       <c r="K27" t="n">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="L27" t="n">
-        <v>585.97</v>
+        <v>5384</v>
       </c>
       <c r="M27" t="n">
-        <v>8.5</v>
+        <v>0.7</v>
       </c>
       <c r="N27" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O27" t="b">
         <v>0</v>
@@ -2061,48 +2061,48 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Angelica Schneider</t>
+          <t>Lori Morris</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Different part.</t>
+          <t>Family none certain.</t>
         </is>
       </c>
       <c r="C28" s="2" t="n">
-        <v>45498</v>
+        <v>45612</v>
       </c>
       <c r="D28" t="b">
         <v>0</v>
       </c>
       <c r="E28" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>Spotify</t>
+          <t>ACX Exclusive</t>
         </is>
       </c>
       <c r="G28" t="n">
-        <v>16.06</v>
+        <v>14.51</v>
       </c>
       <c r="H28" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I28" t="n">
-        <v>204</v>
+        <v>604</v>
       </c>
       <c r="J28" t="n">
-        <v>3300</v>
+        <v>5734</v>
       </c>
       <c r="K28" t="n">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="L28" t="n">
-        <v>1638.12</v>
+        <v>1752.81</v>
       </c>
       <c r="M28" t="n">
-        <v>2</v>
+        <v>3.3</v>
       </c>
       <c r="N28" t="b">
         <v>1</v>
@@ -2111,7 +2111,7 @@
         <v>0</v>
       </c>
       <c r="P28" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q28" t="b">
         <v>0</v>
@@ -2120,22 +2120,22 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Jeremiah Brown</t>
+          <t>James Reynolds</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Story future feeling discuss.</t>
+          <t>Republican have draw public.</t>
         </is>
       </c>
       <c r="C29" s="2" t="n">
-        <v>45684</v>
+        <v>45634</v>
       </c>
       <c r="D29" t="b">
         <v>0</v>
       </c>
       <c r="E29" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F29" t="inlineStr">
         <is>
@@ -2143,25 +2143,25 @@
         </is>
       </c>
       <c r="G29" t="n">
-        <v>16.16</v>
+        <v>15.34</v>
       </c>
       <c r="H29" t="b">
         <v>1</v>
       </c>
       <c r="I29" t="n">
-        <v>711</v>
+        <v>842</v>
       </c>
       <c r="J29" t="n">
-        <v>5307</v>
+        <v>5513</v>
       </c>
       <c r="K29" t="n">
         <v>0.2</v>
       </c>
       <c r="L29" t="n">
-        <v>2297.95</v>
+        <v>2583.26</v>
       </c>
       <c r="M29" t="n">
-        <v>2.3</v>
+        <v>2.1</v>
       </c>
       <c r="N29" t="b">
         <v>1</v>
@@ -2179,51 +2179,51 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>David Cox Jr.</t>
+          <t>Lindsey Adams</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Social building off issue kind.</t>
+          <t>Me final particularly.</t>
         </is>
       </c>
       <c r="C30" s="2" t="n">
-        <v>45198</v>
+        <v>45853</v>
       </c>
       <c r="D30" t="b">
         <v>0</v>
       </c>
       <c r="E30" t="n">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>BookFunnel</t>
+          <t>ACX Royalty Share</t>
         </is>
       </c>
       <c r="G30" t="n">
-        <v>16.96</v>
+        <v>8.84</v>
       </c>
       <c r="H30" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I30" t="n">
-        <v>622</v>
+        <v>123</v>
       </c>
       <c r="J30" t="n">
-        <v>3793</v>
+        <v>3294</v>
       </c>
       <c r="K30" t="n">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="L30" t="n">
-        <v>5274.56</v>
+        <v>434.93</v>
       </c>
       <c r="M30" t="n">
-        <v>0.7</v>
+        <v>7.6</v>
       </c>
       <c r="N30" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O30" t="b">
         <v>0</v>
@@ -2238,48 +2238,48 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Nicole Hughes</t>
+          <t>Margaret Joseph</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>House sell human.</t>
+          <t>Big happy fall.</t>
         </is>
       </c>
       <c r="C31" s="2" t="n">
-        <v>45507</v>
+        <v>45323</v>
       </c>
       <c r="D31" t="b">
         <v>0</v>
       </c>
       <c r="E31" t="n">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>ACX Royalty Share</t>
+          <t>Findaway</t>
         </is>
       </c>
       <c r="G31" t="n">
-        <v>11.39</v>
+        <v>10.96</v>
       </c>
       <c r="H31" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I31" t="n">
-        <v>707</v>
+        <v>869</v>
       </c>
       <c r="J31" t="n">
-        <v>3687</v>
+        <v>5158</v>
       </c>
       <c r="K31" t="n">
-        <v>0.4</v>
+        <v>0.225</v>
       </c>
       <c r="L31" t="n">
-        <v>3221.09</v>
+        <v>2142.95</v>
       </c>
       <c r="M31" t="n">
-        <v>1.1</v>
+        <v>2.4</v>
       </c>
       <c r="N31" t="b">
         <v>1</v>
@@ -2288,7 +2288,7 @@
         <v>0</v>
       </c>
       <c r="P31" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q31" t="b">
         <v>0</v>
@@ -2297,110 +2297,110 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Justin Peterson</t>
+          <t>Joshua Stevens</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Senior result director street improve.</t>
+          <t>Thousand citizen.</t>
         </is>
       </c>
       <c r="C32" s="2" t="n">
-        <v>45292</v>
+        <v>45487</v>
       </c>
       <c r="D32" t="b">
         <v>0</v>
       </c>
       <c r="E32" t="n">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>BookFunnel</t>
+          <t>ACX Royalty Share</t>
         </is>
       </c>
       <c r="G32" t="n">
-        <v>16.77</v>
+        <v>9.220000000000001</v>
       </c>
       <c r="H32" t="b">
         <v>1</v>
       </c>
       <c r="I32" t="n">
-        <v>944</v>
+        <v>219</v>
       </c>
       <c r="J32" t="n">
-        <v>4994</v>
+        <v>5872</v>
       </c>
       <c r="K32" t="n">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="L32" t="n">
-        <v>7915.44</v>
+        <v>201.92</v>
       </c>
       <c r="M32" t="n">
-        <v>0.6</v>
+        <v>29.1</v>
       </c>
       <c r="N32" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O32" t="b">
         <v>0</v>
       </c>
       <c r="P32" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q32" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Melissa Nelson</t>
+          <t>Nathan Estrada</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Inside lawyer some experience.</t>
+          <t>Specific guy point involve human.</t>
         </is>
       </c>
       <c r="C33" s="2" t="n">
-        <v>45567</v>
+        <v>45847</v>
       </c>
       <c r="D33" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E33" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>Findaway</t>
+          <t>BookFunnel</t>
         </is>
       </c>
       <c r="G33" t="n">
-        <v>19.21</v>
+        <v>15.77</v>
       </c>
       <c r="H33" t="b">
         <v>0</v>
       </c>
       <c r="I33" t="n">
-        <v>676</v>
+        <v>196</v>
       </c>
       <c r="J33" t="n">
-        <v>3411</v>
+        <v>2540</v>
       </c>
       <c r="K33" t="n">
-        <v>0.45</v>
+        <v>1</v>
       </c>
       <c r="L33" t="n">
-        <v>5843.68</v>
+        <v>3090.92</v>
       </c>
       <c r="M33" t="n">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
       <c r="N33" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O33" t="b">
         <v>0</v>
@@ -2415,48 +2415,48 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Cheryl Gilbert</t>
+          <t>Lori Adams</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Democratic region simple fine chance.</t>
+          <t>Young best chance pay.</t>
         </is>
       </c>
       <c r="C34" s="2" t="n">
-        <v>45657</v>
+        <v>45264</v>
       </c>
       <c r="D34" t="b">
         <v>0</v>
       </c>
       <c r="E34" t="n">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>ACX Royalty Share</t>
+          <t>BookFunnel</t>
         </is>
       </c>
       <c r="G34" t="n">
-        <v>14.32</v>
+        <v>13.45</v>
       </c>
       <c r="H34" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I34" t="n">
-        <v>890</v>
+        <v>387</v>
       </c>
       <c r="J34" t="n">
-        <v>5496</v>
+        <v>4233</v>
       </c>
       <c r="K34" t="n">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="L34" t="n">
-        <v>5097.92</v>
+        <v>2602.57</v>
       </c>
       <c r="M34" t="n">
-        <v>1.1</v>
+        <v>1.6</v>
       </c>
       <c r="N34" t="b">
         <v>1</v>
@@ -2474,51 +2474,51 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Mark Roberts</t>
+          <t>Lauren Gregory</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Former him article perform capital.</t>
+          <t>Who interview hot town.</t>
         </is>
       </c>
       <c r="C35" s="2" t="n">
-        <v>45518</v>
+        <v>45865</v>
       </c>
       <c r="D35" t="b">
         <v>0</v>
       </c>
       <c r="E35" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>ACX Royalty Share</t>
+          <t>BookFunnel</t>
         </is>
       </c>
       <c r="G35" t="n">
-        <v>12.41</v>
+        <v>12.82</v>
       </c>
       <c r="H35" t="b">
         <v>0</v>
       </c>
       <c r="I35" t="n">
-        <v>498</v>
+        <v>128</v>
       </c>
       <c r="J35" t="n">
-        <v>5716</v>
+        <v>5651</v>
       </c>
       <c r="K35" t="n">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="L35" t="n">
-        <v>2472.07</v>
+        <v>1640.96</v>
       </c>
       <c r="M35" t="n">
-        <v>2.3</v>
+        <v>3.4</v>
       </c>
       <c r="N35" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O35" t="b">
         <v>0</v>
@@ -2533,48 +2533,48 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Tonya Marquez</t>
+          <t>Megan Brown</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Health police.</t>
+          <t>Type style amount.</t>
         </is>
       </c>
       <c r="C36" s="2" t="n">
-        <v>45165</v>
+        <v>45231</v>
       </c>
       <c r="D36" t="b">
         <v>0</v>
       </c>
       <c r="E36" t="n">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>Spotify</t>
+          <t>Findaway</t>
         </is>
       </c>
       <c r="G36" t="n">
-        <v>18.21</v>
+        <v>12.06</v>
       </c>
       <c r="H36" t="b">
         <v>1</v>
       </c>
       <c r="I36" t="n">
-        <v>547</v>
+        <v>240</v>
       </c>
       <c r="J36" t="n">
-        <v>2669</v>
+        <v>3684</v>
       </c>
       <c r="K36" t="n">
-        <v>0.25</v>
+        <v>0.225</v>
       </c>
       <c r="L36" t="n">
-        <v>2490.22</v>
+        <v>651.24</v>
       </c>
       <c r="M36" t="n">
-        <v>1.1</v>
+        <v>5.7</v>
       </c>
       <c r="N36" t="b">
         <v>1</v>
@@ -2592,48 +2592,48 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Aaron Rose</t>
+          <t>Cory Harris</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Car job there.</t>
+          <t>Whether player.</t>
         </is>
       </c>
       <c r="C37" s="2" t="n">
-        <v>45435</v>
+        <v>45206</v>
       </c>
       <c r="D37" t="b">
         <v>0</v>
       </c>
       <c r="E37" t="n">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>BookFunnel</t>
+          <t>Spotify</t>
         </is>
       </c>
       <c r="G37" t="n">
-        <v>8.220000000000001</v>
+        <v>15.21</v>
       </c>
       <c r="H37" t="b">
         <v>1</v>
       </c>
       <c r="I37" t="n">
-        <v>489</v>
+        <v>357</v>
       </c>
       <c r="J37" t="n">
-        <v>2009</v>
+        <v>3693</v>
       </c>
       <c r="K37" t="n">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="L37" t="n">
-        <v>2009.79</v>
+        <v>1357.49</v>
       </c>
       <c r="M37" t="n">
-        <v>1</v>
+        <v>2.7</v>
       </c>
       <c r="N37" t="b">
         <v>1</v>
@@ -2651,48 +2651,48 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Courtney Murphy</t>
+          <t>Lisa Kemp</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Must art behavior.</t>
+          <t>Before site seek according ten.</t>
         </is>
       </c>
       <c r="C38" s="2" t="n">
-        <v>45463</v>
+        <v>45569</v>
       </c>
       <c r="D38" t="b">
         <v>0</v>
       </c>
       <c r="E38" t="n">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>ACX Exclusive</t>
+          <t>ACX Royalty Share</t>
         </is>
       </c>
       <c r="G38" t="n">
-        <v>14.84</v>
+        <v>17</v>
       </c>
       <c r="H38" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I38" t="n">
-        <v>383</v>
+        <v>826</v>
       </c>
       <c r="J38" t="n">
-        <v>5973</v>
+        <v>4254</v>
       </c>
       <c r="K38" t="n">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="L38" t="n">
-        <v>1136.74</v>
+        <v>5616.8</v>
       </c>
       <c r="M38" t="n">
-        <v>5.3</v>
+        <v>0.8</v>
       </c>
       <c r="N38" t="b">
         <v>1</v>
@@ -2701,7 +2701,7 @@
         <v>0</v>
       </c>
       <c r="P38" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q38" t="b">
         <v>0</v>
@@ -2710,16 +2710,16 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Scott Ross</t>
+          <t>Bonnie Gomez</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Off stuff couple.</t>
+          <t>Old read couple create.</t>
         </is>
       </c>
       <c r="C39" s="2" t="n">
-        <v>45411</v>
+        <v>45419</v>
       </c>
       <c r="D39" t="b">
         <v>0</v>
@@ -2733,25 +2733,25 @@
         </is>
       </c>
       <c r="G39" t="n">
-        <v>14.12</v>
+        <v>13.18</v>
       </c>
       <c r="H39" t="b">
         <v>1</v>
       </c>
       <c r="I39" t="n">
-        <v>245</v>
+        <v>903</v>
       </c>
       <c r="J39" t="n">
-        <v>1516</v>
+        <v>5818</v>
       </c>
       <c r="K39" t="n">
         <v>0.225</v>
       </c>
       <c r="L39" t="n">
-        <v>778.37</v>
+        <v>2677.85</v>
       </c>
       <c r="M39" t="n">
-        <v>1.9</v>
+        <v>2.2</v>
       </c>
       <c r="N39" t="b">
         <v>1</v>
@@ -2760,7 +2760,7 @@
         <v>0</v>
       </c>
       <c r="P39" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q39" t="b">
         <v>0</v>
@@ -2769,48 +2769,48 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Mary Carson</t>
+          <t>Travis Gallagher</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Talk through.</t>
+          <t>Write significant seem.</t>
         </is>
       </c>
       <c r="C40" s="2" t="n">
-        <v>45212</v>
+        <v>45278</v>
       </c>
       <c r="D40" t="b">
         <v>0</v>
       </c>
       <c r="E40" t="n">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>Spotify</t>
+          <t>BookFunnel</t>
         </is>
       </c>
       <c r="G40" t="n">
-        <v>15.7</v>
+        <v>15.47</v>
       </c>
       <c r="H40" t="b">
         <v>1</v>
       </c>
       <c r="I40" t="n">
-        <v>791</v>
+        <v>958</v>
       </c>
       <c r="J40" t="n">
-        <v>5438</v>
+        <v>1511</v>
       </c>
       <c r="K40" t="n">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="L40" t="n">
-        <v>3104.67</v>
+        <v>7410.13</v>
       </c>
       <c r="M40" t="n">
-        <v>1.8</v>
+        <v>0.2</v>
       </c>
       <c r="N40" t="b">
         <v>1</v>
@@ -2819,57 +2819,57 @@
         <v>0</v>
       </c>
       <c r="P40" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q40" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Taylor Johnson</t>
+          <t>Gregory Brown</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Wear pick network staff.</t>
+          <t>Chance which.</t>
         </is>
       </c>
       <c r="C41" s="2" t="n">
-        <v>45243</v>
+        <v>45198</v>
       </c>
       <c r="D41" t="b">
         <v>0</v>
       </c>
       <c r="E41" t="n">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>ACX Exclusive</t>
+          <t>BookFunnel</t>
         </is>
       </c>
       <c r="G41" t="n">
-        <v>14.73</v>
+        <v>17.06</v>
       </c>
       <c r="H41" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I41" t="n">
-        <v>272</v>
+        <v>815</v>
       </c>
       <c r="J41" t="n">
-        <v>2581</v>
+        <v>5560</v>
       </c>
       <c r="K41" t="n">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="L41" t="n">
-        <v>1602.62</v>
+        <v>6951.95</v>
       </c>
       <c r="M41" t="n">
-        <v>1.6</v>
+        <v>0.8</v>
       </c>
       <c r="N41" t="b">
         <v>1</v>
@@ -2881,28 +2881,28 @@
         <v>0</v>
       </c>
       <c r="Q41" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Gary Sanders</t>
+          <t>Jordan Bender</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Guess hear rather.</t>
+          <t>Improve while early performance happy.</t>
         </is>
       </c>
       <c r="C42" s="2" t="n">
-        <v>45303</v>
+        <v>45714</v>
       </c>
       <c r="D42" t="b">
         <v>0</v>
       </c>
       <c r="E42" t="n">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="F42" t="inlineStr">
         <is>
@@ -2910,28 +2910,28 @@
         </is>
       </c>
       <c r="G42" t="n">
-        <v>10.39</v>
+        <v>19.41</v>
       </c>
       <c r="H42" t="b">
         <v>1</v>
       </c>
       <c r="I42" t="n">
-        <v>941</v>
+        <v>243</v>
       </c>
       <c r="J42" t="n">
-        <v>2838</v>
+        <v>4282</v>
       </c>
       <c r="K42" t="n">
         <v>0.1</v>
       </c>
       <c r="L42" t="n">
-        <v>977.7</v>
+        <v>471.66</v>
       </c>
       <c r="M42" t="n">
-        <v>2.9</v>
+        <v>9.1</v>
       </c>
       <c r="N42" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O42" t="b">
         <v>0</v>
@@ -2946,48 +2946,48 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Walter Martinez</t>
+          <t>Brenda Cherry MD</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Research each brother film.</t>
+          <t>Decade nor day nor.</t>
         </is>
       </c>
       <c r="C43" s="2" t="n">
-        <v>45217</v>
+        <v>45398</v>
       </c>
       <c r="D43" t="b">
         <v>0</v>
       </c>
       <c r="E43" t="n">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>Findaway</t>
+          <t>ACX Exclusive</t>
         </is>
       </c>
       <c r="G43" t="n">
-        <v>14.44</v>
+        <v>13.77</v>
       </c>
       <c r="H43" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I43" t="n">
-        <v>346</v>
+        <v>278</v>
       </c>
       <c r="J43" t="n">
-        <v>3360</v>
+        <v>5794</v>
       </c>
       <c r="K43" t="n">
-        <v>0.225</v>
+        <v>0.4</v>
       </c>
       <c r="L43" t="n">
-        <v>1124.15</v>
+        <v>1531.22</v>
       </c>
       <c r="M43" t="n">
-        <v>3</v>
+        <v>3.8</v>
       </c>
       <c r="N43" t="b">
         <v>1</v>
@@ -3005,57 +3005,57 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Timothy Lopez</t>
+          <t>Theresa Campbell</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Exist trip.</t>
+          <t>American attention clear.</t>
         </is>
       </c>
       <c r="C44" s="2" t="n">
-        <v>45803</v>
+        <v>45612</v>
       </c>
       <c r="D44" t="b">
         <v>0</v>
       </c>
       <c r="E44" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>Findaway</t>
+          <t>ACX Exclusive</t>
         </is>
       </c>
       <c r="G44" t="n">
-        <v>14.16</v>
+        <v>15.3</v>
       </c>
       <c r="H44" t="b">
         <v>1</v>
       </c>
       <c r="I44" t="n">
-        <v>454</v>
+        <v>941</v>
       </c>
       <c r="J44" t="n">
-        <v>3197</v>
+        <v>5519</v>
       </c>
       <c r="K44" t="n">
-        <v>0.225</v>
+        <v>0.2</v>
       </c>
       <c r="L44" t="n">
-        <v>1446.44</v>
+        <v>2879.46</v>
       </c>
       <c r="M44" t="n">
-        <v>2.2</v>
+        <v>1.9</v>
       </c>
       <c r="N44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O44" t="b">
         <v>0</v>
       </c>
       <c r="P44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q44" t="b">
         <v>0</v>
@@ -3064,48 +3064,48 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Christopher Miller</t>
+          <t>Brenda Morales</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Matter glass discussion.</t>
+          <t>State everyone community.</t>
         </is>
       </c>
       <c r="C45" s="2" t="n">
-        <v>45627</v>
+        <v>45582</v>
       </c>
       <c r="D45" t="b">
         <v>0</v>
       </c>
       <c r="E45" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>Findaway</t>
+          <t>BookFunnel</t>
         </is>
       </c>
       <c r="G45" t="n">
-        <v>11.98</v>
+        <v>9.43</v>
       </c>
       <c r="H45" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I45" t="n">
-        <v>573</v>
+        <v>813</v>
       </c>
       <c r="J45" t="n">
-        <v>4566</v>
+        <v>4983</v>
       </c>
       <c r="K45" t="n">
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="L45" t="n">
-        <v>3089.04</v>
+        <v>3833.3</v>
       </c>
       <c r="M45" t="n">
-        <v>1.5</v>
+        <v>1.3</v>
       </c>
       <c r="N45" t="b">
         <v>1</v>
@@ -3117,28 +3117,28 @@
         <v>0</v>
       </c>
       <c r="Q45" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Mark Miller</t>
+          <t>David Arnold</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Catch for.</t>
+          <t>Person manager.</t>
         </is>
       </c>
       <c r="C46" s="2" t="n">
-        <v>45781</v>
+        <v>45854</v>
       </c>
       <c r="D46" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E46" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F46" t="inlineStr">
         <is>
@@ -3146,28 +3146,28 @@
         </is>
       </c>
       <c r="G46" t="n">
-        <v>18.92</v>
+        <v>18.93</v>
       </c>
       <c r="H46" t="b">
         <v>0</v>
       </c>
       <c r="I46" t="n">
-        <v>379</v>
+        <v>215</v>
       </c>
       <c r="J46" t="n">
-        <v>1606</v>
+        <v>3995</v>
       </c>
       <c r="K46" t="n">
         <v>0.4</v>
       </c>
       <c r="L46" t="n">
-        <v>2868.27</v>
+        <v>1627.98</v>
       </c>
       <c r="M46" t="n">
-        <v>0.6</v>
+        <v>2.5</v>
       </c>
       <c r="N46" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O46" t="b">
         <v>0</v>
@@ -3182,22 +3182,22 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Richard Gonzalez</t>
+          <t>Steven Ponce</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Agency phone country news itself.</t>
+          <t>Thus record culture.</t>
         </is>
       </c>
       <c r="C47" s="2" t="n">
-        <v>45499</v>
+        <v>45531</v>
       </c>
       <c r="D47" t="b">
         <v>0</v>
       </c>
       <c r="E47" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F47" t="inlineStr">
         <is>
@@ -3205,34 +3205,34 @@
         </is>
       </c>
       <c r="G47" t="n">
-        <v>8.43</v>
+        <v>12.7</v>
       </c>
       <c r="H47" t="b">
         <v>1</v>
       </c>
       <c r="I47" t="n">
-        <v>280</v>
+        <v>865</v>
       </c>
       <c r="J47" t="n">
-        <v>5874</v>
+        <v>3615</v>
       </c>
       <c r="K47" t="n">
         <v>0.2</v>
       </c>
       <c r="L47" t="n">
-        <v>472.08</v>
+        <v>2197.1</v>
       </c>
       <c r="M47" t="n">
-        <v>12.4</v>
+        <v>1.6</v>
       </c>
       <c r="N47" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O47" t="b">
         <v>0</v>
       </c>
       <c r="P47" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q47" t="b">
         <v>0</v>
@@ -3241,22 +3241,22 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Alan Brooks</t>
+          <t>David Murray</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Lose half air tell.</t>
+          <t>Participant itself market religious president.</t>
         </is>
       </c>
       <c r="C48" s="2" t="n">
-        <v>45679</v>
+        <v>45480</v>
       </c>
       <c r="D48" t="b">
         <v>0</v>
       </c>
       <c r="E48" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="F48" t="inlineStr">
         <is>
@@ -3264,28 +3264,28 @@
         </is>
       </c>
       <c r="G48" t="n">
-        <v>18.95</v>
+        <v>13.89</v>
       </c>
       <c r="H48" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I48" t="n">
-        <v>204</v>
+        <v>351</v>
       </c>
       <c r="J48" t="n">
-        <v>3910</v>
+        <v>2772</v>
       </c>
       <c r="K48" t="n">
-        <v>0.1</v>
+        <v>0.4</v>
       </c>
       <c r="L48" t="n">
-        <v>386.58</v>
+        <v>1950.16</v>
       </c>
       <c r="M48" t="n">
-        <v>10.1</v>
+        <v>1.4</v>
       </c>
       <c r="N48" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O48" t="b">
         <v>0</v>
@@ -3300,48 +3300,48 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Anna Scott</t>
+          <t>Bryan Lynn</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Organization listen.</t>
+          <t>Since former contain.</t>
         </is>
       </c>
       <c r="C49" s="2" t="n">
-        <v>45288</v>
+        <v>45752</v>
       </c>
       <c r="D49" t="b">
         <v>0</v>
       </c>
       <c r="E49" t="n">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>Spotify</t>
+          <t>ACX Exclusive</t>
         </is>
       </c>
       <c r="G49" t="n">
-        <v>10.32</v>
+        <v>16.57</v>
       </c>
       <c r="H49" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I49" t="n">
-        <v>396</v>
+        <v>540</v>
       </c>
       <c r="J49" t="n">
-        <v>2990</v>
+        <v>5229</v>
       </c>
       <c r="K49" t="n">
-        <v>0.25</v>
+        <v>0.4</v>
       </c>
       <c r="L49" t="n">
-        <v>1021.68</v>
+        <v>3579.12</v>
       </c>
       <c r="M49" t="n">
-        <v>2.9</v>
+        <v>1.5</v>
       </c>
       <c r="N49" t="b">
         <v>1</v>
@@ -3359,22 +3359,22 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Andrew Escobar</t>
+          <t>Kristy Hunt</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>She environment school collection provide.</t>
+          <t>Again watch.</t>
         </is>
       </c>
       <c r="C50" s="2" t="n">
-        <v>45161</v>
+        <v>45683</v>
       </c>
       <c r="D50" t="b">
         <v>0</v>
       </c>
       <c r="E50" t="n">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="F50" t="inlineStr">
         <is>
@@ -3382,25 +3382,25 @@
         </is>
       </c>
       <c r="G50" t="n">
-        <v>10.66</v>
+        <v>19.18</v>
       </c>
       <c r="H50" t="b">
         <v>1</v>
       </c>
       <c r="I50" t="n">
-        <v>367</v>
+        <v>615</v>
       </c>
       <c r="J50" t="n">
-        <v>2525</v>
+        <v>3996</v>
       </c>
       <c r="K50" t="n">
         <v>0.225</v>
       </c>
       <c r="L50" t="n">
-        <v>880.25</v>
+        <v>2654.03</v>
       </c>
       <c r="M50" t="n">
-        <v>2.9</v>
+        <v>1.5</v>
       </c>
       <c r="N50" t="b">
         <v>1</v>
@@ -3418,57 +3418,57 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Phyllis Flowers</t>
+          <t>Jessica Garcia</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Consumer total include reason.</t>
+          <t>Method worry without.</t>
         </is>
       </c>
       <c r="C51" s="2" t="n">
-        <v>45280</v>
+        <v>45809</v>
       </c>
       <c r="D51" t="b">
         <v>0</v>
       </c>
       <c r="E51" t="n">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>ACX Exclusive</t>
+          <t>ACX Royalty Share</t>
         </is>
       </c>
       <c r="G51" t="n">
-        <v>12.69</v>
+        <v>14.74</v>
       </c>
       <c r="H51" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I51" t="n">
-        <v>733</v>
+        <v>390</v>
       </c>
       <c r="J51" t="n">
-        <v>5813</v>
+        <v>5242</v>
       </c>
       <c r="K51" t="n">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="L51" t="n">
-        <v>1860.35</v>
+        <v>2299.44</v>
       </c>
       <c r="M51" t="n">
-        <v>3.1</v>
+        <v>2.3</v>
       </c>
       <c r="N51" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O51" t="b">
         <v>0</v>
       </c>
       <c r="P51" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q51" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
Updated Break Even functionality
</commit_message>
<xml_diff>
--- a/FakeRoyaltyData.xlsx
+++ b/FakeRoyaltyData.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S51"/>
+  <dimension ref="A1:T51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -533,26 +533,31 @@
           <t>Overachiever</t>
         </is>
       </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>ACX Royalty Share Risk</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Theresa Abbott</t>
+          <t>Bryan Haynes</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Serious nothing once.</t>
+          <t>Explain ahead.</t>
         </is>
       </c>
       <c r="C2" s="2" t="n">
-        <v>45258</v>
+        <v>45799</v>
       </c>
       <c r="D2" t="b">
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -560,36 +565,36 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>19.07</v>
+        <v>8.210000000000001</v>
       </c>
       <c r="H2" t="n">
-        <v>3971.5606194396</v>
+        <v>3932.968438557998</v>
       </c>
       <c r="I2" t="b">
         <v>0</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>Taylor James</t>
+          <t>Rachel Scott</t>
         </is>
       </c>
       <c r="K2" t="b">
         <v>0</v>
       </c>
       <c r="L2" t="n">
-        <v>470</v>
+        <v>195</v>
       </c>
       <c r="M2" t="n">
         <v>0.4</v>
       </c>
       <c r="N2" t="n">
-        <v>3585.16</v>
+        <v>640.38</v>
       </c>
       <c r="O2" t="n">
-        <v>1.1</v>
+        <v>6.1</v>
       </c>
       <c r="P2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q2" t="b">
         <v>0</v>
@@ -598,65 +603,70 @@
         <v>0</v>
       </c>
       <c r="S2" t="b">
+        <v>0</v>
+      </c>
+      <c r="T2" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Edward Jones</t>
+          <t>Jonathan Wilkins</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Write reality management.</t>
+          <t>Represent however.</t>
         </is>
       </c>
       <c r="C3" s="2" t="n">
-        <v>45387</v>
+        <v>45351</v>
       </c>
       <c r="D3" t="b">
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>BookFunnel</t>
+          <t>ACX Royalty Share</t>
         </is>
       </c>
       <c r="G3" t="n">
-        <v>15.3</v>
+        <v>16.82</v>
       </c>
       <c r="H3" t="n">
-        <v>6449.470619203234</v>
+        <v>0</v>
       </c>
       <c r="I3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>Samantha Prescott</t>
+          <t>AI Narrator</t>
         </is>
       </c>
       <c r="K3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L3" t="n">
-        <v>752</v>
+        <v>270</v>
       </c>
       <c r="M3" t="n">
-        <v>1</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="N3" t="n">
-        <v>11505.6</v>
-      </c>
-      <c r="O3" t="n">
-        <v>0.6</v>
+        <v>317.9</v>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>Never</t>
+        </is>
       </c>
       <c r="P3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q3" t="b">
         <v>0</v>
@@ -666,38 +676,41 @@
       </c>
       <c r="S3" t="b">
         <v>0</v>
+      </c>
+      <c r="T3" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Cindy Johnson</t>
+          <t>Jessica King</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>School lay like guess.</t>
+          <t>Factor positive ahead kitchen.</t>
         </is>
       </c>
       <c r="C4" s="2" t="n">
-        <v>45319</v>
+        <v>45422</v>
       </c>
       <c r="D4" t="b">
         <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Spotify</t>
+          <t>ACX Exclusive</t>
         </is>
       </c>
       <c r="G4" t="n">
-        <v>12.21</v>
+        <v>9.07</v>
       </c>
       <c r="H4" t="n">
-        <v>3688.627705826369</v>
+        <v>3651.262443047395</v>
       </c>
       <c r="I4" t="b">
         <v>0</v>
@@ -711,16 +724,16 @@
         <v>0</v>
       </c>
       <c r="L4" t="n">
-        <v>913</v>
+        <v>471</v>
       </c>
       <c r="M4" t="n">
-        <v>0.47</v>
+        <v>0.4</v>
       </c>
       <c r="N4" t="n">
-        <v>5239.43</v>
+        <v>1708.79</v>
       </c>
       <c r="O4" t="n">
-        <v>0.7</v>
+        <v>2.1</v>
       </c>
       <c r="P4" t="b">
         <v>1</v>
@@ -732,62 +745,65 @@
         <v>0</v>
       </c>
       <c r="S4" t="b">
+        <v>0</v>
+      </c>
+      <c r="T4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Daniel Bright</t>
+          <t>Anthony Martinez</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Whatever deep gun situation week.</t>
+          <t>Moment year challenge.</t>
         </is>
       </c>
       <c r="C5" s="2" t="n">
-        <v>45140</v>
+        <v>45272</v>
       </c>
       <c r="D5" t="b">
         <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>BookFunnel</t>
+          <t>ACX Royalty Share</t>
         </is>
       </c>
       <c r="G5" t="n">
-        <v>15.7</v>
+        <v>14.36</v>
       </c>
       <c r="H5" t="n">
-        <v>5429.449913715401</v>
+        <v>950.7898537906642</v>
       </c>
       <c r="I5" t="b">
         <v>0</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>Samantha Prescott</t>
+          <t>AI Narrator</t>
         </is>
       </c>
       <c r="K5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L5" t="n">
-        <v>968</v>
+        <v>233</v>
       </c>
       <c r="M5" t="n">
-        <v>1</v>
+        <v>0.202</v>
       </c>
       <c r="N5" t="n">
-        <v>15197.6</v>
+        <v>675.87</v>
       </c>
       <c r="O5" t="n">
-        <v>0.4</v>
+        <v>1.4</v>
       </c>
       <c r="P5" t="b">
         <v>1</v>
@@ -799,28 +815,31 @@
         <v>0</v>
       </c>
       <c r="S5" t="b">
+        <v>0</v>
+      </c>
+      <c r="T5" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Dakota Taylor</t>
+          <t>Donald Lewis</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Note practice.</t>
+          <t>Side along home join.</t>
         </is>
       </c>
       <c r="C6" s="2" t="n">
-        <v>45515</v>
+        <v>45371</v>
       </c>
       <c r="D6" t="b">
         <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
@@ -828,33 +847,33 @@
         </is>
       </c>
       <c r="G6" t="n">
-        <v>15.24</v>
+        <v>12.78</v>
       </c>
       <c r="H6" t="n">
-        <v>569.1045028602059</v>
+        <v>6377.844990895401</v>
       </c>
       <c r="I6" t="b">
         <v>0</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>AI Narrator</t>
+          <t>Ava Winters</t>
         </is>
       </c>
       <c r="K6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L6" t="n">
-        <v>829</v>
+        <v>686</v>
       </c>
       <c r="M6" t="n">
         <v>0.4</v>
       </c>
       <c r="N6" t="n">
-        <v>5053.58</v>
+        <v>3506.83</v>
       </c>
       <c r="O6" t="n">
-        <v>0.1</v>
+        <v>1.8</v>
       </c>
       <c r="P6" t="b">
         <v>1</v>
@@ -866,62 +885,65 @@
         <v>0</v>
       </c>
       <c r="S6" t="b">
+        <v>0</v>
+      </c>
+      <c r="T6" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Leah Edwards</t>
+          <t>Rebecca Lindsey</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Color writer professional.</t>
+          <t>Behind again up visit.</t>
         </is>
       </c>
       <c r="C7" s="2" t="n">
-        <v>45478</v>
+        <v>45727</v>
       </c>
       <c r="D7" t="b">
         <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Spotify</t>
+          <t>Findaway</t>
         </is>
       </c>
       <c r="G7" t="n">
-        <v>14.19</v>
+        <v>19.11</v>
       </c>
       <c r="H7" t="n">
-        <v>3041.019055061529</v>
+        <v>6593.356572053783</v>
       </c>
       <c r="I7" t="b">
         <v>0</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>Taylor James</t>
+          <t>Ava Winters</t>
         </is>
       </c>
       <c r="K7" t="b">
         <v>0</v>
       </c>
       <c r="L7" t="n">
-        <v>232</v>
+        <v>470</v>
       </c>
       <c r="M7" t="n">
-        <v>0.396</v>
+        <v>0.354</v>
       </c>
       <c r="N7" t="n">
-        <v>1303.66</v>
+        <v>3179.52</v>
       </c>
       <c r="O7" t="n">
-        <v>2.3</v>
+        <v>2.1</v>
       </c>
       <c r="P7" t="b">
         <v>1</v>
@@ -933,65 +955,68 @@
         <v>0</v>
       </c>
       <c r="S7" t="b">
+        <v>0</v>
+      </c>
+      <c r="T7" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Kerri Lewis</t>
+          <t>Tara Martin</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Story number usually.</t>
+          <t>Over write street national.</t>
         </is>
       </c>
       <c r="C8" s="2" t="n">
-        <v>45797</v>
+        <v>45514</v>
       </c>
       <c r="D8" t="b">
         <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Spotify</t>
+          <t>Findaway</t>
         </is>
       </c>
       <c r="G8" t="n">
-        <v>19.87</v>
+        <v>14.19</v>
       </c>
       <c r="H8" t="n">
-        <v>6013.847733186208</v>
+        <v>3050.656946880579</v>
       </c>
       <c r="I8" t="b">
         <v>0</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>Ava Winters</t>
+          <t>Taylor James</t>
         </is>
       </c>
       <c r="K8" t="b">
         <v>0</v>
       </c>
       <c r="L8" t="n">
-        <v>246</v>
+        <v>897</v>
       </c>
       <c r="M8" t="n">
-        <v>0.309</v>
+        <v>0.314</v>
       </c>
       <c r="N8" t="n">
-        <v>1510.4</v>
+        <v>3996.73</v>
       </c>
       <c r="O8" t="n">
-        <v>4</v>
+        <v>0.8</v>
       </c>
       <c r="P8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q8" t="b">
         <v>0</v>
@@ -1000,62 +1025,65 @@
         <v>0</v>
       </c>
       <c r="S8" t="b">
+        <v>0</v>
+      </c>
+      <c r="T8" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Chad Farley</t>
+          <t>Andrea Matthews</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Industry scene own true.</t>
+          <t>Require she practice rich matter.</t>
         </is>
       </c>
       <c r="C9" s="2" t="n">
-        <v>45662</v>
+        <v>45401</v>
       </c>
       <c r="D9" t="b">
         <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>BookFunnel</t>
+          <t>Findaway</t>
         </is>
       </c>
       <c r="G9" t="n">
-        <v>14.02</v>
+        <v>12.73</v>
       </c>
       <c r="H9" t="n">
-        <v>211.1348780633007</v>
+        <v>6611.345762147565</v>
       </c>
       <c r="I9" t="b">
         <v>0</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>AI Narrator</t>
+          <t>Ava Winters</t>
         </is>
       </c>
       <c r="K9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L9" t="n">
-        <v>609</v>
+        <v>470</v>
       </c>
       <c r="M9" t="n">
-        <v>1</v>
+        <v>0.399</v>
       </c>
       <c r="N9" t="n">
-        <v>8538.18</v>
+        <v>2387.26</v>
       </c>
       <c r="O9" t="n">
-        <v>0</v>
+        <v>2.8</v>
       </c>
       <c r="P9" t="b">
         <v>1</v>
@@ -1067,62 +1095,65 @@
         <v>0</v>
       </c>
       <c r="S9" t="b">
+        <v>0</v>
+      </c>
+      <c r="T9" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Seth Medina</t>
+          <t>Kenneth Williams</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Hand shoulder food.</t>
+          <t>Also market leader prove.</t>
         </is>
       </c>
       <c r="C10" s="2" t="n">
-        <v>45300</v>
+        <v>45746</v>
       </c>
       <c r="D10" t="b">
         <v>0</v>
       </c>
       <c r="E10" t="n">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Findaway</t>
+          <t>Spotify</t>
         </is>
       </c>
       <c r="G10" t="n">
-        <v>15.23</v>
+        <v>11.54</v>
       </c>
       <c r="H10" t="n">
-        <v>6602.479020597135</v>
+        <v>3529.160304959022</v>
       </c>
       <c r="I10" t="b">
         <v>0</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>Jason Clarke</t>
+          <t>Taylor James</t>
         </is>
       </c>
       <c r="K10" t="b">
         <v>0</v>
       </c>
       <c r="L10" t="n">
-        <v>231</v>
+        <v>283</v>
       </c>
       <c r="M10" t="n">
-        <v>0.417</v>
+        <v>0.317</v>
       </c>
       <c r="N10" t="n">
-        <v>1467.06</v>
+        <v>1035.26</v>
       </c>
       <c r="O10" t="n">
-        <v>4.5</v>
+        <v>3.4</v>
       </c>
       <c r="P10" t="b">
         <v>1</v>
@@ -1134,65 +1165,68 @@
         <v>0</v>
       </c>
       <c r="S10" t="b">
+        <v>0</v>
+      </c>
+      <c r="T10" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Julie Ramirez</t>
+          <t>Tiffany Hernandez</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Body think.</t>
+          <t>Seven perhaps.</t>
         </is>
       </c>
       <c r="C11" s="2" t="n">
-        <v>45289</v>
+        <v>45734</v>
       </c>
       <c r="D11" t="b">
         <v>0</v>
       </c>
       <c r="E11" t="n">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Spotify</t>
+          <t>Findaway</t>
         </is>
       </c>
       <c r="G11" t="n">
-        <v>13.64</v>
+        <v>17.58</v>
       </c>
       <c r="H11" t="n">
-        <v>3051.74517999494</v>
+        <v>6180.114869840088</v>
       </c>
       <c r="I11" t="b">
         <v>0</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>Taylor James</t>
+          <t>Jason Clarke</t>
         </is>
       </c>
       <c r="K11" t="b">
         <v>0</v>
       </c>
       <c r="L11" t="n">
-        <v>499</v>
+        <v>153</v>
       </c>
       <c r="M11" t="n">
-        <v>0.317</v>
+        <v>0.375</v>
       </c>
       <c r="N11" t="n">
-        <v>2157.62</v>
+        <v>1008.65</v>
       </c>
       <c r="O11" t="n">
-        <v>1.4</v>
+        <v>6.1</v>
       </c>
       <c r="P11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q11" t="b">
         <v>0</v>
@@ -1201,62 +1235,65 @@
         <v>0</v>
       </c>
       <c r="S11" t="b">
+        <v>0</v>
+      </c>
+      <c r="T11" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Mrs. Evelyn Foster</t>
+          <t>Rachel Brown</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Provide pattern later.</t>
+          <t>Month realize begin.</t>
         </is>
       </c>
       <c r="C12" s="2" t="n">
-        <v>45417</v>
+        <v>45229</v>
       </c>
       <c r="D12" t="b">
         <v>0</v>
       </c>
       <c r="E12" t="n">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Spotify</t>
+          <t>BookFunnel</t>
         </is>
       </c>
       <c r="G12" t="n">
-        <v>14.93</v>
+        <v>15.27</v>
       </c>
       <c r="H12" t="n">
-        <v>4243.818289821167</v>
+        <v>443.1865504897143</v>
       </c>
       <c r="I12" t="b">
         <v>0</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>Ava Winters</t>
+          <t>AI Narrator</t>
         </is>
       </c>
       <c r="K12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L12" t="n">
-        <v>486</v>
+        <v>552</v>
       </c>
       <c r="M12" t="n">
-        <v>0.367</v>
+        <v>1</v>
       </c>
       <c r="N12" t="n">
-        <v>2662.94</v>
+        <v>8429.040000000001</v>
       </c>
       <c r="O12" t="n">
-        <v>1.6</v>
+        <v>0.1</v>
       </c>
       <c r="P12" t="b">
         <v>1</v>
@@ -1268,28 +1305,31 @@
         <v>0</v>
       </c>
       <c r="S12" t="b">
+        <v>0</v>
+      </c>
+      <c r="T12" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Jessica Roberts</t>
+          <t>Kimberly Bailey</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>News almost.</t>
+          <t>Likely various religious.</t>
         </is>
       </c>
       <c r="C13" s="2" t="n">
-        <v>45643</v>
+        <v>45794</v>
       </c>
       <c r="D13" t="b">
         <v>0</v>
       </c>
       <c r="E13" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
@@ -1297,36 +1337,36 @@
         </is>
       </c>
       <c r="G13" t="n">
-        <v>17.42</v>
+        <v>9</v>
       </c>
       <c r="H13" t="n">
-        <v>344.55310581266</v>
+        <v>5704.111562454361</v>
       </c>
       <c r="I13" t="b">
         <v>0</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>AI Narrator</t>
+          <t>Jason Clarke</t>
         </is>
       </c>
       <c r="K13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L13" t="n">
-        <v>710</v>
+        <v>197</v>
       </c>
       <c r="M13" t="n">
-        <v>0.335</v>
+        <v>0.367</v>
       </c>
       <c r="N13" t="n">
-        <v>4143.35</v>
+        <v>650.6900000000001</v>
       </c>
       <c r="O13" t="n">
-        <v>0.1</v>
+        <v>8.800000000000001</v>
       </c>
       <c r="P13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q13" t="b">
         <v>0</v>
@@ -1335,62 +1375,65 @@
         <v>0</v>
       </c>
       <c r="S13" t="b">
+        <v>0</v>
+      </c>
+      <c r="T13" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Kristin Williams</t>
+          <t>Joseph Rodriguez</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Business range support dream.</t>
+          <t>Trip movement miss daughter.</t>
         </is>
       </c>
       <c r="C14" s="2" t="n">
-        <v>45464</v>
+        <v>45340</v>
       </c>
       <c r="D14" t="b">
         <v>0</v>
       </c>
       <c r="E14" t="n">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Spotify</t>
+          <t>ACX Exclusive</t>
         </is>
       </c>
       <c r="G14" t="n">
-        <v>16.06</v>
+        <v>19.35</v>
       </c>
       <c r="H14" t="n">
-        <v>2616.700112424114</v>
+        <v>7800.075621364695</v>
       </c>
       <c r="I14" t="b">
         <v>0</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>Taylor James</t>
+          <t>Jason Clarke</t>
         </is>
       </c>
       <c r="K14" t="b">
         <v>0</v>
       </c>
       <c r="L14" t="n">
-        <v>609</v>
+        <v>823</v>
       </c>
       <c r="M14" t="n">
-        <v>0.49</v>
+        <v>0.4</v>
       </c>
       <c r="N14" t="n">
-        <v>4792.46</v>
+        <v>6370.02</v>
       </c>
       <c r="O14" t="n">
-        <v>0.5</v>
+        <v>1.2</v>
       </c>
       <c r="P14" t="b">
         <v>1</v>
@@ -1402,65 +1445,70 @@
         <v>0</v>
       </c>
       <c r="S14" t="b">
+        <v>0</v>
+      </c>
+      <c r="T14" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Maria Bailey</t>
+          <t>Maria Berry</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>People water behavior indeed.</t>
+          <t>How father bad fight maintain.</t>
         </is>
       </c>
       <c r="C15" s="2" t="n">
-        <v>45337</v>
+        <v>45859</v>
       </c>
       <c r="D15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E15" t="n">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Findaway</t>
+          <t>Spotify</t>
         </is>
       </c>
       <c r="G15" t="n">
-        <v>10.83</v>
+        <v>10.01</v>
       </c>
       <c r="H15" t="n">
-        <v>7073.864567961144</v>
+        <v>0</v>
       </c>
       <c r="I15" t="b">
         <v>0</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>Ava Winters</t>
+          <t>AI Narrator</t>
         </is>
       </c>
       <c r="K15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L15" t="n">
-        <v>958</v>
+        <v>231</v>
       </c>
       <c r="M15" t="n">
-        <v>0.432</v>
+        <v>0.447</v>
       </c>
       <c r="N15" t="n">
-        <v>4482.06</v>
-      </c>
-      <c r="O15" t="n">
-        <v>1.6</v>
+        <v>1033.6</v>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>Never</t>
+        </is>
       </c>
       <c r="P15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q15" t="b">
         <v>0</v>
@@ -1469,28 +1517,31 @@
         <v>0</v>
       </c>
       <c r="S15" t="b">
+        <v>0</v>
+      </c>
+      <c r="T15" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Jacob Hill</t>
+          <t>Amber King</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Happen interview.</t>
+          <t>Enjoy strategy least.</t>
         </is>
       </c>
       <c r="C16" s="2" t="n">
-        <v>45361</v>
+        <v>45816</v>
       </c>
       <c r="D16" t="b">
         <v>0</v>
       </c>
       <c r="E16" t="n">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
@@ -1498,33 +1549,33 @@
         </is>
       </c>
       <c r="G16" t="n">
-        <v>14.89</v>
+        <v>13.87</v>
       </c>
       <c r="H16" t="n">
-        <v>3092.594750532939</v>
+        <v>434.4362099128309</v>
       </c>
       <c r="I16" t="b">
         <v>0</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>Taylor James</t>
+          <t>AI Narrator</t>
         </is>
       </c>
       <c r="K16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L16" t="n">
-        <v>272</v>
+        <v>301</v>
       </c>
       <c r="M16" t="n">
         <v>0.4</v>
       </c>
       <c r="N16" t="n">
-        <v>1620.03</v>
+        <v>1669.95</v>
       </c>
       <c r="O16" t="n">
-        <v>1.9</v>
+        <v>0.3</v>
       </c>
       <c r="P16" t="b">
         <v>1</v>
@@ -1536,65 +1587,68 @@
         <v>0</v>
       </c>
       <c r="S16" t="b">
+        <v>0</v>
+      </c>
+      <c r="T16" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Jackson Downs</t>
+          <t>Christine Hernandez</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Back man series perform dream.</t>
+          <t>Idea agency capital candidate kid.</t>
         </is>
       </c>
       <c r="C17" s="2" t="n">
-        <v>45467</v>
+        <v>45348</v>
       </c>
       <c r="D17" t="b">
         <v>0</v>
       </c>
       <c r="E17" t="n">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Findaway</t>
+          <t>ACX Royalty Share</t>
         </is>
       </c>
       <c r="G17" t="n">
-        <v>10.19</v>
+        <v>15.78</v>
       </c>
       <c r="H17" t="n">
-        <v>3076.261700102999</v>
+        <v>9732.347567428691</v>
       </c>
       <c r="I17" t="b">
         <v>0</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>Rachel Scott</t>
+          <t>Jason Clarke</t>
         </is>
       </c>
       <c r="K17" t="b">
         <v>0</v>
       </c>
       <c r="L17" t="n">
-        <v>357</v>
+        <v>78</v>
       </c>
       <c r="M17" t="n">
-        <v>0.332</v>
+        <v>0.221</v>
       </c>
       <c r="N17" t="n">
-        <v>1207.76</v>
+        <v>272.02</v>
       </c>
       <c r="O17" t="n">
-        <v>2.5</v>
+        <v>35.8</v>
       </c>
       <c r="P17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q17" t="b">
         <v>0</v>
@@ -1604,41 +1658,44 @@
       </c>
       <c r="S17" t="b">
         <v>0</v>
+      </c>
+      <c r="T17" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Justin Johnson</t>
+          <t>Regina Lee</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Develop sure when.</t>
+          <t>Upon drop forward.</t>
         </is>
       </c>
       <c r="C18" s="2" t="n">
-        <v>45445</v>
+        <v>45673</v>
       </c>
       <c r="D18" t="b">
         <v>0</v>
       </c>
       <c r="E18" t="n">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>ACX Royalty Share</t>
+          <t>ACX Exclusive</t>
         </is>
       </c>
       <c r="G18" t="n">
-        <v>15.94</v>
+        <v>10.45</v>
       </c>
       <c r="H18" t="n">
-        <v>2634.576151152556</v>
+        <v>3329.354960952243</v>
       </c>
       <c r="I18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -1649,16 +1706,16 @@
         <v>0</v>
       </c>
       <c r="L18" t="n">
-        <v>539</v>
+        <v>219</v>
       </c>
       <c r="M18" t="n">
-        <v>0.1</v>
+        <v>0.4</v>
       </c>
       <c r="N18" t="n">
-        <v>859.17</v>
+        <v>915.42</v>
       </c>
       <c r="O18" t="n">
-        <v>3.1</v>
+        <v>3.6</v>
       </c>
       <c r="P18" t="b">
         <v>1</v>
@@ -1670,62 +1727,65 @@
         <v>0</v>
       </c>
       <c r="S18" t="b">
+        <v>0</v>
+      </c>
+      <c r="T18" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Diana King</t>
+          <t>Carol Lewis</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Suggest get spring.</t>
+          <t>Could poor also school can.</t>
         </is>
       </c>
       <c r="C19" s="2" t="n">
-        <v>45256</v>
+        <v>45511</v>
       </c>
       <c r="D19" t="b">
         <v>0</v>
       </c>
       <c r="E19" t="n">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Findaway</t>
+          <t>Spotify</t>
         </is>
       </c>
       <c r="G19" t="n">
-        <v>9.720000000000001</v>
+        <v>19.26</v>
       </c>
       <c r="H19" t="n">
-        <v>405.4911525221137</v>
+        <v>5472.196858004498</v>
       </c>
       <c r="I19" t="b">
         <v>0</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>AI Narrator</t>
+          <t>Jason Clarke</t>
         </is>
       </c>
       <c r="K19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L19" t="n">
-        <v>979</v>
+        <v>943</v>
       </c>
       <c r="M19" t="n">
-        <v>0.426</v>
+        <v>0.361</v>
       </c>
       <c r="N19" t="n">
-        <v>4053.76</v>
+        <v>6556.55</v>
       </c>
       <c r="O19" t="n">
-        <v>0.1</v>
+        <v>0.8</v>
       </c>
       <c r="P19" t="b">
         <v>1</v>
@@ -1737,62 +1797,65 @@
         <v>0</v>
       </c>
       <c r="S19" t="b">
+        <v>0</v>
+      </c>
+      <c r="T19" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Tina Cox MD</t>
+          <t>James Lucas</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Them raise economy.</t>
+          <t>Particularly raise.</t>
         </is>
       </c>
       <c r="C20" s="2" t="n">
-        <v>45429</v>
+        <v>45682</v>
       </c>
       <c r="D20" t="b">
         <v>0</v>
       </c>
       <c r="E20" t="n">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Spotify</t>
+          <t>BookFunnel</t>
         </is>
       </c>
       <c r="G20" t="n">
-        <v>9.43</v>
+        <v>19.7</v>
       </c>
       <c r="H20" t="n">
-        <v>6584.880334570367</v>
+        <v>6351.566400707906</v>
       </c>
       <c r="I20" t="b">
         <v>0</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>Jason Clarke</t>
+          <t>Samantha Prescott</t>
         </is>
       </c>
       <c r="K20" t="b">
         <v>0</v>
       </c>
       <c r="L20" t="n">
-        <v>744</v>
+        <v>981</v>
       </c>
       <c r="M20" t="n">
-        <v>0.441</v>
+        <v>1</v>
       </c>
       <c r="N20" t="n">
-        <v>3094.02</v>
+        <v>19325.7</v>
       </c>
       <c r="O20" t="n">
-        <v>2.1</v>
+        <v>0.3</v>
       </c>
       <c r="P20" t="b">
         <v>1</v>
@@ -1804,28 +1867,31 @@
         <v>0</v>
       </c>
       <c r="S20" t="b">
+        <v>0</v>
+      </c>
+      <c r="T20" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Jason Mora</t>
+          <t>Charles Lin DVM</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Through shake movie sense.</t>
+          <t>Shoulder box action family never.</t>
         </is>
       </c>
       <c r="C21" s="2" t="n">
-        <v>45533</v>
+        <v>45169</v>
       </c>
       <c r="D21" t="b">
         <v>0</v>
       </c>
       <c r="E21" t="n">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
@@ -1833,33 +1899,33 @@
         </is>
       </c>
       <c r="G21" t="n">
-        <v>9.880000000000001</v>
+        <v>17.38</v>
       </c>
       <c r="H21" t="n">
-        <v>4376.229864806502</v>
+        <v>7145.364156454812</v>
       </c>
       <c r="I21" t="b">
         <v>0</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>Samantha Prescott</t>
+          <t>Ava Winters</t>
         </is>
       </c>
       <c r="K21" t="b">
         <v>0</v>
       </c>
       <c r="L21" t="n">
-        <v>292</v>
+        <v>529</v>
       </c>
       <c r="M21" t="n">
         <v>0.4</v>
       </c>
       <c r="N21" t="n">
-        <v>1153.98</v>
+        <v>3677.61</v>
       </c>
       <c r="O21" t="n">
-        <v>3.8</v>
+        <v>1.9</v>
       </c>
       <c r="P21" t="b">
         <v>1</v>
@@ -1871,62 +1937,65 @@
         <v>0</v>
       </c>
       <c r="S21" t="b">
+        <v>0</v>
+      </c>
+      <c r="T21" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Charles Thompson</t>
+          <t>Jason Keller</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Old and beyond down.</t>
+          <t>Player man.</t>
         </is>
       </c>
       <c r="C22" s="2" t="n">
-        <v>45381</v>
+        <v>45151</v>
       </c>
       <c r="D22" t="b">
         <v>0</v>
       </c>
       <c r="E22" t="n">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Spotify</t>
+          <t>Findaway</t>
         </is>
       </c>
       <c r="G22" t="n">
-        <v>8.869999999999999</v>
+        <v>11.02</v>
       </c>
       <c r="H22" t="n">
-        <v>4828.122299117817</v>
+        <v>2133.771964044494</v>
       </c>
       <c r="I22" t="b">
         <v>0</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>Samantha Prescott</t>
+          <t>Rachel Scott</t>
         </is>
       </c>
       <c r="K22" t="b">
         <v>0</v>
       </c>
       <c r="L22" t="n">
-        <v>655</v>
+        <v>514</v>
       </c>
       <c r="M22" t="n">
-        <v>0.405</v>
+        <v>0.318</v>
       </c>
       <c r="N22" t="n">
-        <v>2352.99</v>
+        <v>1801.24</v>
       </c>
       <c r="O22" t="n">
-        <v>2.1</v>
+        <v>1.2</v>
       </c>
       <c r="P22" t="b">
         <v>1</v>
@@ -1938,62 +2007,65 @@
         <v>0</v>
       </c>
       <c r="S22" t="b">
+        <v>0</v>
+      </c>
+      <c r="T22" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Billy Bernard</t>
+          <t>Jessica Mcbride</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Space high someone dream.</t>
+          <t>Bag point physical receive price.</t>
         </is>
       </c>
       <c r="C23" s="2" t="n">
-        <v>45317</v>
+        <v>45294</v>
       </c>
       <c r="D23" t="b">
         <v>0</v>
       </c>
       <c r="E23" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>ACX Exclusive</t>
+          <t>ACX Royalty Share</t>
         </is>
       </c>
       <c r="G23" t="n">
-        <v>8.81</v>
+        <v>18.86</v>
       </c>
       <c r="H23" t="n">
-        <v>6001.17296238856</v>
+        <v>8084.186305809782</v>
       </c>
       <c r="I23" t="b">
         <v>0</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>Ava Winters</t>
+          <t>Jason Clarke</t>
         </is>
       </c>
       <c r="K23" t="b">
         <v>0</v>
       </c>
       <c r="L23" t="n">
-        <v>609</v>
+        <v>284</v>
       </c>
       <c r="M23" t="n">
-        <v>0.4</v>
+        <v>0.191</v>
       </c>
       <c r="N23" t="n">
-        <v>2146.12</v>
+        <v>1023.04</v>
       </c>
       <c r="O23" t="n">
-        <v>2.8</v>
+        <v>7.9</v>
       </c>
       <c r="P23" t="b">
         <v>1</v>
@@ -2006,64 +2078,69 @@
       </c>
       <c r="S23" t="b">
         <v>0</v>
+      </c>
+      <c r="T23" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Matthew Perkins</t>
+          <t>Scott Welch</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Maintain this animal.</t>
+          <t>Produce law actually risk.</t>
         </is>
       </c>
       <c r="C24" s="2" t="n">
-        <v>45368</v>
+        <v>45731</v>
       </c>
       <c r="D24" t="b">
         <v>0</v>
       </c>
       <c r="E24" t="n">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>BookFunnel</t>
+          <t>ACX Exclusive</t>
         </is>
       </c>
       <c r="G24" t="n">
-        <v>17.8</v>
+        <v>12.88</v>
       </c>
       <c r="H24" t="n">
-        <v>2463.859690331371</v>
+        <v>0</v>
       </c>
       <c r="I24" t="b">
         <v>0</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>Taylor James</t>
+          <t>AI Narrator</t>
         </is>
       </c>
       <c r="K24" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L24" t="n">
-        <v>623</v>
+        <v>198</v>
       </c>
       <c r="M24" t="n">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="N24" t="n">
-        <v>11089.4</v>
-      </c>
-      <c r="O24" t="n">
-        <v>0.2</v>
+        <v>1020.1</v>
+      </c>
+      <c r="O24" t="inlineStr">
+        <is>
+          <t>Never</t>
+        </is>
       </c>
       <c r="P24" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q24" t="b">
         <v>0</v>
@@ -2072,65 +2149,68 @@
         <v>0</v>
       </c>
       <c r="S24" t="b">
+        <v>0</v>
+      </c>
+      <c r="T24" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Shelby Smith</t>
+          <t>Courtney Warner</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Side prevent talk.</t>
+          <t>Mr effort they that.</t>
         </is>
       </c>
       <c r="C25" s="2" t="n">
-        <v>45861</v>
+        <v>45709</v>
       </c>
       <c r="D25" t="b">
         <v>0</v>
       </c>
       <c r="E25" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Findaway</t>
+          <t>Spotify</t>
         </is>
       </c>
       <c r="G25" t="n">
-        <v>16.02</v>
+        <v>10.79</v>
       </c>
       <c r="H25" t="n">
-        <v>4851.715801831664</v>
+        <v>161.0921807851304</v>
       </c>
       <c r="I25" t="b">
         <v>0</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>Jason Clarke</t>
+          <t>AI Narrator</t>
         </is>
       </c>
       <c r="K25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L25" t="n">
-        <v>248</v>
+        <v>701</v>
       </c>
       <c r="M25" t="n">
-        <v>0.42</v>
+        <v>0.363</v>
       </c>
       <c r="N25" t="n">
-        <v>1668.64</v>
+        <v>2745.66</v>
       </c>
       <c r="O25" t="n">
-        <v>2.9</v>
+        <v>0.1</v>
       </c>
       <c r="P25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q25" t="b">
         <v>0</v>
@@ -2139,62 +2219,65 @@
         <v>0</v>
       </c>
       <c r="S25" t="b">
+        <v>0</v>
+      </c>
+      <c r="T25" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Mrs. Kirsten Nichols</t>
+          <t>Albert Jordan</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Determine ok guy.</t>
+          <t>Space true couple nothing.</t>
         </is>
       </c>
       <c r="C26" s="2" t="n">
-        <v>45362</v>
+        <v>45775</v>
       </c>
       <c r="D26" t="b">
         <v>0</v>
       </c>
       <c r="E26" t="n">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Findaway</t>
+          <t>Spotify</t>
         </is>
       </c>
       <c r="G26" t="n">
-        <v>13.76</v>
+        <v>10.09</v>
       </c>
       <c r="H26" t="n">
-        <v>6494.54544827551</v>
+        <v>280.6909876651985</v>
       </c>
       <c r="I26" t="b">
         <v>0</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>Ava Winters</t>
+          <t>AI Narrator</t>
         </is>
       </c>
       <c r="K26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L26" t="n">
-        <v>299</v>
+        <v>254</v>
       </c>
       <c r="M26" t="n">
-        <v>0.408</v>
+        <v>0.362</v>
       </c>
       <c r="N26" t="n">
-        <v>1678.61</v>
+        <v>927.76</v>
       </c>
       <c r="O26" t="n">
-        <v>3.9</v>
+        <v>0.3</v>
       </c>
       <c r="P26" t="b">
         <v>1</v>
@@ -2206,28 +2289,31 @@
         <v>0</v>
       </c>
       <c r="S26" t="b">
+        <v>0</v>
+      </c>
+      <c r="T26" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Diana Castillo</t>
+          <t>Karen Marshall</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Write hundred approach.</t>
+          <t>Toward down among process when.</t>
         </is>
       </c>
       <c r="C27" s="2" t="n">
-        <v>45305</v>
+        <v>45855</v>
       </c>
       <c r="D27" t="b">
         <v>0</v>
       </c>
       <c r="E27" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="F27" t="inlineStr">
         <is>
@@ -2235,36 +2321,36 @@
         </is>
       </c>
       <c r="G27" t="n">
-        <v>16.9</v>
+        <v>18.54</v>
       </c>
       <c r="H27" t="n">
-        <v>6277.883018632792</v>
+        <v>7917.203898939063</v>
       </c>
       <c r="I27" t="b">
         <v>0</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>Ava Winters</t>
+          <t>Samantha Prescott</t>
         </is>
       </c>
       <c r="K27" t="b">
         <v>0</v>
       </c>
       <c r="L27" t="n">
-        <v>811</v>
+        <v>48</v>
       </c>
       <c r="M27" t="n">
-        <v>0.4</v>
+        <v>0.228</v>
       </c>
       <c r="N27" t="n">
-        <v>5482.36</v>
+        <v>202.9</v>
       </c>
       <c r="O27" t="n">
-        <v>1.1</v>
+        <v>39</v>
       </c>
       <c r="P27" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q27" t="b">
         <v>0</v>
@@ -2274,27 +2360,30 @@
       </c>
       <c r="S27" t="b">
         <v>0</v>
+      </c>
+      <c r="T27" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Bryan Quinn</t>
+          <t>Roger Stevens</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Pattern if true food own.</t>
+          <t>That responsibility pick keep.</t>
         </is>
       </c>
       <c r="C28" s="2" t="n">
-        <v>45455</v>
+        <v>45728</v>
       </c>
       <c r="D28" t="b">
         <v>0</v>
       </c>
       <c r="E28" t="n">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="F28" t="inlineStr">
         <is>
@@ -2302,33 +2391,33 @@
         </is>
       </c>
       <c r="G28" t="n">
-        <v>19.77</v>
+        <v>8.550000000000001</v>
       </c>
       <c r="H28" t="n">
-        <v>3620.095240934913</v>
+        <v>4935.122344311648</v>
       </c>
       <c r="I28" t="b">
         <v>0</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>Rachel Scott</t>
+          <t>Jason Clarke</t>
         </is>
       </c>
       <c r="K28" t="b">
         <v>0</v>
       </c>
       <c r="L28" t="n">
-        <v>299</v>
+        <v>491</v>
       </c>
       <c r="M28" t="n">
         <v>0.4</v>
       </c>
       <c r="N28" t="n">
-        <v>2364.49</v>
+        <v>1679.22</v>
       </c>
       <c r="O28" t="n">
-        <v>1.5</v>
+        <v>2.9</v>
       </c>
       <c r="P28" t="b">
         <v>1</v>
@@ -2340,62 +2429,65 @@
         <v>0</v>
       </c>
       <c r="S28" t="b">
+        <v>0</v>
+      </c>
+      <c r="T28" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Jodi Kelley</t>
+          <t>Toni Malone</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Account use.</t>
+          <t>World debate.</t>
         </is>
       </c>
       <c r="C29" s="2" t="n">
-        <v>45637</v>
+        <v>45669</v>
       </c>
       <c r="D29" t="b">
         <v>0</v>
       </c>
       <c r="E29" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>BookFunnel</t>
+          <t>ACX Exclusive</t>
         </is>
       </c>
       <c r="G29" t="n">
-        <v>10.3</v>
+        <v>10.18</v>
       </c>
       <c r="H29" t="n">
-        <v>2657.871140360051</v>
+        <v>177.8722044981239</v>
       </c>
       <c r="I29" t="b">
         <v>0</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>Taylor James</t>
+          <t>AI Narrator</t>
         </is>
       </c>
       <c r="K29" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L29" t="n">
-        <v>989</v>
+        <v>317</v>
       </c>
       <c r="M29" t="n">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="N29" t="n">
-        <v>10186.7</v>
+        <v>1290.82</v>
       </c>
       <c r="O29" t="n">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="P29" t="b">
         <v>1</v>
@@ -2407,62 +2499,65 @@
         <v>0</v>
       </c>
       <c r="S29" t="b">
+        <v>0</v>
+      </c>
+      <c r="T29" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Jasmine Lopez</t>
+          <t>Brad Harris</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Nothing feel thank building.</t>
+          <t>Must main it candidate.</t>
         </is>
       </c>
       <c r="C30" s="2" t="n">
-        <v>45167</v>
+        <v>45289</v>
       </c>
       <c r="D30" t="b">
         <v>0</v>
       </c>
       <c r="E30" t="n">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>ACX Exclusive</t>
+          <t>ACX Royalty Share</t>
         </is>
       </c>
       <c r="G30" t="n">
-        <v>8.02</v>
+        <v>16.58</v>
       </c>
       <c r="H30" t="n">
-        <v>3949.528805500076</v>
+        <v>230.2967331481006</v>
       </c>
       <c r="I30" t="b">
         <v>0</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>Taylor James</t>
+          <t>AI Narrator</t>
         </is>
       </c>
       <c r="K30" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L30" t="n">
-        <v>359</v>
+        <v>245</v>
       </c>
       <c r="M30" t="n">
-        <v>0.4</v>
+        <v>0.245</v>
       </c>
       <c r="N30" t="n">
-        <v>1151.67</v>
+        <v>995.21</v>
       </c>
       <c r="O30" t="n">
-        <v>3.4</v>
+        <v>0.2</v>
       </c>
       <c r="P30" t="b">
         <v>1</v>
@@ -2474,95 +2569,101 @@
         <v>0</v>
       </c>
       <c r="S30" t="b">
+        <v>0</v>
+      </c>
+      <c r="T30" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Nicole Hardy DVM</t>
+          <t>Samantha Schaefer</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Majority letter show where book.</t>
+          <t>Five low his reflect.</t>
         </is>
       </c>
       <c r="C31" s="2" t="n">
-        <v>45441</v>
+        <v>45341</v>
       </c>
       <c r="D31" t="b">
         <v>0</v>
       </c>
       <c r="E31" t="n">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>Spotify</t>
+          <t>ACX Royalty Share</t>
         </is>
       </c>
       <c r="G31" t="n">
-        <v>19.88</v>
+        <v>13.42</v>
       </c>
       <c r="H31" t="n">
-        <v>7271.037458549548</v>
+        <v>4029.323494215169</v>
       </c>
       <c r="I31" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>Samantha Prescott</t>
+          <t>Rachel Scott</t>
         </is>
       </c>
       <c r="K31" t="b">
         <v>0</v>
       </c>
       <c r="L31" t="n">
-        <v>764</v>
+        <v>95</v>
       </c>
       <c r="M31" t="n">
-        <v>0.399</v>
+        <v>0.063</v>
       </c>
       <c r="N31" t="n">
-        <v>6060.14</v>
+        <v>80.31999999999999</v>
       </c>
       <c r="O31" t="n">
-        <v>1.2</v>
+        <v>50.2</v>
       </c>
       <c r="P31" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q31" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R31" t="b">
         <v>0</v>
       </c>
       <c r="S31" t="b">
         <v>0</v>
+      </c>
+      <c r="T31" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Gerald Nelson</t>
+          <t>Samantha Mcdonald</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Program eat media.</t>
+          <t>Establish face.</t>
         </is>
       </c>
       <c r="C32" s="2" t="n">
-        <v>45293</v>
+        <v>45512</v>
       </c>
       <c r="D32" t="b">
         <v>0</v>
       </c>
       <c r="E32" t="n">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="F32" t="inlineStr">
         <is>
@@ -2570,33 +2671,33 @@
         </is>
       </c>
       <c r="G32" t="n">
-        <v>19.85</v>
+        <v>13.73</v>
       </c>
       <c r="H32" t="n">
-        <v>3752.336607164008</v>
+        <v>3094.046588307478</v>
       </c>
       <c r="I32" t="b">
         <v>0</v>
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>Rachel Scott</t>
+          <t>Taylor James</t>
         </is>
       </c>
       <c r="K32" t="b">
         <v>0</v>
       </c>
       <c r="L32" t="n">
-        <v>275</v>
+        <v>567</v>
       </c>
       <c r="M32" t="n">
         <v>0.4</v>
       </c>
       <c r="N32" t="n">
-        <v>2183.5</v>
+        <v>3113.96</v>
       </c>
       <c r="O32" t="n">
-        <v>1.7</v>
+        <v>1</v>
       </c>
       <c r="P32" t="b">
         <v>1</v>
@@ -2608,28 +2709,31 @@
         <v>0</v>
       </c>
       <c r="S32" t="b">
+        <v>0</v>
+      </c>
+      <c r="T32" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Dr. Daisy Franklin</t>
+          <t>Christopher Bowen</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Start value down every night.</t>
+          <t>Rest write probably.</t>
         </is>
       </c>
       <c r="C33" s="2" t="n">
-        <v>45849</v>
+        <v>45472</v>
       </c>
       <c r="D33" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E33" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="F33" t="inlineStr">
         <is>
@@ -2637,33 +2741,33 @@
         </is>
       </c>
       <c r="G33" t="n">
-        <v>14.73</v>
+        <v>16.81</v>
       </c>
       <c r="H33" t="n">
-        <v>3131.246597003927</v>
+        <v>9262.428372689799</v>
       </c>
       <c r="I33" t="b">
         <v>1</v>
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>Taylor James</t>
+          <t>Samantha Prescott</t>
         </is>
       </c>
       <c r="K33" t="b">
         <v>0</v>
       </c>
       <c r="L33" t="n">
-        <v>193</v>
+        <v>211</v>
       </c>
       <c r="M33" t="n">
-        <v>0.1</v>
+        <v>0.0655</v>
       </c>
       <c r="N33" t="n">
-        <v>284.29</v>
+        <v>232.32</v>
       </c>
       <c r="O33" t="n">
-        <v>11</v>
+        <v>39.9</v>
       </c>
       <c r="P33" t="b">
         <v>0</v>
@@ -2672,42 +2776,45 @@
         <v>0</v>
       </c>
       <c r="R33" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S33" t="b">
         <v>0</v>
+      </c>
+      <c r="T33" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Joseph Savage</t>
+          <t>Steven Williams</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Spend determine near want high.</t>
+          <t>Kitchen her Republican simple.</t>
         </is>
       </c>
       <c r="C34" s="2" t="n">
-        <v>45143</v>
+        <v>45805</v>
       </c>
       <c r="D34" t="b">
         <v>0</v>
       </c>
       <c r="E34" t="n">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>ACX Exclusive</t>
+          <t>Findaway</t>
         </is>
       </c>
       <c r="G34" t="n">
-        <v>8.58</v>
+        <v>14.57</v>
       </c>
       <c r="H34" t="n">
-        <v>6086.161916518998</v>
+        <v>4066.88634362504</v>
       </c>
       <c r="I34" t="b">
         <v>0</v>
@@ -2721,19 +2828,19 @@
         <v>0</v>
       </c>
       <c r="L34" t="n">
-        <v>473</v>
+        <v>323</v>
       </c>
       <c r="M34" t="n">
-        <v>0.4</v>
+        <v>0.342</v>
       </c>
       <c r="N34" t="n">
-        <v>1623.34</v>
+        <v>1609.49</v>
       </c>
       <c r="O34" t="n">
-        <v>3.7</v>
+        <v>2.5</v>
       </c>
       <c r="P34" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q34" t="b">
         <v>0</v>
@@ -2742,39 +2849,42 @@
         <v>0</v>
       </c>
       <c r="S34" t="b">
+        <v>0</v>
+      </c>
+      <c r="T34" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>John Romero</t>
+          <t>Kimberly Cruz</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Team anyone name.</t>
+          <t>Get affect high fight when.</t>
         </is>
       </c>
       <c r="C35" s="2" t="n">
-        <v>45544</v>
+        <v>45280</v>
       </c>
       <c r="D35" t="b">
         <v>0</v>
       </c>
       <c r="E35" t="n">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>BookFunnel</t>
+          <t>ACX Royalty Share</t>
         </is>
       </c>
       <c r="G35" t="n">
-        <v>16.34</v>
+        <v>18.96</v>
       </c>
       <c r="H35" t="n">
-        <v>4184.708874649185</v>
+        <v>10385.97987287411</v>
       </c>
       <c r="I35" t="b">
         <v>0</v>
@@ -2788,16 +2898,16 @@
         <v>0</v>
       </c>
       <c r="L35" t="n">
-        <v>909</v>
+        <v>159</v>
       </c>
       <c r="M35" t="n">
-        <v>1</v>
+        <v>0.211</v>
       </c>
       <c r="N35" t="n">
-        <v>14853.06</v>
+        <v>636.09</v>
       </c>
       <c r="O35" t="n">
-        <v>0.3</v>
+        <v>16.3</v>
       </c>
       <c r="P35" t="b">
         <v>1</v>
@@ -2810,61 +2920,64 @@
       </c>
       <c r="S35" t="b">
         <v>0</v>
+      </c>
+      <c r="T35" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Mark Gray</t>
+          <t>Gregory Gomez</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Bring expert dinner during.</t>
+          <t>Behavior ball else.</t>
         </is>
       </c>
       <c r="C36" s="2" t="n">
-        <v>45430</v>
+        <v>45229</v>
       </c>
       <c r="D36" t="b">
         <v>0</v>
       </c>
       <c r="E36" t="n">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>BookFunnel</t>
+          <t>Spotify</t>
         </is>
       </c>
       <c r="G36" t="n">
-        <v>15.23</v>
+        <v>10.79</v>
       </c>
       <c r="H36" t="n">
-        <v>2248.29855226716</v>
+        <v>5286.160244129313</v>
       </c>
       <c r="I36" t="b">
         <v>0</v>
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>Rachel Scott</t>
+          <t>Jason Clarke</t>
         </is>
       </c>
       <c r="K36" t="b">
         <v>0</v>
       </c>
       <c r="L36" t="n">
-        <v>246</v>
+        <v>363</v>
       </c>
       <c r="M36" t="n">
-        <v>1</v>
+        <v>0.306</v>
       </c>
       <c r="N36" t="n">
-        <v>3746.58</v>
+        <v>1198.53</v>
       </c>
       <c r="O36" t="n">
-        <v>0.6</v>
+        <v>4.4</v>
       </c>
       <c r="P36" t="b">
         <v>1</v>
@@ -2876,28 +2989,31 @@
         <v>0</v>
       </c>
       <c r="S36" t="b">
+        <v>0</v>
+      </c>
+      <c r="T36" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Kelly Smith</t>
+          <t>Mary Waller</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Moment identify.</t>
+          <t>Create loss sure record continue.</t>
         </is>
       </c>
       <c r="C37" s="2" t="n">
-        <v>45275</v>
+        <v>45653</v>
       </c>
       <c r="D37" t="b">
         <v>0</v>
       </c>
       <c r="E37" t="n">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="F37" t="inlineStr">
         <is>
@@ -2905,33 +3021,33 @@
         </is>
       </c>
       <c r="G37" t="n">
-        <v>19.79</v>
+        <v>10.85</v>
       </c>
       <c r="H37" t="n">
-        <v>5062.885089052737</v>
+        <v>3302.527276903202</v>
       </c>
       <c r="I37" t="b">
         <v>0</v>
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>Ava Winters</t>
+          <t>Rachel Scott</t>
         </is>
       </c>
       <c r="K37" t="b">
         <v>0</v>
       </c>
       <c r="L37" t="n">
-        <v>573</v>
+        <v>711</v>
       </c>
       <c r="M37" t="n">
-        <v>0.382</v>
+        <v>0.419</v>
       </c>
       <c r="N37" t="n">
-        <v>4331.75</v>
+        <v>3232.31</v>
       </c>
       <c r="O37" t="n">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="P37" t="b">
         <v>1</v>
@@ -2943,129 +3059,135 @@
         <v>0</v>
       </c>
       <c r="S37" t="b">
+        <v>0</v>
+      </c>
+      <c r="T37" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Crystal Khan</t>
+          <t>Mark Stevens</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Though design gas side.</t>
+          <t>Cause eat.</t>
         </is>
       </c>
       <c r="C38" s="2" t="n">
-        <v>45472</v>
+        <v>45496</v>
       </c>
       <c r="D38" t="b">
         <v>0</v>
       </c>
       <c r="E38" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>Spotify</t>
+          <t>ACX Royalty Share</t>
         </is>
       </c>
       <c r="G38" t="n">
-        <v>8.5</v>
+        <v>17.7</v>
       </c>
       <c r="H38" t="n">
-        <v>3859.138353235028</v>
+        <v>7973.674143276128</v>
       </c>
       <c r="I38" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>Taylor James</t>
+          <t>Jason Clarke</t>
         </is>
       </c>
       <c r="K38" t="b">
         <v>0</v>
       </c>
       <c r="L38" t="n">
-        <v>739</v>
+        <v>276</v>
       </c>
       <c r="M38" t="n">
-        <v>0.49</v>
+        <v>0.078</v>
       </c>
       <c r="N38" t="n">
-        <v>3077.93</v>
+        <v>381.05</v>
       </c>
       <c r="O38" t="n">
-        <v>1.3</v>
+        <v>20.9</v>
       </c>
       <c r="P38" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q38" t="b">
         <v>0</v>
       </c>
       <c r="R38" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S38" t="b">
         <v>0</v>
+      </c>
+      <c r="T38" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Ms. Rose Harmon MD</t>
+          <t>Gloria Juarez</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Memory third watch.</t>
+          <t>There white.</t>
         </is>
       </c>
       <c r="C39" s="2" t="n">
-        <v>45187</v>
+        <v>45304</v>
       </c>
       <c r="D39" t="b">
         <v>0</v>
       </c>
       <c r="E39" t="n">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>Findaway</t>
+          <t>ACX Royalty Share</t>
         </is>
       </c>
       <c r="G39" t="n">
-        <v>17.59</v>
+        <v>12.89</v>
       </c>
       <c r="H39" t="n">
-        <v>6979.35525063278</v>
+        <v>4027.99906805048</v>
       </c>
       <c r="I39" t="b">
         <v>0</v>
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>Samantha Prescott</t>
+          <t>Taylor James</t>
         </is>
       </c>
       <c r="K39" t="b">
         <v>0</v>
       </c>
       <c r="L39" t="n">
-        <v>765</v>
+        <v>86</v>
       </c>
       <c r="M39" t="n">
-        <v>0.328</v>
+        <v>0.227</v>
       </c>
       <c r="N39" t="n">
-        <v>4413.68</v>
+        <v>251.64</v>
       </c>
       <c r="O39" t="n">
-        <v>1.6</v>
+        <v>16</v>
       </c>
       <c r="P39" t="b">
         <v>1</v>
@@ -3077,62 +3199,65 @@
         <v>0</v>
       </c>
       <c r="S39" t="b">
+        <v>0</v>
+      </c>
+      <c r="T39" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>William Fuller</t>
+          <t>Johnny Martinez</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Civil marriage big play.</t>
+          <t>Stage common at subject.</t>
         </is>
       </c>
       <c r="C40" s="2" t="n">
-        <v>45392</v>
+        <v>45512</v>
       </c>
       <c r="D40" t="b">
         <v>0</v>
       </c>
       <c r="E40" t="n">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>Spotify</t>
+          <t>Findaway</t>
         </is>
       </c>
       <c r="G40" t="n">
-        <v>12.63</v>
+        <v>11.54</v>
       </c>
       <c r="H40" t="n">
-        <v>4842.130489993237</v>
+        <v>5498.529841641285</v>
       </c>
       <c r="I40" t="b">
         <v>0</v>
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>Jason Clarke</t>
+          <t>Ava Winters</t>
         </is>
       </c>
       <c r="K40" t="b">
         <v>0</v>
       </c>
       <c r="L40" t="n">
-        <v>329</v>
+        <v>861</v>
       </c>
       <c r="M40" t="n">
-        <v>0.357</v>
+        <v>0.319</v>
       </c>
       <c r="N40" t="n">
-        <v>1483.43</v>
+        <v>3169.56</v>
       </c>
       <c r="O40" t="n">
-        <v>3.3</v>
+        <v>1.7</v>
       </c>
       <c r="P40" t="b">
         <v>1</v>
@@ -3144,62 +3269,65 @@
         <v>0</v>
       </c>
       <c r="S40" t="b">
+        <v>0</v>
+      </c>
+      <c r="T40" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Alexis Chapman DDS</t>
+          <t>Andrew Dunlap</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>The stuff respond still choice.</t>
+          <t>Down ago significant.</t>
         </is>
       </c>
       <c r="C41" s="2" t="n">
-        <v>45599</v>
+        <v>45410</v>
       </c>
       <c r="D41" t="b">
         <v>0</v>
       </c>
       <c r="E41" t="n">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>ACX Exclusive</t>
+          <t>Findaway</t>
         </is>
       </c>
       <c r="G41" t="n">
-        <v>10.86</v>
+        <v>8.109999999999999</v>
       </c>
       <c r="H41" t="n">
-        <v>3292.584483705556</v>
+        <v>4261.109492778802</v>
       </c>
       <c r="I41" t="b">
         <v>0</v>
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>Rachel Scott</t>
+          <t>Jason Clarke</t>
         </is>
       </c>
       <c r="K41" t="b">
         <v>0</v>
       </c>
       <c r="L41" t="n">
-        <v>511</v>
+        <v>865</v>
       </c>
       <c r="M41" t="n">
-        <v>0.4</v>
+        <v>0.371</v>
       </c>
       <c r="N41" t="n">
-        <v>2219.78</v>
+        <v>2602.62</v>
       </c>
       <c r="O41" t="n">
-        <v>1.5</v>
+        <v>1.6</v>
       </c>
       <c r="P41" t="b">
         <v>1</v>
@@ -3211,65 +3339,68 @@
         <v>0</v>
       </c>
       <c r="S41" t="b">
+        <v>0</v>
+      </c>
+      <c r="T41" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Amanda Thomas</t>
+          <t>Dennis Parker</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Perform after seem image.</t>
+          <t>Live adult image.</t>
         </is>
       </c>
       <c r="C42" s="2" t="n">
-        <v>45619</v>
+        <v>45812</v>
       </c>
       <c r="D42" t="b">
         <v>0</v>
       </c>
       <c r="E42" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>ACX Exclusive</t>
+          <t>ACX Royalty Share</t>
         </is>
       </c>
       <c r="G42" t="n">
-        <v>13.47</v>
+        <v>19.48</v>
       </c>
       <c r="H42" t="n">
-        <v>7757.751366704997</v>
+        <v>3236.402075185601</v>
       </c>
       <c r="I42" t="b">
         <v>0</v>
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>Samantha Prescott</t>
+          <t>Rachel Scott</t>
         </is>
       </c>
       <c r="K42" t="b">
         <v>0</v>
       </c>
       <c r="L42" t="n">
-        <v>989</v>
+        <v>77</v>
       </c>
       <c r="M42" t="n">
-        <v>0.4</v>
+        <v>0.225</v>
       </c>
       <c r="N42" t="n">
-        <v>5328.73</v>
+        <v>337.49</v>
       </c>
       <c r="O42" t="n">
-        <v>1.5</v>
+        <v>9.6</v>
       </c>
       <c r="P42" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q42" t="b">
         <v>0</v>
@@ -3279,61 +3410,64 @@
       </c>
       <c r="S42" t="b">
         <v>0</v>
+      </c>
+      <c r="T42" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Brian Butler</t>
+          <t>Kayla Moreno</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Animal upon fly general.</t>
+          <t>Receive difficult travel report.</t>
         </is>
       </c>
       <c r="C43" s="2" t="n">
-        <v>45306</v>
+        <v>45293</v>
       </c>
       <c r="D43" t="b">
         <v>0</v>
       </c>
       <c r="E43" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>Findaway</t>
+          <t>Spotify</t>
         </is>
       </c>
       <c r="G43" t="n">
-        <v>19.23</v>
+        <v>19.71</v>
       </c>
       <c r="H43" t="n">
-        <v>7367.958593861322</v>
+        <v>3265.211656626933</v>
       </c>
       <c r="I43" t="b">
         <v>0</v>
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>Jason Clarke</t>
+          <t>Taylor James</t>
         </is>
       </c>
       <c r="K43" t="b">
         <v>0</v>
       </c>
       <c r="L43" t="n">
-        <v>354</v>
+        <v>201</v>
       </c>
       <c r="M43" t="n">
-        <v>0.394</v>
+        <v>0.355</v>
       </c>
       <c r="N43" t="n">
-        <v>2682.12</v>
+        <v>1406.41</v>
       </c>
       <c r="O43" t="n">
-        <v>2.7</v>
+        <v>2.3</v>
       </c>
       <c r="P43" t="b">
         <v>1</v>
@@ -3345,62 +3479,65 @@
         <v>0</v>
       </c>
       <c r="S43" t="b">
+        <v>0</v>
+      </c>
+      <c r="T43" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Bonnie Garcia</t>
+          <t>Cody Maldonado</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Purpose subject wife eat.</t>
+          <t>Dream gun.</t>
         </is>
       </c>
       <c r="C44" s="2" t="n">
-        <v>45222</v>
+        <v>45718</v>
       </c>
       <c r="D44" t="b">
         <v>0</v>
       </c>
       <c r="E44" t="n">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>BookFunnel</t>
+          <t>Spotify</t>
         </is>
       </c>
       <c r="G44" t="n">
-        <v>10.44</v>
+        <v>8.720000000000001</v>
       </c>
       <c r="H44" t="n">
-        <v>2093.742299154831</v>
+        <v>4135.171719864784</v>
       </c>
       <c r="I44" t="b">
         <v>0</v>
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>Rachel Scott</t>
+          <t>Samantha Prescott</t>
         </is>
       </c>
       <c r="K44" t="b">
         <v>0</v>
       </c>
       <c r="L44" t="n">
-        <v>666</v>
+        <v>387</v>
       </c>
       <c r="M44" t="n">
-        <v>1</v>
+        <v>0.437</v>
       </c>
       <c r="N44" t="n">
-        <v>6953.04</v>
+        <v>1474.72</v>
       </c>
       <c r="O44" t="n">
-        <v>0.3</v>
+        <v>2.8</v>
       </c>
       <c r="P44" t="b">
         <v>1</v>
@@ -3412,62 +3549,65 @@
         <v>0</v>
       </c>
       <c r="S44" t="b">
+        <v>0</v>
+      </c>
+      <c r="T44" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Craig Bush</t>
+          <t>William Trujillo</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Pass traditional effect imagine here.</t>
+          <t>Sort keep provide every sit.</t>
         </is>
       </c>
       <c r="C45" s="2" t="n">
-        <v>45410</v>
+        <v>45186</v>
       </c>
       <c r="D45" t="b">
         <v>0</v>
       </c>
       <c r="E45" t="n">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>Spotify</t>
+          <t>Findaway</t>
         </is>
       </c>
       <c r="G45" t="n">
-        <v>14.99</v>
+        <v>8.48</v>
       </c>
       <c r="H45" t="n">
-        <v>2750.155268467994</v>
+        <v>3778.334159415333</v>
       </c>
       <c r="I45" t="b">
         <v>0</v>
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>Taylor James</t>
+          <t>Rachel Scott</t>
         </is>
       </c>
       <c r="K45" t="b">
         <v>0</v>
       </c>
       <c r="L45" t="n">
-        <v>377</v>
+        <v>997</v>
       </c>
       <c r="M45" t="n">
-        <v>0.376</v>
+        <v>0.325</v>
       </c>
       <c r="N45" t="n">
-        <v>2124.86</v>
+        <v>2747.73</v>
       </c>
       <c r="O45" t="n">
-        <v>1.3</v>
+        <v>1.4</v>
       </c>
       <c r="P45" t="b">
         <v>1</v>
@@ -3479,28 +3619,31 @@
         <v>0</v>
       </c>
       <c r="S45" t="b">
+        <v>0</v>
+      </c>
+      <c r="T45" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Barry Rodriguez</t>
+          <t>Kevin Howard</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Out lead contain.</t>
+          <t>Him good data evidence road.</t>
         </is>
       </c>
       <c r="C46" s="2" t="n">
-        <v>45261</v>
+        <v>45570</v>
       </c>
       <c r="D46" t="b">
         <v>0</v>
       </c>
       <c r="E46" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="F46" t="inlineStr">
         <is>
@@ -3508,33 +3651,33 @@
         </is>
       </c>
       <c r="G46" t="n">
-        <v>14.23</v>
+        <v>15.73</v>
       </c>
       <c r="H46" t="n">
-        <v>5849.88716951962</v>
+        <v>7157.333187254329</v>
       </c>
       <c r="I46" t="b">
         <v>0</v>
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>Ava Winters</t>
+          <t>Jason Clarke</t>
         </is>
       </c>
       <c r="K46" t="b">
         <v>0</v>
       </c>
       <c r="L46" t="n">
-        <v>426</v>
+        <v>707</v>
       </c>
       <c r="M46" t="n">
-        <v>0.388</v>
+        <v>0.483</v>
       </c>
       <c r="N46" t="n">
-        <v>2352.05</v>
+        <v>5371.5</v>
       </c>
       <c r="O46" t="n">
-        <v>2.5</v>
+        <v>1.3</v>
       </c>
       <c r="P46" t="b">
         <v>1</v>
@@ -3546,28 +3689,31 @@
         <v>0</v>
       </c>
       <c r="S46" t="b">
+        <v>0</v>
+      </c>
+      <c r="T46" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Linda Green</t>
+          <t>Sabrina Smith</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Doctor war fear.</t>
+          <t>High coach.</t>
         </is>
       </c>
       <c r="C47" s="2" t="n">
-        <v>45514</v>
+        <v>45298</v>
       </c>
       <c r="D47" t="b">
         <v>0</v>
       </c>
       <c r="E47" t="n">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="F47" t="inlineStr">
         <is>
@@ -3575,33 +3721,33 @@
         </is>
       </c>
       <c r="G47" t="n">
-        <v>8.4</v>
+        <v>17.98</v>
       </c>
       <c r="H47" t="n">
-        <v>5527.424390927449</v>
+        <v>6913.189846568979</v>
       </c>
       <c r="I47" t="b">
         <v>0</v>
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>Ava Winters</t>
+          <t>Jason Clarke</t>
         </is>
       </c>
       <c r="K47" t="b">
         <v>0</v>
       </c>
       <c r="L47" t="n">
-        <v>982</v>
+        <v>264</v>
       </c>
       <c r="M47" t="n">
-        <v>0.4</v>
+        <v>0.238</v>
       </c>
       <c r="N47" t="n">
-        <v>3299.52</v>
+        <v>1129.72</v>
       </c>
       <c r="O47" t="n">
-        <v>1.7</v>
+        <v>6.1</v>
       </c>
       <c r="P47" t="b">
         <v>1</v>
@@ -3614,61 +3760,64 @@
       </c>
       <c r="S47" t="b">
         <v>0</v>
+      </c>
+      <c r="T47" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Erica Johnson</t>
+          <t>Kelly Sexton</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Newspaper company example everyone.</t>
+          <t>Or either moment side.</t>
         </is>
       </c>
       <c r="C48" s="2" t="n">
-        <v>45622</v>
+        <v>45425</v>
       </c>
       <c r="D48" t="b">
         <v>0</v>
       </c>
       <c r="E48" t="n">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>ACX Exclusive</t>
+          <t>ACX Royalty Share</t>
         </is>
       </c>
       <c r="G48" t="n">
-        <v>14.54</v>
+        <v>11.31</v>
       </c>
       <c r="H48" t="n">
-        <v>6069.419161170575</v>
+        <v>964.7915755083902</v>
       </c>
       <c r="I48" t="b">
         <v>0</v>
       </c>
       <c r="J48" t="inlineStr">
         <is>
-          <t>Samantha Prescott</t>
+          <t>AI Narrator</t>
         </is>
       </c>
       <c r="K48" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L48" t="n">
-        <v>964</v>
+        <v>100</v>
       </c>
       <c r="M48" t="n">
-        <v>0.4</v>
+        <v>0.201</v>
       </c>
       <c r="N48" t="n">
-        <v>5606.62</v>
+        <v>227.33</v>
       </c>
       <c r="O48" t="n">
-        <v>1.1</v>
+        <v>4.2</v>
       </c>
       <c r="P48" t="b">
         <v>1</v>
@@ -3680,28 +3829,31 @@
         <v>0</v>
       </c>
       <c r="S48" t="b">
+        <v>0</v>
+      </c>
+      <c r="T48" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Shari Allen</t>
+          <t>Michelle Perez</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Painting draw.</t>
+          <t>What blue all.</t>
         </is>
       </c>
       <c r="C49" s="2" t="n">
-        <v>45648</v>
+        <v>45601</v>
       </c>
       <c r="D49" t="b">
         <v>0</v>
       </c>
       <c r="E49" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F49" t="inlineStr">
         <is>
@@ -3709,33 +3861,33 @@
         </is>
       </c>
       <c r="G49" t="n">
-        <v>10.07</v>
+        <v>11.31</v>
       </c>
       <c r="H49" t="n">
-        <v>6233.370393843223</v>
+        <v>3324.995815170355</v>
       </c>
       <c r="I49" t="b">
         <v>0</v>
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t>Ava Winters</t>
+          <t>Rachel Scott</t>
         </is>
       </c>
       <c r="K49" t="b">
         <v>0</v>
       </c>
       <c r="L49" t="n">
-        <v>746</v>
+        <v>285</v>
       </c>
       <c r="M49" t="n">
-        <v>0.31</v>
+        <v>0.406</v>
       </c>
       <c r="N49" t="n">
-        <v>2328.79</v>
+        <v>1308.68</v>
       </c>
       <c r="O49" t="n">
-        <v>2.7</v>
+        <v>2.5</v>
       </c>
       <c r="P49" t="b">
         <v>1</v>
@@ -3747,65 +3899,68 @@
         <v>0</v>
       </c>
       <c r="S49" t="b">
+        <v>0</v>
+      </c>
+      <c r="T49" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Tammy Sosa</t>
+          <t>Brian Rowe</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Floor treat rule one.</t>
+          <t>And business week.</t>
         </is>
       </c>
       <c r="C50" s="2" t="n">
-        <v>45392</v>
+        <v>45801</v>
       </c>
       <c r="D50" t="b">
         <v>0</v>
       </c>
       <c r="E50" t="n">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>ACX Exclusive</t>
+          <t>Spotify</t>
         </is>
       </c>
       <c r="G50" t="n">
-        <v>14.67</v>
+        <v>11.1</v>
       </c>
       <c r="H50" t="n">
-        <v>2228.167513817042</v>
+        <v>7272.63214523308</v>
       </c>
       <c r="I50" t="b">
         <v>0</v>
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t>Rachel Scott</t>
+          <t>Ava Winters</t>
         </is>
       </c>
       <c r="K50" t="b">
         <v>0</v>
       </c>
       <c r="L50" t="n">
-        <v>701</v>
+        <v>218</v>
       </c>
       <c r="M50" t="n">
-        <v>0.4</v>
+        <v>0.325</v>
       </c>
       <c r="N50" t="n">
-        <v>4113.47</v>
+        <v>786.4299999999999</v>
       </c>
       <c r="O50" t="n">
-        <v>0.5</v>
+        <v>9.199999999999999</v>
       </c>
       <c r="P50" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q50" t="b">
         <v>0</v>
@@ -3814,28 +3969,31 @@
         <v>0</v>
       </c>
       <c r="S50" t="b">
+        <v>0</v>
+      </c>
+      <c r="T50" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Brenda Henry</t>
+          <t>Melinda Morrison</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Create per page.</t>
+          <t>Front level million smile water.</t>
         </is>
       </c>
       <c r="C51" s="2" t="n">
-        <v>45329</v>
+        <v>45368</v>
       </c>
       <c r="D51" t="b">
         <v>0</v>
       </c>
       <c r="E51" t="n">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F51" t="inlineStr">
         <is>
@@ -3843,33 +4001,33 @@
         </is>
       </c>
       <c r="G51" t="n">
-        <v>19.83</v>
+        <v>9.66</v>
       </c>
       <c r="H51" t="n">
-        <v>7377.280533952046</v>
+        <v>7481.23356019066</v>
       </c>
       <c r="I51" t="b">
         <v>0</v>
       </c>
       <c r="J51" t="inlineStr">
         <is>
-          <t>Samantha Prescott</t>
+          <t>Ava Winters</t>
         </is>
       </c>
       <c r="K51" t="b">
         <v>0</v>
       </c>
       <c r="L51" t="n">
-        <v>359</v>
+        <v>573</v>
       </c>
       <c r="M51" t="n">
-        <v>0.363</v>
+        <v>0.493</v>
       </c>
       <c r="N51" t="n">
-        <v>2584.19</v>
+        <v>2728.84</v>
       </c>
       <c r="O51" t="n">
-        <v>2.9</v>
+        <v>2.7</v>
       </c>
       <c r="P51" t="b">
         <v>1</v>
@@ -3881,6 +4039,9 @@
         <v>0</v>
       </c>
       <c r="S51" t="b">
+        <v>0</v>
+      </c>
+      <c r="T51" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated narrator_split logic to exclude AI narrators
</commit_message>
<xml_diff>
--- a/FakeRoyaltyData.xlsx
+++ b/FakeRoyaltyData.xlsx
@@ -16,9 +16,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
     <numFmt numFmtId="165" formatCode="YYYY-MM-DD"/>
+    <numFmt numFmtId="166" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="167" formatCode="YYYY-MM-DD HH:MM:SS"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -58,12 +60,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -429,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T51"/>
+  <dimension ref="A1:U51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -510,30 +513,35 @@
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>Months to Break Even</t>
+          <t>Est. Months to Break Even</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>Has Broken Even</t>
+          <t>Break Even Status</t>
         </is>
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
+          <t>Break Even Date</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
           <t>Loss Leader</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>Risky Combo</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>Overachiever</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>ACX Royalty Share Risk</t>
         </is>
@@ -542,33 +550,33 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Bryan Haynes</t>
+          <t>Zachary Mitchell</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Explain ahead.</t>
+          <t>Door season.</t>
         </is>
       </c>
       <c r="C2" s="2" t="n">
-        <v>45799</v>
+        <v>45534</v>
       </c>
       <c r="D2" t="b">
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>ACX Exclusive</t>
+          <t>Findaway</t>
         </is>
       </c>
       <c r="G2" t="n">
-        <v>8.210000000000001</v>
+        <v>9.19</v>
       </c>
       <c r="H2" t="n">
-        <v>3932.968438557998</v>
+        <v>3341.705740653547</v>
       </c>
       <c r="I2" t="b">
         <v>0</v>
@@ -582,22 +590,24 @@
         <v>0</v>
       </c>
       <c r="L2" t="n">
-        <v>195</v>
+        <v>493</v>
       </c>
       <c r="M2" t="n">
-        <v>0.4</v>
+        <v>0.352</v>
       </c>
       <c r="N2" t="n">
-        <v>640.38</v>
+        <v>1594.8</v>
       </c>
       <c r="O2" t="n">
-        <v>6.1</v>
-      </c>
-      <c r="P2" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q2" t="b">
-        <v>0</v>
+        <v>2.1</v>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>Broken Even</t>
+        </is>
+      </c>
+      <c r="Q2" s="3" t="n">
+        <v>45595</v>
       </c>
       <c r="R2" t="b">
         <v>0</v>
@@ -606,28 +616,31 @@
         <v>0</v>
       </c>
       <c r="T2" t="b">
+        <v>0</v>
+      </c>
+      <c r="U2" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Jonathan Wilkins</t>
+          <t>Shaun Acevedo</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Represent however.</t>
+          <t>Physical hour learn try.</t>
         </is>
       </c>
       <c r="C3" s="2" t="n">
-        <v>45351</v>
+        <v>45207</v>
       </c>
       <c r="D3" t="b">
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -635,10 +648,10 @@
         </is>
       </c>
       <c r="G3" t="n">
-        <v>16.82</v>
+        <v>8.109999999999999</v>
       </c>
       <c r="H3" t="n">
-        <v>0</v>
+        <v>440.8970725424173</v>
       </c>
       <c r="I3" t="b">
         <v>1</v>
@@ -652,24 +665,28 @@
         <v>1</v>
       </c>
       <c r="L3" t="n">
-        <v>270</v>
+        <v>213</v>
       </c>
       <c r="M3" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.065</v>
       </c>
       <c r="N3" t="n">
-        <v>317.9</v>
+        <v>112.28</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>Never</t>
-        </is>
-      </c>
-      <c r="P3" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q3" t="b">
-        <v>0</v>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>Unclear - No Earnings Yet</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
       </c>
       <c r="R3" t="b">
         <v>0</v>
@@ -678,68 +695,73 @@
         <v>0</v>
       </c>
       <c r="T3" t="b">
+        <v>0</v>
+      </c>
+      <c r="U3" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Jessica King</t>
+          <t>Jennifer Hamilton</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Factor positive ahead kitchen.</t>
+          <t>People wide after student.</t>
         </is>
       </c>
       <c r="C4" s="2" t="n">
-        <v>45422</v>
+        <v>45361</v>
       </c>
       <c r="D4" t="b">
         <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>ACX Exclusive</t>
+          <t>BookFunnel</t>
         </is>
       </c>
       <c r="G4" t="n">
-        <v>9.07</v>
+        <v>15.97</v>
       </c>
       <c r="H4" t="n">
-        <v>3651.262443047395</v>
+        <v>0</v>
       </c>
       <c r="I4" t="b">
         <v>0</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>Rachel Scott</t>
+          <t>AI Narrator</t>
         </is>
       </c>
       <c r="K4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L4" t="n">
-        <v>471</v>
+        <v>397</v>
       </c>
       <c r="M4" t="n">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="N4" t="n">
-        <v>1708.79</v>
+        <v>6340.09</v>
       </c>
       <c r="O4" t="n">
-        <v>2.1</v>
-      </c>
-      <c r="P4" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q4" t="b">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>Already Profitable</t>
+        </is>
+      </c>
+      <c r="Q4" s="3" t="n">
+        <v>45361</v>
       </c>
       <c r="R4" t="b">
         <v>0</v>
@@ -748,28 +770,31 @@
         <v>0</v>
       </c>
       <c r="T4" t="b">
+        <v>0</v>
+      </c>
+      <c r="U4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Anthony Martinez</t>
+          <t>Christopher Chambers</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Moment year challenge.</t>
+          <t>Practice culture.</t>
         </is>
       </c>
       <c r="C5" s="2" t="n">
-        <v>45272</v>
+        <v>45372</v>
       </c>
       <c r="D5" t="b">
         <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
@@ -777,109 +802,120 @@
         </is>
       </c>
       <c r="G5" t="n">
-        <v>14.36</v>
+        <v>16.87</v>
       </c>
       <c r="H5" t="n">
-        <v>950.7898537906642</v>
+        <v>7429.580411962652</v>
       </c>
       <c r="I5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>AI Narrator</t>
+          <t>Samantha Prescott</t>
         </is>
       </c>
       <c r="K5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L5" t="n">
-        <v>233</v>
+        <v>49</v>
       </c>
       <c r="M5" t="n">
-        <v>0.202</v>
+        <v>0.053</v>
       </c>
       <c r="N5" t="n">
-        <v>675.87</v>
-      </c>
-      <c r="O5" t="n">
-        <v>1.4</v>
-      </c>
-      <c r="P5" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q5" t="b">
-        <v>0</v>
+        <v>43.81</v>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>Unclear - No Earnings Yet</t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
       </c>
       <c r="R5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T5" t="b">
         <v>0</v>
+      </c>
+      <c r="U5" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Donald Lewis</t>
+          <t>Harold Chambers</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Side along home join.</t>
+          <t>Time remain.</t>
         </is>
       </c>
       <c r="C6" s="2" t="n">
-        <v>45371</v>
+        <v>45163</v>
       </c>
       <c r="D6" t="b">
         <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>ACX Exclusive</t>
+          <t>BookFunnel</t>
         </is>
       </c>
       <c r="G6" t="n">
-        <v>12.78</v>
+        <v>17.99</v>
       </c>
       <c r="H6" t="n">
-        <v>6377.844990895401</v>
+        <v>4975.916428301225</v>
       </c>
       <c r="I6" t="b">
         <v>0</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>Ava Winters</t>
+          <t>Samantha Prescott</t>
         </is>
       </c>
       <c r="K6" t="b">
         <v>0</v>
       </c>
       <c r="L6" t="n">
-        <v>686</v>
+        <v>823</v>
       </c>
       <c r="M6" t="n">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="N6" t="n">
-        <v>3506.83</v>
+        <v>14805.77</v>
       </c>
       <c r="O6" t="n">
-        <v>1.8</v>
-      </c>
-      <c r="P6" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q6" t="b">
-        <v>0</v>
+        <v>0.3</v>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>Broken Even</t>
+        </is>
+      </c>
+      <c r="Q6" s="3" t="n">
+        <v>45163</v>
       </c>
       <c r="R6" t="b">
         <v>0</v>
@@ -888,68 +924,73 @@
         <v>0</v>
       </c>
       <c r="T6" t="b">
+        <v>0</v>
+      </c>
+      <c r="U6" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Rebecca Lindsey</t>
+          <t>Melinda Hanson</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Behind again up visit.</t>
+          <t>Local head hotel.</t>
         </is>
       </c>
       <c r="C7" s="2" t="n">
-        <v>45727</v>
+        <v>45560</v>
       </c>
       <c r="D7" t="b">
         <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Findaway</t>
+          <t>Spotify</t>
         </is>
       </c>
       <c r="G7" t="n">
-        <v>19.11</v>
+        <v>13.1</v>
       </c>
       <c r="H7" t="n">
-        <v>6593.356572053783</v>
+        <v>2112.535741254155</v>
       </c>
       <c r="I7" t="b">
         <v>0</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>Ava Winters</t>
+          <t>Taylor James</t>
         </is>
       </c>
       <c r="K7" t="b">
         <v>0</v>
       </c>
       <c r="L7" t="n">
-        <v>470</v>
+        <v>577</v>
       </c>
       <c r="M7" t="n">
-        <v>0.354</v>
+        <v>0.433</v>
       </c>
       <c r="N7" t="n">
-        <v>3179.52</v>
+        <v>3272.92</v>
       </c>
       <c r="O7" t="n">
-        <v>2.1</v>
-      </c>
-      <c r="P7" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q7" t="b">
-        <v>0</v>
+        <v>0.6</v>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>Broken Even</t>
+        </is>
+      </c>
+      <c r="Q7" s="3" t="n">
+        <v>45560</v>
       </c>
       <c r="R7" t="b">
         <v>0</v>
@@ -958,68 +999,73 @@
         <v>0</v>
       </c>
       <c r="T7" t="b">
+        <v>0</v>
+      </c>
+      <c r="U7" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Tara Martin</t>
+          <t>Sarah Murphy</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Over write street national.</t>
+          <t>Purpose Mr parent.</t>
         </is>
       </c>
       <c r="C8" s="2" t="n">
-        <v>45514</v>
+        <v>45705</v>
       </c>
       <c r="D8" t="b">
         <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Findaway</t>
+          <t>BookFunnel</t>
         </is>
       </c>
       <c r="G8" t="n">
-        <v>14.19</v>
+        <v>14.66</v>
       </c>
       <c r="H8" t="n">
-        <v>3050.656946880579</v>
+        <v>7666.295898688704</v>
       </c>
       <c r="I8" t="b">
         <v>0</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>Taylor James</t>
+          <t>Ava Winters</t>
         </is>
       </c>
       <c r="K8" t="b">
         <v>0</v>
       </c>
       <c r="L8" t="n">
-        <v>897</v>
+        <v>519</v>
       </c>
       <c r="M8" t="n">
-        <v>0.314</v>
+        <v>1</v>
       </c>
       <c r="N8" t="n">
-        <v>3996.73</v>
+        <v>7608.54</v>
       </c>
       <c r="O8" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="P8" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q8" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>Broken Even</t>
+        </is>
+      </c>
+      <c r="Q8" s="3" t="n">
+        <v>45733</v>
       </c>
       <c r="R8" t="b">
         <v>0</v>
@@ -1028,68 +1074,73 @@
         <v>0</v>
       </c>
       <c r="T8" t="b">
+        <v>0</v>
+      </c>
+      <c r="U8" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Andrea Matthews</t>
+          <t>John Mccormick</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Require she practice rich matter.</t>
+          <t>Popular hot team fill.</t>
         </is>
       </c>
       <c r="C9" s="2" t="n">
-        <v>45401</v>
+        <v>45516</v>
       </c>
       <c r="D9" t="b">
         <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Findaway</t>
+          <t>BookFunnel</t>
         </is>
       </c>
       <c r="G9" t="n">
-        <v>12.73</v>
+        <v>11.25</v>
       </c>
       <c r="H9" t="n">
-        <v>6611.345762147565</v>
+        <v>2450.005873265604</v>
       </c>
       <c r="I9" t="b">
         <v>0</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>Ava Winters</t>
+          <t>Rachel Scott</t>
         </is>
       </c>
       <c r="K9" t="b">
         <v>0</v>
       </c>
       <c r="L9" t="n">
-        <v>470</v>
+        <v>283</v>
       </c>
       <c r="M9" t="n">
-        <v>0.399</v>
+        <v>1</v>
       </c>
       <c r="N9" t="n">
-        <v>2387.26</v>
+        <v>3183.75</v>
       </c>
       <c r="O9" t="n">
-        <v>2.8</v>
-      </c>
-      <c r="P9" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q9" t="b">
-        <v>0</v>
+        <v>0.8</v>
+      </c>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>Broken Even</t>
+        </is>
+      </c>
+      <c r="Q9" s="3" t="n">
+        <v>45516</v>
       </c>
       <c r="R9" t="b">
         <v>0</v>
@@ -1098,28 +1149,31 @@
         <v>0</v>
       </c>
       <c r="T9" t="b">
+        <v>0</v>
+      </c>
+      <c r="U9" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Kenneth Williams</t>
+          <t>Dr. Robert Rodriguez</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Also market leader prove.</t>
+          <t>Sure now.</t>
         </is>
       </c>
       <c r="C10" s="2" t="n">
-        <v>45746</v>
+        <v>45548</v>
       </c>
       <c r="D10" t="b">
         <v>0</v>
       </c>
       <c r="E10" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
@@ -1127,39 +1181,41 @@
         </is>
       </c>
       <c r="G10" t="n">
-        <v>11.54</v>
+        <v>8.48</v>
       </c>
       <c r="H10" t="n">
-        <v>3529.160304959022</v>
+        <v>769.4661118451934</v>
       </c>
       <c r="I10" t="b">
         <v>0</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>Taylor James</t>
+          <t>AI Narrator</t>
         </is>
       </c>
       <c r="K10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L10" t="n">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="M10" t="n">
-        <v>0.317</v>
+        <v>0.435</v>
       </c>
       <c r="N10" t="n">
-        <v>1035.26</v>
+        <v>1021.8</v>
       </c>
       <c r="O10" t="n">
-        <v>3.4</v>
-      </c>
-      <c r="P10" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q10" t="b">
-        <v>0</v>
+        <v>0.8</v>
+      </c>
+      <c r="P10" t="inlineStr">
+        <is>
+          <t>Broken Even</t>
+        </is>
+      </c>
+      <c r="Q10" s="3" t="n">
+        <v>45548</v>
       </c>
       <c r="R10" t="b">
         <v>0</v>
@@ -1168,68 +1224,73 @@
         <v>0</v>
       </c>
       <c r="T10" t="b">
+        <v>0</v>
+      </c>
+      <c r="U10" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Tiffany Hernandez</t>
+          <t>Brian Fitzgerald</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Seven perhaps.</t>
+          <t>Second very central ten.</t>
         </is>
       </c>
       <c r="C11" s="2" t="n">
-        <v>45734</v>
+        <v>45238</v>
       </c>
       <c r="D11" t="b">
         <v>0</v>
       </c>
       <c r="E11" t="n">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Findaway</t>
+          <t>BookFunnel</t>
         </is>
       </c>
       <c r="G11" t="n">
-        <v>17.58</v>
+        <v>18.99</v>
       </c>
       <c r="H11" t="n">
-        <v>6180.114869840088</v>
+        <v>7230.368140198609</v>
       </c>
       <c r="I11" t="b">
         <v>0</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>Jason Clarke</t>
+          <t>Ava Winters</t>
         </is>
       </c>
       <c r="K11" t="b">
         <v>0</v>
       </c>
       <c r="L11" t="n">
-        <v>153</v>
+        <v>539</v>
       </c>
       <c r="M11" t="n">
-        <v>0.375</v>
+        <v>1</v>
       </c>
       <c r="N11" t="n">
-        <v>1008.65</v>
+        <v>10235.61</v>
       </c>
       <c r="O11" t="n">
-        <v>6.1</v>
-      </c>
-      <c r="P11" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q11" t="b">
-        <v>0</v>
+        <v>0.7</v>
+      </c>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>Broken Even</t>
+        </is>
+      </c>
+      <c r="Q11" s="3" t="n">
+        <v>45238</v>
       </c>
       <c r="R11" t="b">
         <v>0</v>
@@ -1238,68 +1299,73 @@
         <v>0</v>
       </c>
       <c r="T11" t="b">
+        <v>0</v>
+      </c>
+      <c r="U11" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Rachel Brown</t>
+          <t>Eric James</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Month realize begin.</t>
+          <t>Customer wife necessary try.</t>
         </is>
       </c>
       <c r="C12" s="2" t="n">
-        <v>45229</v>
+        <v>45456</v>
       </c>
       <c r="D12" t="b">
         <v>0</v>
       </c>
       <c r="E12" t="n">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>BookFunnel</t>
+          <t>ACX Exclusive</t>
         </is>
       </c>
       <c r="G12" t="n">
-        <v>15.27</v>
+        <v>19.56</v>
       </c>
       <c r="H12" t="n">
-        <v>443.1865504897143</v>
+        <v>5536.372903618159</v>
       </c>
       <c r="I12" t="b">
         <v>0</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>AI Narrator</t>
+          <t>Jason Clarke</t>
         </is>
       </c>
       <c r="K12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L12" t="n">
-        <v>552</v>
+        <v>525</v>
       </c>
       <c r="M12" t="n">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="N12" t="n">
-        <v>8429.040000000001</v>
+        <v>4107.6</v>
       </c>
       <c r="O12" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="P12" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q12" t="b">
-        <v>0</v>
+        <v>1.3</v>
+      </c>
+      <c r="P12" t="inlineStr">
+        <is>
+          <t>Broken Even</t>
+        </is>
+      </c>
+      <c r="Q12" s="3" t="n">
+        <v>45486</v>
       </c>
       <c r="R12" t="b">
         <v>0</v>
@@ -1308,68 +1374,73 @@
         <v>0</v>
       </c>
       <c r="T12" t="b">
+        <v>0</v>
+      </c>
+      <c r="U12" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Kimberly Bailey</t>
+          <t>Lisa Wiley MD</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Likely various religious.</t>
+          <t>Science adult offer anyone together.</t>
         </is>
       </c>
       <c r="C13" s="2" t="n">
-        <v>45794</v>
+        <v>45726</v>
       </c>
       <c r="D13" t="b">
         <v>0</v>
       </c>
       <c r="E13" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Spotify</t>
+          <t>BookFunnel</t>
         </is>
       </c>
       <c r="G13" t="n">
-        <v>9</v>
+        <v>17.49</v>
       </c>
       <c r="H13" t="n">
-        <v>5704.111562454361</v>
+        <v>0</v>
       </c>
       <c r="I13" t="b">
         <v>0</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>Jason Clarke</t>
+          <t>AI Narrator</t>
         </is>
       </c>
       <c r="K13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L13" t="n">
-        <v>197</v>
+        <v>593</v>
       </c>
       <c r="M13" t="n">
-        <v>0.367</v>
+        <v>1</v>
       </c>
       <c r="N13" t="n">
-        <v>650.6900000000001</v>
+        <v>10371.57</v>
       </c>
       <c r="O13" t="n">
-        <v>8.800000000000001</v>
-      </c>
-      <c r="P13" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q13" t="b">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="P13" t="inlineStr">
+        <is>
+          <t>Already Profitable</t>
+        </is>
+      </c>
+      <c r="Q13" s="3" t="n">
+        <v>45726</v>
       </c>
       <c r="R13" t="b">
         <v>0</v>
@@ -1378,68 +1449,73 @@
         <v>0</v>
       </c>
       <c r="T13" t="b">
+        <v>0</v>
+      </c>
+      <c r="U13" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Joseph Rodriguez</t>
+          <t>Kathleen Castillo</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Trip movement miss daughter.</t>
+          <t>Middle control could.</t>
         </is>
       </c>
       <c r="C14" s="2" t="n">
-        <v>45340</v>
+        <v>45823</v>
       </c>
       <c r="D14" t="b">
         <v>0</v>
       </c>
       <c r="E14" t="n">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>ACX Exclusive</t>
+          <t>BookFunnel</t>
         </is>
       </c>
       <c r="G14" t="n">
-        <v>19.35</v>
+        <v>19.94</v>
       </c>
       <c r="H14" t="n">
-        <v>7800.075621364695</v>
+        <v>4382.863249673006</v>
       </c>
       <c r="I14" t="b">
         <v>0</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>Jason Clarke</t>
+          <t>Ava Winters</t>
         </is>
       </c>
       <c r="K14" t="b">
         <v>0</v>
       </c>
       <c r="L14" t="n">
-        <v>823</v>
+        <v>137</v>
       </c>
       <c r="M14" t="n">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="N14" t="n">
-        <v>6370.02</v>
+        <v>2731.78</v>
       </c>
       <c r="O14" t="n">
-        <v>1.2</v>
-      </c>
-      <c r="P14" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q14" t="b">
-        <v>0</v>
+        <v>1.6</v>
+      </c>
+      <c r="P14" t="inlineStr">
+        <is>
+          <t>In Progress</t>
+        </is>
+      </c>
+      <c r="Q14" s="3" t="n">
+        <v>45853</v>
       </c>
       <c r="R14" t="b">
         <v>0</v>
@@ -1448,70 +1524,73 @@
         <v>0</v>
       </c>
       <c r="T14" t="b">
+        <v>0</v>
+      </c>
+      <c r="U14" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Maria Berry</t>
+          <t>Richard West</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>How father bad fight maintain.</t>
+          <t>Carry wonder.</t>
         </is>
       </c>
       <c r="C15" s="2" t="n">
-        <v>45859</v>
+        <v>45459</v>
       </c>
       <c r="D15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E15" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Spotify</t>
+          <t>Findaway</t>
         </is>
       </c>
       <c r="G15" t="n">
-        <v>10.01</v>
+        <v>16.09</v>
       </c>
       <c r="H15" t="n">
-        <v>0</v>
+        <v>3961.137660849773</v>
       </c>
       <c r="I15" t="b">
         <v>0</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>AI Narrator</t>
+          <t>Taylor James</t>
         </is>
       </c>
       <c r="K15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L15" t="n">
-        <v>231</v>
+        <v>542</v>
       </c>
       <c r="M15" t="n">
-        <v>0.447</v>
+        <v>0.364</v>
       </c>
       <c r="N15" t="n">
-        <v>1033.6</v>
-      </c>
-      <c r="O15" t="inlineStr">
-        <is>
-          <t>Never</t>
-        </is>
-      </c>
-      <c r="P15" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q15" t="b">
-        <v>0</v>
+        <v>3174.36</v>
+      </c>
+      <c r="O15" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="P15" t="inlineStr">
+        <is>
+          <t>Broken Even</t>
+        </is>
+      </c>
+      <c r="Q15" s="3" t="n">
+        <v>45489</v>
       </c>
       <c r="R15" t="b">
         <v>0</v>
@@ -1520,68 +1599,73 @@
         <v>0</v>
       </c>
       <c r="T15" t="b">
+        <v>0</v>
+      </c>
+      <c r="U15" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Amber King</t>
+          <t>Caitlin Valencia</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Enjoy strategy least.</t>
+          <t>Shoulder general to.</t>
         </is>
       </c>
       <c r="C16" s="2" t="n">
-        <v>45816</v>
+        <v>45709</v>
       </c>
       <c r="D16" t="b">
         <v>0</v>
       </c>
       <c r="E16" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>ACX Exclusive</t>
+          <t>ACX Royalty Share</t>
         </is>
       </c>
       <c r="G16" t="n">
-        <v>13.87</v>
+        <v>19.94</v>
       </c>
       <c r="H16" t="n">
-        <v>434.4362099128309</v>
+        <v>2560.983935912456</v>
       </c>
       <c r="I16" t="b">
         <v>0</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>AI Narrator</t>
+          <t>Rachel Scott</t>
         </is>
       </c>
       <c r="K16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L16" t="n">
-        <v>301</v>
+        <v>68</v>
       </c>
       <c r="M16" t="n">
-        <v>0.4</v>
+        <v>0.238</v>
       </c>
       <c r="N16" t="n">
-        <v>1669.95</v>
+        <v>322.71</v>
       </c>
       <c r="O16" t="n">
-        <v>0.3</v>
-      </c>
-      <c r="P16" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q16" t="b">
-        <v>0</v>
+        <v>7.9</v>
+      </c>
+      <c r="P16" t="inlineStr">
+        <is>
+          <t>In Progress</t>
+        </is>
+      </c>
+      <c r="Q16" s="3" t="n">
+        <v>45921</v>
       </c>
       <c r="R16" t="b">
         <v>0</v>
@@ -1591,27 +1675,30 @@
       </c>
       <c r="T16" t="b">
         <v>0</v>
+      </c>
+      <c r="U16" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Christine Hernandez</t>
+          <t>Jesse Roman</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Idea agency capital candidate kid.</t>
+          <t>Reveal interest nearly.</t>
         </is>
       </c>
       <c r="C17" s="2" t="n">
-        <v>45348</v>
+        <v>45854</v>
       </c>
       <c r="D17" t="b">
         <v>0</v>
       </c>
       <c r="E17" t="n">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
@@ -1619,39 +1706,41 @@
         </is>
       </c>
       <c r="G17" t="n">
-        <v>15.78</v>
+        <v>15.88</v>
       </c>
       <c r="H17" t="n">
-        <v>9732.347567428691</v>
+        <v>3509.962943414947</v>
       </c>
       <c r="I17" t="b">
         <v>0</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>Jason Clarke</t>
+          <t>Taylor James</t>
         </is>
       </c>
       <c r="K17" t="b">
         <v>0</v>
       </c>
       <c r="L17" t="n">
-        <v>78</v>
+        <v>28</v>
       </c>
       <c r="M17" t="n">
-        <v>0.221</v>
+        <v>0.225</v>
       </c>
       <c r="N17" t="n">
-        <v>272.02</v>
+        <v>100.04</v>
       </c>
       <c r="O17" t="n">
-        <v>35.8</v>
-      </c>
-      <c r="P17" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q17" t="b">
-        <v>0</v>
+        <v>35.1</v>
+      </c>
+      <c r="P17" t="inlineStr">
+        <is>
+          <t>In Progress</t>
+        </is>
+      </c>
+      <c r="Q17" s="3" t="n">
+        <v>46920</v>
       </c>
       <c r="R17" t="b">
         <v>0</v>
@@ -1660,138 +1749,152 @@
         <v>0</v>
       </c>
       <c r="T17" t="b">
+        <v>0</v>
+      </c>
+      <c r="U17" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Regina Lee</t>
+          <t>Jennifer Shelton</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Upon drop forward.</t>
+          <t>Model population support matter contain.</t>
         </is>
       </c>
       <c r="C18" s="2" t="n">
-        <v>45673</v>
+        <v>45468</v>
       </c>
       <c r="D18" t="b">
         <v>0</v>
       </c>
       <c r="E18" t="n">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>ACX Exclusive</t>
+          <t>ACX Royalty Share</t>
         </is>
       </c>
       <c r="G18" t="n">
-        <v>10.45</v>
+        <v>19.8</v>
       </c>
       <c r="H18" t="n">
-        <v>3329.354960952243</v>
+        <v>838.1780411346118</v>
       </c>
       <c r="I18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>Rachel Scott</t>
+          <t>AI Narrator</t>
         </is>
       </c>
       <c r="K18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L18" t="n">
-        <v>219</v>
+        <v>81</v>
       </c>
       <c r="M18" t="n">
-        <v>0.4</v>
+        <v>0.06950000000000001</v>
       </c>
       <c r="N18" t="n">
-        <v>915.42</v>
-      </c>
-      <c r="O18" t="n">
-        <v>3.6</v>
-      </c>
-      <c r="P18" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q18" t="b">
-        <v>0</v>
+        <v>111.46</v>
+      </c>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="P18" t="inlineStr">
+        <is>
+          <t>Unclear - No Earnings Yet</t>
+        </is>
+      </c>
+      <c r="Q18" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
       </c>
       <c r="R18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S18" t="b">
         <v>0</v>
       </c>
       <c r="T18" t="b">
         <v>0</v>
+      </c>
+      <c r="U18" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Carol Lewis</t>
+          <t>Tyler Lindsey</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Could poor also school can.</t>
+          <t>Table no.</t>
         </is>
       </c>
       <c r="C19" s="2" t="n">
-        <v>45511</v>
+        <v>45230</v>
       </c>
       <c r="D19" t="b">
         <v>0</v>
       </c>
       <c r="E19" t="n">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Spotify</t>
+          <t>ACX Exclusive</t>
         </is>
       </c>
       <c r="G19" t="n">
-        <v>19.26</v>
+        <v>18.78</v>
       </c>
       <c r="H19" t="n">
-        <v>5472.196858004498</v>
+        <v>3229.064146287317</v>
       </c>
       <c r="I19" t="b">
         <v>0</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>Jason Clarke</t>
+          <t>Taylor James</t>
         </is>
       </c>
       <c r="K19" t="b">
         <v>0</v>
       </c>
       <c r="L19" t="n">
-        <v>943</v>
+        <v>893</v>
       </c>
       <c r="M19" t="n">
-        <v>0.361</v>
+        <v>0.4</v>
       </c>
       <c r="N19" t="n">
-        <v>6556.55</v>
+        <v>6708.22</v>
       </c>
       <c r="O19" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="P19" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q19" t="b">
-        <v>0</v>
+        <v>0.5</v>
+      </c>
+      <c r="P19" t="inlineStr">
+        <is>
+          <t>Broken Even</t>
+        </is>
+      </c>
+      <c r="Q19" s="3" t="n">
+        <v>45230</v>
       </c>
       <c r="R19" t="b">
         <v>0</v>
@@ -1800,138 +1903,152 @@
         <v>0</v>
       </c>
       <c r="T19" t="b">
+        <v>0</v>
+      </c>
+      <c r="U19" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>James Lucas</t>
+          <t>Beth Smith</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Particularly raise.</t>
+          <t>Letter firm everyone me.</t>
         </is>
       </c>
       <c r="C20" s="2" t="n">
-        <v>45682</v>
+        <v>45423</v>
       </c>
       <c r="D20" t="b">
         <v>0</v>
       </c>
       <c r="E20" t="n">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>BookFunnel</t>
+          <t>ACX Royalty Share</t>
         </is>
       </c>
       <c r="G20" t="n">
-        <v>19.7</v>
+        <v>18.14</v>
       </c>
       <c r="H20" t="n">
-        <v>6351.566400707906</v>
+        <v>271.0429071568856</v>
       </c>
       <c r="I20" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>Samantha Prescott</t>
+          <t>AI Narrator</t>
         </is>
       </c>
       <c r="K20" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L20" t="n">
-        <v>981</v>
+        <v>70</v>
       </c>
       <c r="M20" t="n">
-        <v>1</v>
+        <v>0.0725</v>
       </c>
       <c r="N20" t="n">
-        <v>19325.7</v>
-      </c>
-      <c r="O20" t="n">
-        <v>0.3</v>
-      </c>
-      <c r="P20" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q20" t="b">
-        <v>0</v>
+        <v>92.06</v>
+      </c>
+      <c r="O20" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="P20" t="inlineStr">
+        <is>
+          <t>Unclear - No Earnings Yet</t>
+        </is>
+      </c>
+      <c r="Q20" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
       </c>
       <c r="R20" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S20" t="b">
         <v>0</v>
       </c>
       <c r="T20" t="b">
         <v>0</v>
+      </c>
+      <c r="U20" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Charles Lin DVM</t>
+          <t>Gina Wood</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Shoulder box action family never.</t>
+          <t>Attention only poor fast.</t>
         </is>
       </c>
       <c r="C21" s="2" t="n">
-        <v>45169</v>
+        <v>45252</v>
       </c>
       <c r="D21" t="b">
         <v>0</v>
       </c>
       <c r="E21" t="n">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>ACX Exclusive</t>
+          <t>Spotify</t>
         </is>
       </c>
       <c r="G21" t="n">
-        <v>17.38</v>
+        <v>15.33</v>
       </c>
       <c r="H21" t="n">
-        <v>7145.364156454812</v>
+        <v>3285.422706093346</v>
       </c>
       <c r="I21" t="b">
         <v>0</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>Ava Winters</t>
+          <t>Rachel Scott</t>
         </is>
       </c>
       <c r="K21" t="b">
         <v>0</v>
       </c>
       <c r="L21" t="n">
-        <v>529</v>
+        <v>687</v>
       </c>
       <c r="M21" t="n">
-        <v>0.4</v>
+        <v>0.44</v>
       </c>
       <c r="N21" t="n">
-        <v>3677.61</v>
+        <v>4633.95</v>
       </c>
       <c r="O21" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="P21" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q21" t="b">
-        <v>0</v>
+        <v>0.7</v>
+      </c>
+      <c r="P21" t="inlineStr">
+        <is>
+          <t>Broken Even</t>
+        </is>
+      </c>
+      <c r="Q21" s="3" t="n">
+        <v>45252</v>
       </c>
       <c r="R21" t="b">
         <v>0</v>
@@ -1940,22 +2057,25 @@
         <v>0</v>
       </c>
       <c r="T21" t="b">
+        <v>0</v>
+      </c>
+      <c r="U21" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Jason Keller</t>
+          <t>Thomas Harding</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Player man.</t>
+          <t>Young force mean.</t>
         </is>
       </c>
       <c r="C22" s="2" t="n">
-        <v>45151</v>
+        <v>45170</v>
       </c>
       <c r="D22" t="b">
         <v>0</v>
@@ -1965,43 +2085,45 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Findaway</t>
+          <t>BookFunnel</t>
         </is>
       </c>
       <c r="G22" t="n">
-        <v>11.02</v>
+        <v>15.17</v>
       </c>
       <c r="H22" t="n">
-        <v>2133.771964044494</v>
+        <v>2779.422082054393</v>
       </c>
       <c r="I22" t="b">
         <v>0</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>Rachel Scott</t>
+          <t>Taylor James</t>
         </is>
       </c>
       <c r="K22" t="b">
         <v>0</v>
       </c>
       <c r="L22" t="n">
-        <v>514</v>
+        <v>618</v>
       </c>
       <c r="M22" t="n">
-        <v>0.318</v>
+        <v>1</v>
       </c>
       <c r="N22" t="n">
-        <v>1801.24</v>
+        <v>9375.059999999999</v>
       </c>
       <c r="O22" t="n">
-        <v>1.2</v>
-      </c>
-      <c r="P22" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q22" t="b">
-        <v>0</v>
+        <v>0.3</v>
+      </c>
+      <c r="P22" t="inlineStr">
+        <is>
+          <t>Broken Even</t>
+        </is>
+      </c>
+      <c r="Q22" s="3" t="n">
+        <v>45170</v>
       </c>
       <c r="R22" t="b">
         <v>0</v>
@@ -2010,68 +2132,73 @@
         <v>0</v>
       </c>
       <c r="T22" t="b">
+        <v>0</v>
+      </c>
+      <c r="U22" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Jessica Mcbride</t>
+          <t>Robert Snow Jr.</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Bag point physical receive price.</t>
+          <t>Organization lot blue.</t>
         </is>
       </c>
       <c r="C23" s="2" t="n">
-        <v>45294</v>
+        <v>45230</v>
       </c>
       <c r="D23" t="b">
         <v>0</v>
       </c>
       <c r="E23" t="n">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>ACX Royalty Share</t>
+          <t>Findaway</t>
         </is>
       </c>
       <c r="G23" t="n">
-        <v>18.86</v>
+        <v>11.49</v>
       </c>
       <c r="H23" t="n">
-        <v>8084.186305809782</v>
+        <v>2653.002800785634</v>
       </c>
       <c r="I23" t="b">
         <v>0</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>Jason Clarke</t>
+          <t>Rachel Scott</t>
         </is>
       </c>
       <c r="K23" t="b">
         <v>0</v>
       </c>
       <c r="L23" t="n">
-        <v>284</v>
+        <v>613</v>
       </c>
       <c r="M23" t="n">
-        <v>0.191</v>
+        <v>0.36</v>
       </c>
       <c r="N23" t="n">
-        <v>1023.04</v>
+        <v>2535.61</v>
       </c>
       <c r="O23" t="n">
-        <v>7.9</v>
-      </c>
-      <c r="P23" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q23" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="P23" t="inlineStr">
+        <is>
+          <t>Broken Even</t>
+        </is>
+      </c>
+      <c r="Q23" s="3" t="n">
+        <v>45260</v>
       </c>
       <c r="R23" t="b">
         <v>0</v>
@@ -2080,28 +2207,31 @@
         <v>0</v>
       </c>
       <c r="T23" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="U23" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Scott Welch</t>
+          <t>Melanie Rosario</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Produce law actually risk.</t>
+          <t>Choice power store team.</t>
         </is>
       </c>
       <c r="C24" s="2" t="n">
-        <v>45731</v>
+        <v>45703</v>
       </c>
       <c r="D24" t="b">
         <v>0</v>
       </c>
       <c r="E24" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
@@ -2109,10 +2239,10 @@
         </is>
       </c>
       <c r="G24" t="n">
-        <v>12.88</v>
+        <v>14.84</v>
       </c>
       <c r="H24" t="n">
-        <v>0</v>
+        <v>741.3379050737858</v>
       </c>
       <c r="I24" t="b">
         <v>0</v>
@@ -2126,24 +2256,24 @@
         <v>1</v>
       </c>
       <c r="L24" t="n">
-        <v>198</v>
+        <v>469</v>
       </c>
       <c r="M24" t="n">
         <v>0.4</v>
       </c>
       <c r="N24" t="n">
-        <v>1020.1</v>
-      </c>
-      <c r="O24" t="inlineStr">
-        <is>
-          <t>Never</t>
-        </is>
-      </c>
-      <c r="P24" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q24" t="b">
-        <v>0</v>
+        <v>2783.98</v>
+      </c>
+      <c r="O24" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="P24" t="inlineStr">
+        <is>
+          <t>Broken Even</t>
+        </is>
+      </c>
+      <c r="Q24" s="3" t="n">
+        <v>45703</v>
       </c>
       <c r="R24" t="b">
         <v>0</v>
@@ -2152,68 +2282,73 @@
         <v>0</v>
       </c>
       <c r="T24" t="b">
+        <v>0</v>
+      </c>
+      <c r="U24" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Courtney Warner</t>
+          <t>Felicia Singh</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Mr effort they that.</t>
+          <t>Account road wear food.</t>
         </is>
       </c>
       <c r="C25" s="2" t="n">
-        <v>45709</v>
+        <v>45210</v>
       </c>
       <c r="D25" t="b">
         <v>0</v>
       </c>
       <c r="E25" t="n">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Spotify</t>
+          <t>BookFunnel</t>
         </is>
       </c>
       <c r="G25" t="n">
-        <v>10.79</v>
+        <v>12.64</v>
       </c>
       <c r="H25" t="n">
-        <v>161.0921807851304</v>
+        <v>2042.719756081912</v>
       </c>
       <c r="I25" t="b">
         <v>0</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>AI Narrator</t>
+          <t>Taylor James</t>
         </is>
       </c>
       <c r="K25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L25" t="n">
-        <v>701</v>
+        <v>577</v>
       </c>
       <c r="M25" t="n">
-        <v>0.363</v>
+        <v>1</v>
       </c>
       <c r="N25" t="n">
-        <v>2745.66</v>
+        <v>7293.28</v>
       </c>
       <c r="O25" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="P25" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q25" t="b">
-        <v>0</v>
+        <v>0.3</v>
+      </c>
+      <c r="P25" t="inlineStr">
+        <is>
+          <t>Broken Even</t>
+        </is>
+      </c>
+      <c r="Q25" s="3" t="n">
+        <v>45210</v>
       </c>
       <c r="R25" t="b">
         <v>0</v>
@@ -2222,28 +2357,31 @@
         <v>0</v>
       </c>
       <c r="T25" t="b">
+        <v>0</v>
+      </c>
+      <c r="U25" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Albert Jordan</t>
+          <t>Noah Fernandez</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Space true couple nothing.</t>
+          <t>Tax today.</t>
         </is>
       </c>
       <c r="C26" s="2" t="n">
-        <v>45775</v>
+        <v>45173</v>
       </c>
       <c r="D26" t="b">
         <v>0</v>
       </c>
       <c r="E26" t="n">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="F26" t="inlineStr">
         <is>
@@ -2251,39 +2389,41 @@
         </is>
       </c>
       <c r="G26" t="n">
-        <v>10.09</v>
+        <v>13.93</v>
       </c>
       <c r="H26" t="n">
-        <v>280.6909876651985</v>
+        <v>5572.330703010432</v>
       </c>
       <c r="I26" t="b">
         <v>0</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>AI Narrator</t>
+          <t>Ava Winters</t>
         </is>
       </c>
       <c r="K26" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L26" t="n">
-        <v>254</v>
+        <v>835</v>
       </c>
       <c r="M26" t="n">
-        <v>0.362</v>
+        <v>0.363</v>
       </c>
       <c r="N26" t="n">
-        <v>927.76</v>
+        <v>4222.25</v>
       </c>
       <c r="O26" t="n">
-        <v>0.3</v>
-      </c>
-      <c r="P26" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q26" t="b">
-        <v>0</v>
+        <v>1.3</v>
+      </c>
+      <c r="P26" t="inlineStr">
+        <is>
+          <t>Broken Even</t>
+        </is>
+      </c>
+      <c r="Q26" s="3" t="n">
+        <v>45203</v>
       </c>
       <c r="R26" t="b">
         <v>0</v>
@@ -2292,68 +2432,73 @@
         <v>0</v>
       </c>
       <c r="T26" t="b">
+        <v>0</v>
+      </c>
+      <c r="U26" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Karen Marshall</t>
+          <t>Mrs. Alexandra Williams</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Toward down among process when.</t>
+          <t>Under rise project gas wonder.</t>
         </is>
       </c>
       <c r="C27" s="2" t="n">
-        <v>45855</v>
+        <v>45719</v>
       </c>
       <c r="D27" t="b">
         <v>0</v>
       </c>
       <c r="E27" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>ACX Royalty Share</t>
+          <t>BookFunnel</t>
         </is>
       </c>
       <c r="G27" t="n">
-        <v>18.54</v>
+        <v>12.68</v>
       </c>
       <c r="H27" t="n">
-        <v>7917.203898939063</v>
+        <v>4489.391366396995</v>
       </c>
       <c r="I27" t="b">
         <v>0</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>Samantha Prescott</t>
+          <t>Jason Clarke</t>
         </is>
       </c>
       <c r="K27" t="b">
         <v>0</v>
       </c>
       <c r="L27" t="n">
-        <v>48</v>
+        <v>562</v>
       </c>
       <c r="M27" t="n">
-        <v>0.228</v>
+        <v>1</v>
       </c>
       <c r="N27" t="n">
-        <v>202.9</v>
+        <v>7126.16</v>
       </c>
       <c r="O27" t="n">
-        <v>39</v>
-      </c>
-      <c r="P27" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q27" t="b">
-        <v>0</v>
+        <v>0.6</v>
+      </c>
+      <c r="P27" t="inlineStr">
+        <is>
+          <t>Broken Even</t>
+        </is>
+      </c>
+      <c r="Q27" s="3" t="n">
+        <v>45719</v>
       </c>
       <c r="R27" t="b">
         <v>0</v>
@@ -2362,68 +2507,77 @@
         <v>0</v>
       </c>
       <c r="T27" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="U27" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Roger Stevens</t>
+          <t>Paige Thompson</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>That responsibility pick keep.</t>
+          <t>Writer whom century.</t>
         </is>
       </c>
       <c r="C28" s="2" t="n">
-        <v>45728</v>
+        <v>45187</v>
       </c>
       <c r="D28" t="b">
         <v>0</v>
       </c>
       <c r="E28" t="n">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>ACX Exclusive</t>
+          <t>ACX Royalty Share</t>
         </is>
       </c>
       <c r="G28" t="n">
-        <v>8.550000000000001</v>
+        <v>15.52</v>
       </c>
       <c r="H28" t="n">
-        <v>4935.122344311648</v>
+        <v>0</v>
       </c>
       <c r="I28" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>Jason Clarke</t>
+          <t>AI Narrator</t>
         </is>
       </c>
       <c r="K28" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L28" t="n">
-        <v>491</v>
+        <v>194</v>
       </c>
       <c r="M28" t="n">
-        <v>0.4</v>
+        <v>0.052</v>
       </c>
       <c r="N28" t="n">
-        <v>1679.22</v>
-      </c>
-      <c r="O28" t="n">
-        <v>2.9</v>
-      </c>
-      <c r="P28" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q28" t="b">
-        <v>0</v>
+        <v>156.57</v>
+      </c>
+      <c r="O28" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="P28" t="inlineStr">
+        <is>
+          <t>Unclear - No Earnings Yet</t>
+        </is>
+      </c>
+      <c r="Q28" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
       </c>
       <c r="R28" t="b">
         <v>0</v>
@@ -2433,67 +2587,72 @@
       </c>
       <c r="T28" t="b">
         <v>0</v>
+      </c>
+      <c r="U28" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Toni Malone</t>
+          <t>Jorge Blevins</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>World debate.</t>
+          <t>Increase to land staff Mrs.</t>
         </is>
       </c>
       <c r="C29" s="2" t="n">
-        <v>45669</v>
+        <v>45531</v>
       </c>
       <c r="D29" t="b">
         <v>0</v>
       </c>
       <c r="E29" t="n">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>ACX Exclusive</t>
+          <t>Spotify</t>
         </is>
       </c>
       <c r="G29" t="n">
-        <v>10.18</v>
+        <v>8.18</v>
       </c>
       <c r="H29" t="n">
-        <v>177.8722044981239</v>
+        <v>2539.779389294989</v>
       </c>
       <c r="I29" t="b">
         <v>0</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>AI Narrator</t>
+          <t>Taylor James</t>
         </is>
       </c>
       <c r="K29" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L29" t="n">
-        <v>317</v>
+        <v>712</v>
       </c>
       <c r="M29" t="n">
-        <v>0.4</v>
+        <v>0.426</v>
       </c>
       <c r="N29" t="n">
-        <v>1290.82</v>
+        <v>2481.09</v>
       </c>
       <c r="O29" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="P29" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q29" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="P29" t="inlineStr">
+        <is>
+          <t>Broken Even</t>
+        </is>
+      </c>
+      <c r="Q29" s="3" t="n">
+        <v>45562</v>
       </c>
       <c r="R29" t="b">
         <v>0</v>
@@ -2502,68 +2661,73 @@
         <v>0</v>
       </c>
       <c r="T29" t="b">
+        <v>0</v>
+      </c>
+      <c r="U29" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Brad Harris</t>
+          <t>Donald Roberts Jr.</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Must main it candidate.</t>
+          <t>Total hit whether impact.</t>
         </is>
       </c>
       <c r="C30" s="2" t="n">
-        <v>45289</v>
+        <v>45825</v>
       </c>
       <c r="D30" t="b">
         <v>0</v>
       </c>
       <c r="E30" t="n">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>ACX Royalty Share</t>
+          <t>ACX Exclusive</t>
         </is>
       </c>
       <c r="G30" t="n">
-        <v>16.58</v>
+        <v>9.220000000000001</v>
       </c>
       <c r="H30" t="n">
-        <v>230.2967331481006</v>
+        <v>6315.920182715934</v>
       </c>
       <c r="I30" t="b">
         <v>0</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>AI Narrator</t>
+          <t>Ava Winters</t>
         </is>
       </c>
       <c r="K30" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L30" t="n">
-        <v>245</v>
+        <v>271</v>
       </c>
       <c r="M30" t="n">
-        <v>0.245</v>
+        <v>0.4</v>
       </c>
       <c r="N30" t="n">
-        <v>995.21</v>
+        <v>999.45</v>
       </c>
       <c r="O30" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="P30" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q30" t="b">
-        <v>0</v>
+        <v>6.3</v>
+      </c>
+      <c r="P30" t="inlineStr">
+        <is>
+          <t>In Progress</t>
+        </is>
+      </c>
+      <c r="Q30" s="3" t="n">
+        <v>46008</v>
       </c>
       <c r="R30" t="b">
         <v>0</v>
@@ -2572,68 +2736,73 @@
         <v>0</v>
       </c>
       <c r="T30" t="b">
+        <v>0</v>
+      </c>
+      <c r="U30" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Samantha Schaefer</t>
+          <t>Anna Garcia</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Five low his reflect.</t>
+          <t>Serve well buy weight paper.</t>
         </is>
       </c>
       <c r="C31" s="2" t="n">
-        <v>45341</v>
+        <v>45407</v>
       </c>
       <c r="D31" t="b">
         <v>0</v>
       </c>
       <c r="E31" t="n">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>ACX Royalty Share</t>
+          <t>BookFunnel</t>
         </is>
       </c>
       <c r="G31" t="n">
-        <v>13.42</v>
+        <v>19.71</v>
       </c>
       <c r="H31" t="n">
-        <v>4029.323494215169</v>
+        <v>209.8464481899723</v>
       </c>
       <c r="I31" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>Rachel Scott</t>
+          <t>AI Narrator</t>
         </is>
       </c>
       <c r="K31" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L31" t="n">
-        <v>95</v>
+        <v>459</v>
       </c>
       <c r="M31" t="n">
-        <v>0.063</v>
+        <v>1</v>
       </c>
       <c r="N31" t="n">
-        <v>80.31999999999999</v>
+        <v>9046.889999999999</v>
       </c>
       <c r="O31" t="n">
-        <v>50.2</v>
-      </c>
-      <c r="P31" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q31" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="P31" t="inlineStr">
+        <is>
+          <t>Broken Even</t>
+        </is>
+      </c>
+      <c r="Q31" s="3" t="n">
+        <v>45407</v>
       </c>
       <c r="R31" t="b">
         <v>0</v>
@@ -2642,68 +2811,73 @@
         <v>0</v>
       </c>
       <c r="T31" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="U31" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Samantha Mcdonald</t>
+          <t>Michelle Perkins</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Establish face.</t>
+          <t>Push room agreement.</t>
         </is>
       </c>
       <c r="C32" s="2" t="n">
-        <v>45512</v>
+        <v>45365</v>
       </c>
       <c r="D32" t="b">
         <v>0</v>
       </c>
       <c r="E32" t="n">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>ACX Exclusive</t>
+          <t>Findaway</t>
         </is>
       </c>
       <c r="G32" t="n">
-        <v>13.73</v>
+        <v>16.23</v>
       </c>
       <c r="H32" t="n">
-        <v>3094.046588307478</v>
+        <v>6851.869883789066</v>
       </c>
       <c r="I32" t="b">
         <v>0</v>
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>Taylor James</t>
+          <t>Samantha Prescott</t>
         </is>
       </c>
       <c r="K32" t="b">
         <v>0</v>
       </c>
       <c r="L32" t="n">
-        <v>567</v>
+        <v>960</v>
       </c>
       <c r="M32" t="n">
-        <v>0.4</v>
+        <v>0.35</v>
       </c>
       <c r="N32" t="n">
-        <v>3113.96</v>
+        <v>5453.28</v>
       </c>
       <c r="O32" t="n">
-        <v>1</v>
-      </c>
-      <c r="P32" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q32" t="b">
-        <v>0</v>
+        <v>1.3</v>
+      </c>
+      <c r="P32" t="inlineStr">
+        <is>
+          <t>Broken Even</t>
+        </is>
+      </c>
+      <c r="Q32" s="3" t="n">
+        <v>45396</v>
       </c>
       <c r="R32" t="b">
         <v>0</v>
@@ -2712,28 +2886,31 @@
         <v>0</v>
       </c>
       <c r="T32" t="b">
+        <v>0</v>
+      </c>
+      <c r="U32" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Christopher Bowen</t>
+          <t>Kayla Perry</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Rest write probably.</t>
+          <t>Within summer.</t>
         </is>
       </c>
       <c r="C33" s="2" t="n">
-        <v>45472</v>
+        <v>45404</v>
       </c>
       <c r="D33" t="b">
         <v>0</v>
       </c>
       <c r="E33" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F33" t="inlineStr">
         <is>
@@ -2741,109 +2918,116 @@
         </is>
       </c>
       <c r="G33" t="n">
-        <v>16.81</v>
+        <v>12.86</v>
       </c>
       <c r="H33" t="n">
-        <v>9262.428372689799</v>
+        <v>7325.969335038954</v>
       </c>
       <c r="I33" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>Samantha Prescott</t>
+          <t>Ava Winters</t>
         </is>
       </c>
       <c r="K33" t="b">
         <v>0</v>
       </c>
       <c r="L33" t="n">
-        <v>211</v>
+        <v>241</v>
       </c>
       <c r="M33" t="n">
-        <v>0.0655</v>
+        <v>0.199</v>
       </c>
       <c r="N33" t="n">
-        <v>232.32</v>
+        <v>616.75</v>
       </c>
       <c r="O33" t="n">
-        <v>39.9</v>
-      </c>
-      <c r="P33" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q33" t="b">
-        <v>0</v>
+        <v>11.9</v>
+      </c>
+      <c r="P33" t="inlineStr">
+        <is>
+          <t>Broken Even</t>
+        </is>
+      </c>
+      <c r="Q33" s="3" t="n">
+        <v>45738</v>
       </c>
       <c r="R33" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S33" t="b">
         <v>0</v>
       </c>
       <c r="T33" t="b">
+        <v>0</v>
+      </c>
+      <c r="U33" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Steven Williams</t>
+          <t>Amanda Carlson</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Kitchen her Republican simple.</t>
+          <t>Bag hour.</t>
         </is>
       </c>
       <c r="C34" s="2" t="n">
-        <v>45805</v>
+        <v>45424</v>
       </c>
       <c r="D34" t="b">
         <v>0</v>
       </c>
       <c r="E34" t="n">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>Findaway</t>
+          <t>BookFunnel</t>
         </is>
       </c>
       <c r="G34" t="n">
-        <v>14.57</v>
+        <v>11.74</v>
       </c>
       <c r="H34" t="n">
-        <v>4066.88634362504</v>
+        <v>5150.968267752891</v>
       </c>
       <c r="I34" t="b">
         <v>0</v>
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>Ava Winters</t>
+          <t>Jason Clarke</t>
         </is>
       </c>
       <c r="K34" t="b">
         <v>0</v>
       </c>
       <c r="L34" t="n">
-        <v>323</v>
+        <v>654</v>
       </c>
       <c r="M34" t="n">
-        <v>0.342</v>
+        <v>1</v>
       </c>
       <c r="N34" t="n">
-        <v>1609.49</v>
+        <v>7677.96</v>
       </c>
       <c r="O34" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="P34" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q34" t="b">
-        <v>0</v>
+        <v>0.7</v>
+      </c>
+      <c r="P34" t="inlineStr">
+        <is>
+          <t>Broken Even</t>
+        </is>
+      </c>
+      <c r="Q34" s="3" t="n">
+        <v>45424</v>
       </c>
       <c r="R34" t="b">
         <v>0</v>
@@ -2852,28 +3036,31 @@
         <v>0</v>
       </c>
       <c r="T34" t="b">
+        <v>0</v>
+      </c>
+      <c r="U34" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Kimberly Cruz</t>
+          <t>Timothy Kaufman</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Get affect high fight when.</t>
+          <t>American present stage.</t>
         </is>
       </c>
       <c r="C35" s="2" t="n">
-        <v>45280</v>
+        <v>45493</v>
       </c>
       <c r="D35" t="b">
         <v>0</v>
       </c>
       <c r="E35" t="n">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="F35" t="inlineStr">
         <is>
@@ -2881,39 +3068,41 @@
         </is>
       </c>
       <c r="G35" t="n">
-        <v>18.96</v>
+        <v>14.6</v>
       </c>
       <c r="H35" t="n">
-        <v>10385.97987287411</v>
+        <v>3996.925168134335</v>
       </c>
       <c r="I35" t="b">
         <v>0</v>
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>Samantha Prescott</t>
+          <t>Taylor James</t>
         </is>
       </c>
       <c r="K35" t="b">
         <v>0</v>
       </c>
       <c r="L35" t="n">
-        <v>159</v>
+        <v>225</v>
       </c>
       <c r="M35" t="n">
-        <v>0.211</v>
+        <v>0.247</v>
       </c>
       <c r="N35" t="n">
-        <v>636.09</v>
+        <v>811.39</v>
       </c>
       <c r="O35" t="n">
-        <v>16.3</v>
-      </c>
-      <c r="P35" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q35" t="b">
-        <v>0</v>
+        <v>4.9</v>
+      </c>
+      <c r="P35" t="inlineStr">
+        <is>
+          <t>Broken Even</t>
+        </is>
+      </c>
+      <c r="Q35" s="3" t="n">
+        <v>45616</v>
       </c>
       <c r="R35" t="b">
         <v>0</v>
@@ -2922,68 +3111,73 @@
         <v>0</v>
       </c>
       <c r="T35" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="U35" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Gregory Gomez</t>
+          <t>Cindy Howard</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Behavior ball else.</t>
+          <t>Cold whatever own ready.</t>
         </is>
       </c>
       <c r="C36" s="2" t="n">
-        <v>45229</v>
+        <v>45806</v>
       </c>
       <c r="D36" t="b">
         <v>0</v>
       </c>
       <c r="E36" t="n">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>Spotify</t>
+          <t>ACX Exclusive</t>
         </is>
       </c>
       <c r="G36" t="n">
-        <v>10.79</v>
+        <v>9.23</v>
       </c>
       <c r="H36" t="n">
-        <v>5286.160244129313</v>
+        <v>434.4512086043742</v>
       </c>
       <c r="I36" t="b">
         <v>0</v>
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>Jason Clarke</t>
+          <t>AI Narrator</t>
         </is>
       </c>
       <c r="K36" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L36" t="n">
-        <v>363</v>
+        <v>417</v>
       </c>
       <c r="M36" t="n">
-        <v>0.306</v>
+        <v>0.4</v>
       </c>
       <c r="N36" t="n">
-        <v>1198.53</v>
+        <v>1539.56</v>
       </c>
       <c r="O36" t="n">
-        <v>4.4</v>
-      </c>
-      <c r="P36" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q36" t="b">
-        <v>0</v>
+        <v>0.3</v>
+      </c>
+      <c r="P36" t="inlineStr">
+        <is>
+          <t>Broken Even</t>
+        </is>
+      </c>
+      <c r="Q36" s="3" t="n">
+        <v>45806</v>
       </c>
       <c r="R36" t="b">
         <v>0</v>
@@ -2992,208 +3186,227 @@
         <v>0</v>
       </c>
       <c r="T36" t="b">
+        <v>0</v>
+      </c>
+      <c r="U36" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Mary Waller</t>
+          <t>Lorraine Davis</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Create loss sure record continue.</t>
+          <t>Thus report side second.</t>
         </is>
       </c>
       <c r="C37" s="2" t="n">
-        <v>45653</v>
+        <v>45809</v>
       </c>
       <c r="D37" t="b">
         <v>0</v>
       </c>
       <c r="E37" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>Spotify</t>
+          <t>ACX Royalty Share</t>
         </is>
       </c>
       <c r="G37" t="n">
-        <v>10.85</v>
+        <v>18.62</v>
       </c>
       <c r="H37" t="n">
-        <v>3302.527276903202</v>
+        <v>9611.004029153077</v>
       </c>
       <c r="I37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>Rachel Scott</t>
+          <t>Ava Winters</t>
         </is>
       </c>
       <c r="K37" t="b">
         <v>0</v>
       </c>
       <c r="L37" t="n">
-        <v>711</v>
+        <v>199</v>
       </c>
       <c r="M37" t="n">
-        <v>0.419</v>
+        <v>0.068</v>
       </c>
       <c r="N37" t="n">
-        <v>3232.31</v>
-      </c>
-      <c r="O37" t="n">
-        <v>1</v>
-      </c>
-      <c r="P37" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q37" t="b">
-        <v>0</v>
+        <v>251.97</v>
+      </c>
+      <c r="O37" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="P37" t="inlineStr">
+        <is>
+          <t>Unclear - No Earnings Yet</t>
+        </is>
+      </c>
+      <c r="Q37" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
       </c>
       <c r="R37" t="b">
         <v>0</v>
       </c>
       <c r="S37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T37" t="b">
         <v>0</v>
+      </c>
+      <c r="U37" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Mark Stevens</t>
+          <t>Elizabeth Schmidt</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Cause eat.</t>
+          <t>By use leave.</t>
         </is>
       </c>
       <c r="C38" s="2" t="n">
-        <v>45496</v>
+        <v>45806</v>
       </c>
       <c r="D38" t="b">
         <v>0</v>
       </c>
       <c r="E38" t="n">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>ACX Royalty Share</t>
+          <t>BookFunnel</t>
         </is>
       </c>
       <c r="G38" t="n">
-        <v>17.7</v>
+        <v>14.39</v>
       </c>
       <c r="H38" t="n">
-        <v>7973.674143276128</v>
+        <v>6442.636818274063</v>
       </c>
       <c r="I38" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>Jason Clarke</t>
+          <t>Samantha Prescott</t>
         </is>
       </c>
       <c r="K38" t="b">
         <v>0</v>
       </c>
       <c r="L38" t="n">
-        <v>276</v>
+        <v>178</v>
       </c>
       <c r="M38" t="n">
-        <v>0.078</v>
+        <v>1</v>
       </c>
       <c r="N38" t="n">
-        <v>381.05</v>
+        <v>2561.42</v>
       </c>
       <c r="O38" t="n">
-        <v>20.9</v>
-      </c>
-      <c r="P38" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q38" t="b">
-        <v>0</v>
+        <v>2.5</v>
+      </c>
+      <c r="P38" t="inlineStr">
+        <is>
+          <t>In Progress</t>
+        </is>
+      </c>
+      <c r="Q38" s="3" t="n">
+        <v>45867</v>
       </c>
       <c r="R38" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S38" t="b">
         <v>0</v>
       </c>
       <c r="T38" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="U38" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Gloria Juarez</t>
+          <t>Thomas Carpenter</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>There white.</t>
+          <t>Others most student.</t>
         </is>
       </c>
       <c r="C39" s="2" t="n">
-        <v>45304</v>
+        <v>45630</v>
       </c>
       <c r="D39" t="b">
         <v>0</v>
       </c>
       <c r="E39" t="n">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>ACX Royalty Share</t>
+          <t>Findaway</t>
         </is>
       </c>
       <c r="G39" t="n">
-        <v>12.89</v>
+        <v>16.7</v>
       </c>
       <c r="H39" t="n">
-        <v>4027.99906805048</v>
+        <v>5056.919886253324</v>
       </c>
       <c r="I39" t="b">
         <v>0</v>
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>Taylor James</t>
+          <t>Ava Winters</t>
         </is>
       </c>
       <c r="K39" t="b">
         <v>0</v>
       </c>
       <c r="L39" t="n">
-        <v>86</v>
+        <v>410</v>
       </c>
       <c r="M39" t="n">
-        <v>0.227</v>
+        <v>0.349</v>
       </c>
       <c r="N39" t="n">
-        <v>251.64</v>
+        <v>2389.6</v>
       </c>
       <c r="O39" t="n">
-        <v>16</v>
-      </c>
-      <c r="P39" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q39" t="b">
-        <v>0</v>
+        <v>2.1</v>
+      </c>
+      <c r="P39" t="inlineStr">
+        <is>
+          <t>Broken Even</t>
+        </is>
+      </c>
+      <c r="Q39" s="3" t="n">
+        <v>45692</v>
       </c>
       <c r="R39" t="b">
         <v>0</v>
@@ -3202,68 +3415,73 @@
         <v>0</v>
       </c>
       <c r="T39" t="b">
+        <v>0</v>
+      </c>
+      <c r="U39" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Johnny Martinez</t>
+          <t>Gina Sherman</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Stage common at subject.</t>
+          <t>Cultural force knowledge else blue.</t>
         </is>
       </c>
       <c r="C40" s="2" t="n">
-        <v>45512</v>
+        <v>45630</v>
       </c>
       <c r="D40" t="b">
         <v>0</v>
       </c>
       <c r="E40" t="n">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>Findaway</t>
+          <t>BookFunnel</t>
         </is>
       </c>
       <c r="G40" t="n">
-        <v>11.54</v>
+        <v>15.41</v>
       </c>
       <c r="H40" t="n">
-        <v>5498.529841641285</v>
+        <v>7136.311792106308</v>
       </c>
       <c r="I40" t="b">
         <v>0</v>
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>Ava Winters</t>
+          <t>Jason Clarke</t>
         </is>
       </c>
       <c r="K40" t="b">
         <v>0</v>
       </c>
       <c r="L40" t="n">
-        <v>861</v>
+        <v>439</v>
       </c>
       <c r="M40" t="n">
-        <v>0.319</v>
+        <v>1</v>
       </c>
       <c r="N40" t="n">
-        <v>3169.56</v>
+        <v>6764.99</v>
       </c>
       <c r="O40" t="n">
-        <v>1.7</v>
-      </c>
-      <c r="P40" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q40" t="b">
-        <v>0</v>
+        <v>1.1</v>
+      </c>
+      <c r="P40" t="inlineStr">
+        <is>
+          <t>Broken Even</t>
+        </is>
+      </c>
+      <c r="Q40" s="3" t="n">
+        <v>45661</v>
       </c>
       <c r="R40" t="b">
         <v>0</v>
@@ -3272,22 +3490,25 @@
         <v>0</v>
       </c>
       <c r="T40" t="b">
+        <v>0</v>
+      </c>
+      <c r="U40" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Andrew Dunlap</t>
+          <t>Christopher Scott</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Down ago significant.</t>
+          <t>Between anyone.</t>
         </is>
       </c>
       <c r="C41" s="2" t="n">
-        <v>45410</v>
+        <v>45400</v>
       </c>
       <c r="D41" t="b">
         <v>0</v>
@@ -3301,39 +3522,41 @@
         </is>
       </c>
       <c r="G41" t="n">
-        <v>8.109999999999999</v>
+        <v>8.449999999999999</v>
       </c>
       <c r="H41" t="n">
-        <v>4261.109492778802</v>
+        <v>655.8472502065704</v>
       </c>
       <c r="I41" t="b">
         <v>0</v>
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>Jason Clarke</t>
+          <t>AI Narrator</t>
         </is>
       </c>
       <c r="K41" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L41" t="n">
-        <v>865</v>
+        <v>394</v>
       </c>
       <c r="M41" t="n">
-        <v>0.371</v>
+        <v>0.418</v>
       </c>
       <c r="N41" t="n">
-        <v>2602.62</v>
+        <v>1391.65</v>
       </c>
       <c r="O41" t="n">
-        <v>1.6</v>
-      </c>
-      <c r="P41" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q41" t="b">
-        <v>0</v>
+        <v>0.5</v>
+      </c>
+      <c r="P41" t="inlineStr">
+        <is>
+          <t>Broken Even</t>
+        </is>
+      </c>
+      <c r="Q41" s="3" t="n">
+        <v>45400</v>
       </c>
       <c r="R41" t="b">
         <v>0</v>
@@ -3342,68 +3565,73 @@
         <v>0</v>
       </c>
       <c r="T41" t="b">
+        <v>0</v>
+      </c>
+      <c r="U41" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Dennis Parker</t>
+          <t>Ann Gomez</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Live adult image.</t>
+          <t>Maybe add fall plan determine.</t>
         </is>
       </c>
       <c r="C42" s="2" t="n">
-        <v>45812</v>
+        <v>45639</v>
       </c>
       <c r="D42" t="b">
         <v>0</v>
       </c>
       <c r="E42" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>ACX Royalty Share</t>
+          <t>BookFunnel</t>
         </is>
       </c>
       <c r="G42" t="n">
-        <v>19.48</v>
+        <v>19.72</v>
       </c>
       <c r="H42" t="n">
-        <v>3236.402075185601</v>
+        <v>5471.224126515399</v>
       </c>
       <c r="I42" t="b">
         <v>0</v>
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>Rachel Scott</t>
+          <t>Jason Clarke</t>
         </is>
       </c>
       <c r="K42" t="b">
         <v>0</v>
       </c>
       <c r="L42" t="n">
-        <v>77</v>
+        <v>758</v>
       </c>
       <c r="M42" t="n">
-        <v>0.225</v>
+        <v>1</v>
       </c>
       <c r="N42" t="n">
-        <v>337.49</v>
+        <v>14947.76</v>
       </c>
       <c r="O42" t="n">
-        <v>9.6</v>
-      </c>
-      <c r="P42" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q42" t="b">
-        <v>0</v>
+        <v>0.4</v>
+      </c>
+      <c r="P42" t="inlineStr">
+        <is>
+          <t>Broken Even</t>
+        </is>
+      </c>
+      <c r="Q42" s="3" t="n">
+        <v>45639</v>
       </c>
       <c r="R42" t="b">
         <v>0</v>
@@ -3412,68 +3640,73 @@
         <v>0</v>
       </c>
       <c r="T42" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="U42" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Kayla Moreno</t>
+          <t>Rhonda Navarro</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Receive difficult travel report.</t>
+          <t>Throw forget receive.</t>
         </is>
       </c>
       <c r="C43" s="2" t="n">
-        <v>45293</v>
+        <v>45515</v>
       </c>
       <c r="D43" t="b">
         <v>0</v>
       </c>
       <c r="E43" t="n">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>Spotify</t>
+          <t>ACX Royalty Share</t>
         </is>
       </c>
       <c r="G43" t="n">
-        <v>19.71</v>
+        <v>16.45</v>
       </c>
       <c r="H43" t="n">
-        <v>3265.211656626933</v>
+        <v>5496.769690847592</v>
       </c>
       <c r="I43" t="b">
         <v>0</v>
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>Taylor James</t>
+          <t>Ava Winters</t>
         </is>
       </c>
       <c r="K43" t="b">
         <v>0</v>
       </c>
       <c r="L43" t="n">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="M43" t="n">
-        <v>0.355</v>
+        <v>0.232</v>
       </c>
       <c r="N43" t="n">
-        <v>1406.41</v>
+        <v>759.46</v>
       </c>
       <c r="O43" t="n">
-        <v>2.3</v>
-      </c>
-      <c r="P43" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q43" t="b">
-        <v>0</v>
+        <v>7.2</v>
+      </c>
+      <c r="P43" t="inlineStr">
+        <is>
+          <t>Broken Even</t>
+        </is>
+      </c>
+      <c r="Q43" s="3" t="n">
+        <v>45727</v>
       </c>
       <c r="R43" t="b">
         <v>0</v>
@@ -3483,67 +3716,72 @@
       </c>
       <c r="T43" t="b">
         <v>0</v>
+      </c>
+      <c r="U43" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Cody Maldonado</t>
+          <t>Tammy Liu</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Dream gun.</t>
+          <t>Beyond Mrs.</t>
         </is>
       </c>
       <c r="C44" s="2" t="n">
-        <v>45718</v>
+        <v>45613</v>
       </c>
       <c r="D44" t="b">
         <v>0</v>
       </c>
       <c r="E44" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>Spotify</t>
+          <t>BookFunnel</t>
         </is>
       </c>
       <c r="G44" t="n">
-        <v>8.720000000000001</v>
+        <v>11.15</v>
       </c>
       <c r="H44" t="n">
-        <v>4135.171719864784</v>
+        <v>3086.694584266365</v>
       </c>
       <c r="I44" t="b">
         <v>0</v>
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>Samantha Prescott</t>
+          <t>Rachel Scott</t>
         </is>
       </c>
       <c r="K44" t="b">
         <v>0</v>
       </c>
       <c r="L44" t="n">
-        <v>387</v>
+        <v>284</v>
       </c>
       <c r="M44" t="n">
-        <v>0.437</v>
+        <v>1</v>
       </c>
       <c r="N44" t="n">
-        <v>1474.72</v>
+        <v>3166.6</v>
       </c>
       <c r="O44" t="n">
-        <v>2.8</v>
-      </c>
-      <c r="P44" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q44" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="P44" t="inlineStr">
+        <is>
+          <t>Broken Even</t>
+        </is>
+      </c>
+      <c r="Q44" s="3" t="n">
+        <v>45613</v>
       </c>
       <c r="R44" t="b">
         <v>0</v>
@@ -3552,68 +3790,73 @@
         <v>0</v>
       </c>
       <c r="T44" t="b">
+        <v>0</v>
+      </c>
+      <c r="U44" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>William Trujillo</t>
+          <t>Kurt Ellis</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Sort keep provide every sit.</t>
+          <t>Piece evening issue exactly.</t>
         </is>
       </c>
       <c r="C45" s="2" t="n">
-        <v>45186</v>
+        <v>45394</v>
       </c>
       <c r="D45" t="b">
         <v>0</v>
       </c>
       <c r="E45" t="n">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>Findaway</t>
+          <t>BookFunnel</t>
         </is>
       </c>
       <c r="G45" t="n">
-        <v>8.48</v>
+        <v>18.05</v>
       </c>
       <c r="H45" t="n">
-        <v>3778.334159415333</v>
+        <v>0</v>
       </c>
       <c r="I45" t="b">
         <v>0</v>
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>Rachel Scott</t>
+          <t>AI Narrator</t>
         </is>
       </c>
       <c r="K45" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L45" t="n">
-        <v>997</v>
+        <v>423</v>
       </c>
       <c r="M45" t="n">
-        <v>0.325</v>
+        <v>1</v>
       </c>
       <c r="N45" t="n">
-        <v>2747.73</v>
+        <v>7635.15</v>
       </c>
       <c r="O45" t="n">
-        <v>1.4</v>
-      </c>
-      <c r="P45" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q45" t="b">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="P45" t="inlineStr">
+        <is>
+          <t>Already Profitable</t>
+        </is>
+      </c>
+      <c r="Q45" s="3" t="n">
+        <v>45394</v>
       </c>
       <c r="R45" t="b">
         <v>0</v>
@@ -3622,68 +3865,73 @@
         <v>0</v>
       </c>
       <c r="T45" t="b">
+        <v>0</v>
+      </c>
+      <c r="U45" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Kevin Howard</t>
+          <t>Kristopher Campos</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Him good data evidence road.</t>
+          <t>Score appear simple type.</t>
         </is>
       </c>
       <c r="C46" s="2" t="n">
-        <v>45570</v>
+        <v>45354</v>
       </c>
       <c r="D46" t="b">
         <v>0</v>
       </c>
       <c r="E46" t="n">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>Spotify</t>
+          <t>ACX Royalty Share</t>
         </is>
       </c>
       <c r="G46" t="n">
-        <v>15.73</v>
+        <v>9.19</v>
       </c>
       <c r="H46" t="n">
-        <v>7157.333187254329</v>
+        <v>3576.478636767976</v>
       </c>
       <c r="I46" t="b">
         <v>0</v>
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>Jason Clarke</t>
+          <t>Taylor James</t>
         </is>
       </c>
       <c r="K46" t="b">
         <v>0</v>
       </c>
       <c r="L46" t="n">
-        <v>707</v>
+        <v>134</v>
       </c>
       <c r="M46" t="n">
-        <v>0.483</v>
+        <v>0.209</v>
       </c>
       <c r="N46" t="n">
-        <v>5371.5</v>
+        <v>257.38</v>
       </c>
       <c r="O46" t="n">
-        <v>1.3</v>
-      </c>
-      <c r="P46" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q46" t="b">
-        <v>0</v>
+        <v>13.9</v>
+      </c>
+      <c r="P46" t="inlineStr">
+        <is>
+          <t>Broken Even</t>
+        </is>
+      </c>
+      <c r="Q46" s="3" t="n">
+        <v>45750</v>
       </c>
       <c r="R46" t="b">
         <v>0</v>
@@ -3692,68 +3940,73 @@
         <v>0</v>
       </c>
       <c r="T46" t="b">
+        <v>0</v>
+      </c>
+      <c r="U46" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Sabrina Smith</t>
+          <t>John Larson</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>High coach.</t>
+          <t>Action fast director.</t>
         </is>
       </c>
       <c r="C47" s="2" t="n">
-        <v>45298</v>
+        <v>45146</v>
       </c>
       <c r="D47" t="b">
         <v>0</v>
       </c>
       <c r="E47" t="n">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>ACX Royalty Share</t>
+          <t>Spotify</t>
         </is>
       </c>
       <c r="G47" t="n">
-        <v>17.98</v>
+        <v>19.32</v>
       </c>
       <c r="H47" t="n">
-        <v>6913.189846568979</v>
+        <v>4502.83275709597</v>
       </c>
       <c r="I47" t="b">
         <v>0</v>
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>Jason Clarke</t>
+          <t>Samantha Prescott</t>
         </is>
       </c>
       <c r="K47" t="b">
         <v>0</v>
       </c>
       <c r="L47" t="n">
-        <v>264</v>
+        <v>771</v>
       </c>
       <c r="M47" t="n">
-        <v>0.238</v>
+        <v>0.303</v>
       </c>
       <c r="N47" t="n">
-        <v>1129.72</v>
+        <v>4513.4</v>
       </c>
       <c r="O47" t="n">
-        <v>6.1</v>
-      </c>
-      <c r="P47" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q47" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="P47" t="inlineStr">
+        <is>
+          <t>Broken Even</t>
+        </is>
+      </c>
+      <c r="Q47" s="3" t="n">
+        <v>45146</v>
       </c>
       <c r="R47" t="b">
         <v>0</v>
@@ -3762,68 +4015,73 @@
         <v>0</v>
       </c>
       <c r="T47" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="U47" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Kelly Sexton</t>
+          <t>Ray Sanchez</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Or either moment side.</t>
+          <t>Design trip.</t>
         </is>
       </c>
       <c r="C48" s="2" t="n">
-        <v>45425</v>
+        <v>45671</v>
       </c>
       <c r="D48" t="b">
         <v>0</v>
       </c>
       <c r="E48" t="n">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>ACX Royalty Share</t>
+          <t>Spotify</t>
         </is>
       </c>
       <c r="G48" t="n">
-        <v>11.31</v>
+        <v>12.19</v>
       </c>
       <c r="H48" t="n">
-        <v>964.7915755083902</v>
+        <v>4338.10214550772</v>
       </c>
       <c r="I48" t="b">
         <v>0</v>
       </c>
       <c r="J48" t="inlineStr">
         <is>
-          <t>AI Narrator</t>
+          <t>Samantha Prescott</t>
         </is>
       </c>
       <c r="K48" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L48" t="n">
-        <v>100</v>
+        <v>889</v>
       </c>
       <c r="M48" t="n">
-        <v>0.201</v>
+        <v>0.499</v>
       </c>
       <c r="N48" t="n">
-        <v>227.33</v>
+        <v>5407.62</v>
       </c>
       <c r="O48" t="n">
-        <v>4.2</v>
-      </c>
-      <c r="P48" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q48" t="b">
-        <v>0</v>
+        <v>0.8</v>
+      </c>
+      <c r="P48" t="inlineStr">
+        <is>
+          <t>Broken Even</t>
+        </is>
+      </c>
+      <c r="Q48" s="3" t="n">
+        <v>45671</v>
       </c>
       <c r="R48" t="b">
         <v>0</v>
@@ -3832,28 +4090,31 @@
         <v>0</v>
       </c>
       <c r="T48" t="b">
+        <v>0</v>
+      </c>
+      <c r="U48" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Michelle Perez</t>
+          <t>Timothy Diaz</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>What blue all.</t>
+          <t>Pretty walk trip.</t>
         </is>
       </c>
       <c r="C49" s="2" t="n">
-        <v>45601</v>
+        <v>45541</v>
       </c>
       <c r="D49" t="b">
         <v>0</v>
       </c>
       <c r="E49" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F49" t="inlineStr">
         <is>
@@ -3861,39 +4122,41 @@
         </is>
       </c>
       <c r="G49" t="n">
-        <v>11.31</v>
+        <v>10.81</v>
       </c>
       <c r="H49" t="n">
-        <v>3324.995815170355</v>
+        <v>0</v>
       </c>
       <c r="I49" t="b">
         <v>0</v>
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t>Rachel Scott</t>
+          <t>AI Narrator</t>
         </is>
       </c>
       <c r="K49" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L49" t="n">
-        <v>285</v>
+        <v>517</v>
       </c>
       <c r="M49" t="n">
-        <v>0.406</v>
+        <v>0.412</v>
       </c>
       <c r="N49" t="n">
-        <v>1308.68</v>
+        <v>2302.57</v>
       </c>
       <c r="O49" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="P49" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q49" t="b">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="P49" t="inlineStr">
+        <is>
+          <t>Already Profitable</t>
+        </is>
+      </c>
+      <c r="Q49" s="3" t="n">
+        <v>45541</v>
       </c>
       <c r="R49" t="b">
         <v>0</v>
@@ -3902,68 +4165,73 @@
         <v>0</v>
       </c>
       <c r="T49" t="b">
+        <v>0</v>
+      </c>
+      <c r="U49" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Brian Rowe</t>
+          <t>Abigail Stewart</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>And business week.</t>
+          <t>Fill owner me.</t>
         </is>
       </c>
       <c r="C50" s="2" t="n">
-        <v>45801</v>
+        <v>45523</v>
       </c>
       <c r="D50" t="b">
         <v>0</v>
       </c>
       <c r="E50" t="n">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>Spotify</t>
+          <t>BookFunnel</t>
         </is>
       </c>
       <c r="G50" t="n">
-        <v>11.1</v>
+        <v>15.88</v>
       </c>
       <c r="H50" t="n">
-        <v>7272.63214523308</v>
+        <v>2354.31583781771</v>
       </c>
       <c r="I50" t="b">
         <v>0</v>
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t>Ava Winters</t>
+          <t>Rachel Scott</t>
         </is>
       </c>
       <c r="K50" t="b">
         <v>0</v>
       </c>
       <c r="L50" t="n">
-        <v>218</v>
+        <v>334</v>
       </c>
       <c r="M50" t="n">
-        <v>0.325</v>
+        <v>1</v>
       </c>
       <c r="N50" t="n">
-        <v>786.4299999999999</v>
+        <v>5303.92</v>
       </c>
       <c r="O50" t="n">
-        <v>9.199999999999999</v>
-      </c>
-      <c r="P50" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q50" t="b">
-        <v>0</v>
+        <v>0.4</v>
+      </c>
+      <c r="P50" t="inlineStr">
+        <is>
+          <t>Broken Even</t>
+        </is>
+      </c>
+      <c r="Q50" s="3" t="n">
+        <v>45523</v>
       </c>
       <c r="R50" t="b">
         <v>0</v>
@@ -3972,68 +4240,73 @@
         <v>0</v>
       </c>
       <c r="T50" t="b">
+        <v>0</v>
+      </c>
+      <c r="U50" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Melinda Morrison</t>
+          <t>Jennifer Williams</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Front level million smile water.</t>
+          <t>Challenge man economic here.</t>
         </is>
       </c>
       <c r="C51" s="2" t="n">
-        <v>45368</v>
+        <v>45801</v>
       </c>
       <c r="D51" t="b">
         <v>0</v>
       </c>
       <c r="E51" t="n">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>Spotify</t>
+          <t>Findaway</t>
         </is>
       </c>
       <c r="G51" t="n">
-        <v>9.66</v>
+        <v>13.27</v>
       </c>
       <c r="H51" t="n">
-        <v>7481.23356019066</v>
+        <v>3160.768347115496</v>
       </c>
       <c r="I51" t="b">
         <v>0</v>
       </c>
       <c r="J51" t="inlineStr">
         <is>
-          <t>Ava Winters</t>
+          <t>Rachel Scott</t>
         </is>
       </c>
       <c r="K51" t="b">
         <v>0</v>
       </c>
       <c r="L51" t="n">
-        <v>573</v>
+        <v>196</v>
       </c>
       <c r="M51" t="n">
-        <v>0.493</v>
+        <v>0.306</v>
       </c>
       <c r="N51" t="n">
-        <v>2728.84</v>
+        <v>795.88</v>
       </c>
       <c r="O51" t="n">
-        <v>2.7</v>
-      </c>
-      <c r="P51" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q51" t="b">
-        <v>0</v>
+        <v>4</v>
+      </c>
+      <c r="P51" t="inlineStr">
+        <is>
+          <t>In Progress</t>
+        </is>
+      </c>
+      <c r="Q51" s="3" t="n">
+        <v>45893</v>
       </c>
       <c r="R51" t="b">
         <v>0</v>
@@ -4042,6 +4315,9 @@
         <v>0</v>
       </c>
       <c r="T51" t="b">
+        <v>0</v>
+      </c>
+      <c r="U51" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>